<commit_message>
Version 2.0.1: added 1G
</commit_message>
<xml_diff>
--- a/assets/All Classes.xlsx
+++ b/assets/All Classes.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="110">
   <si>
     <t>Macros</t>
   </si>
@@ -166,6 +166,24 @@
     <t>Philosphie</t>
   </si>
   <si>
+    <t>1G</t>
+  </si>
+  <si>
+    <t>SciSoc</t>
+  </si>
+  <si>
+    <t>5M</t>
+  </si>
+  <si>
+    <t>Histo/Geo</t>
+  </si>
+  <si>
+    <t>EduArt</t>
+  </si>
+  <si>
+    <t>4C</t>
+  </si>
+  <si>
     <t>1E</t>
   </si>
   <si>
@@ -173,9 +191,6 @@
   </si>
   <si>
     <t>Dessin</t>
-  </si>
-  <si>
-    <t>5M</t>
   </si>
   <si>
     <t>Projets</t>
@@ -193,7 +208,7 @@
     <t>EduArt3</t>
   </si>
   <si>
-    <t>4C</t>
+    <t>4M</t>
   </si>
   <si>
     <t>1F</t>
@@ -206,12 +221,6 @@
   </si>
   <si>
     <t>EduMusic 3</t>
-  </si>
-  <si>
-    <t>EduArt</t>
-  </si>
-  <si>
-    <t>4M</t>
   </si>
   <si>
     <t>3MA</t>
@@ -529,11 +538,11 @@
     <xf borderId="0" fillId="10" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="13" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf borderId="0" fillId="13" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="13" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1894,17 +1903,13 @@
       <c r="R49" s="16">
         <v>4.0</v>
       </c>
-      <c r="S49" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="T49" s="21">
-        <v>2.0</v>
-      </c>
+      <c r="S49" s="20"/>
+      <c r="T49" s="21"/>
     </row>
     <row r="50">
       <c r="A50" s="7"/>
       <c r="B50" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C50" s="15" t="s">
         <v>8</v>
@@ -1922,14 +1927,14 @@
       <c r="M50" s="12"/>
       <c r="O50" s="7"/>
       <c r="P50" s="8"/>
-      <c r="Q50" s="9"/>
-      <c r="R50" s="10"/>
-      <c r="S50" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="T50" s="21">
-        <v>1.0</v>
-      </c>
+      <c r="Q50" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="R50" s="16">
+        <v>3.0</v>
+      </c>
+      <c r="S50" s="20"/>
+      <c r="T50" s="21"/>
     </row>
     <row r="51">
       <c r="A51" s="7"/>
@@ -1949,17 +1954,11 @@
       <c r="O51" s="7"/>
       <c r="P51" s="8"/>
       <c r="Q51" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="R51" s="16">
-        <v>3.0</v>
-      </c>
-      <c r="S51" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="T51" s="21">
-        <v>2.0</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="R51" s="10"/>
+      <c r="S51" s="20"/>
+      <c r="T51" s="21"/>
     </row>
     <row r="52">
       <c r="A52" s="7"/>
@@ -1978,14 +1977,12 @@
       <c r="M52" s="12"/>
       <c r="O52" s="7"/>
       <c r="P52" s="8"/>
-      <c r="Q52" s="9"/>
+      <c r="Q52" s="15" t="s">
+        <v>19</v>
+      </c>
       <c r="R52" s="10"/>
-      <c r="S52" s="20" t="s">
-        <v>58</v>
-      </c>
-      <c r="T52" s="21">
-        <v>1.0</v>
-      </c>
+      <c r="S52" s="20"/>
+      <c r="T52" s="21"/>
     </row>
     <row r="53">
       <c r="A53" s="7"/>
@@ -2005,11 +2002,17 @@
       <c r="O53" s="7"/>
       <c r="P53" s="8"/>
       <c r="Q53" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="R53" s="16"/>
-      <c r="S53" s="11"/>
-      <c r="T53" s="12"/>
+        <v>54</v>
+      </c>
+      <c r="R53" s="16">
+        <v>3.0</v>
+      </c>
+      <c r="S53" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="T53" s="21">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" s="7"/>
@@ -2030,12 +2033,14 @@
       <c r="M54" s="12"/>
       <c r="O54" s="7"/>
       <c r="P54" s="8"/>
-      <c r="Q54" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="R54" s="16"/>
-      <c r="S54" s="11"/>
-      <c r="T54" s="12"/>
+      <c r="Q54" s="15"/>
+      <c r="R54" s="10"/>
+      <c r="S54" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="T54" s="21">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" s="7"/>
@@ -2054,10 +2059,12 @@
       <c r="M55" s="12"/>
       <c r="O55" s="7"/>
       <c r="P55" s="8"/>
-      <c r="Q55" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="R55" s="10"/>
+      <c r="Q55" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="R55" s="19">
+        <v>2.0</v>
+      </c>
       <c r="S55" s="11"/>
       <c r="T55" s="12"/>
     </row>
@@ -2078,10 +2085,10 @@
       <c r="M56" s="12"/>
       <c r="O56" s="7"/>
       <c r="P56" s="8"/>
-      <c r="Q56" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="R56" s="10"/>
+      <c r="Q56" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="R56" s="22"/>
       <c r="S56" s="11"/>
       <c r="T56" s="12"/>
     </row>
@@ -2102,12 +2109,10 @@
       <c r="M57" s="12"/>
       <c r="O57" s="7"/>
       <c r="P57" s="8"/>
-      <c r="Q57" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="R57" s="16">
-        <v>2.0</v>
-      </c>
+      <c r="Q57" s="32" t="s">
+        <v>46</v>
+      </c>
+      <c r="R57" s="25"/>
       <c r="S57" s="11"/>
       <c r="T57" s="12"/>
     </row>
@@ -2129,7 +2134,7 @@
       <c r="O58" s="7"/>
       <c r="P58" s="8"/>
       <c r="Q58" s="15" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="R58" s="10"/>
       <c r="S58" s="11"/>
@@ -2153,7 +2158,7 @@
       <c r="O59" s="7"/>
       <c r="P59" s="8"/>
       <c r="Q59" s="15" t="s">
-        <v>30</v>
+        <v>55</v>
       </c>
       <c r="R59" s="10"/>
       <c r="S59" s="11"/>
@@ -2179,9 +2184,11 @@
       <c r="O60" s="7"/>
       <c r="P60" s="8"/>
       <c r="Q60" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="R60" s="10"/>
+        <v>32</v>
+      </c>
+      <c r="R60" s="16">
+        <v>1.0</v>
+      </c>
       <c r="S60" s="11"/>
       <c r="T60" s="12"/>
     </row>
@@ -2200,19 +2207,15 @@
       <c r="M61" s="12"/>
       <c r="O61" s="7"/>
       <c r="P61" s="8"/>
-      <c r="Q61" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="R61" s="16">
-        <v>1.0</v>
-      </c>
+      <c r="Q61" s="15"/>
+      <c r="R61" s="16"/>
       <c r="S61" s="11"/>
       <c r="T61" s="12"/>
     </row>
     <row r="62">
       <c r="A62" s="7"/>
       <c r="B62" s="14" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C62" s="15" t="s">
         <v>8</v>
@@ -2229,11 +2232,21 @@
       <c r="L62" s="11"/>
       <c r="M62" s="12"/>
       <c r="O62" s="7"/>
-      <c r="P62" s="8"/>
-      <c r="Q62" s="9"/>
-      <c r="R62" s="10"/>
-      <c r="S62" s="11"/>
-      <c r="T62" s="12"/>
+      <c r="P62" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q62" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="R62" s="19">
+        <v>4.0</v>
+      </c>
+      <c r="S62" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="T62" s="29">
+        <v>2.0</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" s="7"/>
@@ -2251,17 +2264,15 @@
       <c r="L63" s="11"/>
       <c r="M63" s="12"/>
       <c r="O63" s="7"/>
-      <c r="P63" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q63" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="R63" s="16">
-        <v>4.0</v>
-      </c>
-      <c r="S63" s="11"/>
-      <c r="T63" s="12"/>
+      <c r="P63" s="30"/>
+      <c r="Q63" s="23"/>
+      <c r="R63" s="25"/>
+      <c r="S63" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="T63" s="29">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" s="7"/>
@@ -2279,15 +2290,19 @@
       <c r="L64" s="11"/>
       <c r="M64" s="12"/>
       <c r="O64" s="7"/>
-      <c r="P64" s="8"/>
-      <c r="Q64" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="R64" s="16">
+      <c r="P64" s="17"/>
+      <c r="Q64" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="R64" s="24">
         <v>3.0</v>
       </c>
-      <c r="S64" s="11"/>
-      <c r="T64" s="12"/>
+      <c r="S64" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="T64" s="29">
+        <v>2.0</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" s="7"/>
@@ -2305,13 +2320,15 @@
       <c r="L65" s="11"/>
       <c r="M65" s="12"/>
       <c r="O65" s="7"/>
-      <c r="P65" s="8"/>
-      <c r="Q65" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="R65" s="10"/>
-      <c r="S65" s="11"/>
-      <c r="T65" s="12"/>
+      <c r="P65" s="17"/>
+      <c r="Q65" s="23"/>
+      <c r="R65" s="22"/>
+      <c r="S65" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="T65" s="29">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" s="7"/>
@@ -2329,13 +2346,13 @@
       <c r="L66" s="11"/>
       <c r="M66" s="12"/>
       <c r="O66" s="7"/>
-      <c r="P66" s="8"/>
-      <c r="Q66" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="R66" s="16"/>
-      <c r="S66" s="11"/>
-      <c r="T66" s="12"/>
+      <c r="P66" s="17"/>
+      <c r="Q66" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="R66" s="25"/>
+      <c r="S66" s="28"/>
+      <c r="T66" s="33"/>
     </row>
     <row r="67">
       <c r="A67" s="7"/>
@@ -2355,13 +2372,13 @@
       <c r="L67" s="11"/>
       <c r="M67" s="12"/>
       <c r="O67" s="7"/>
-      <c r="P67" s="8"/>
-      <c r="Q67" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="R67" s="10"/>
-      <c r="S67" s="11"/>
-      <c r="T67" s="12"/>
+      <c r="P67" s="17"/>
+      <c r="Q67" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="R67" s="22"/>
+      <c r="S67" s="28"/>
+      <c r="T67" s="33"/>
     </row>
     <row r="68">
       <c r="A68" s="7"/>
@@ -2379,13 +2396,13 @@
       <c r="L68" s="11"/>
       <c r="M68" s="12"/>
       <c r="O68" s="7"/>
-      <c r="P68" s="8"/>
-      <c r="Q68" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="R68" s="10"/>
-      <c r="S68" s="11"/>
-      <c r="T68" s="12"/>
+      <c r="P68" s="17"/>
+      <c r="Q68" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="R68" s="22"/>
+      <c r="S68" s="28"/>
+      <c r="T68" s="33"/>
     </row>
     <row r="69">
       <c r="A69" s="7"/>
@@ -2403,15 +2420,13 @@
       <c r="L69" s="11"/>
       <c r="M69" s="12"/>
       <c r="O69" s="7"/>
-      <c r="P69" s="8"/>
-      <c r="Q69" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="R69" s="16">
-        <v>2.0</v>
-      </c>
-      <c r="S69" s="11"/>
-      <c r="T69" s="12"/>
+      <c r="P69" s="17"/>
+      <c r="Q69" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="R69" s="25"/>
+      <c r="S69" s="28"/>
+      <c r="T69" s="33"/>
     </row>
     <row r="70">
       <c r="A70" s="7"/>
@@ -2429,13 +2444,15 @@
       <c r="L70" s="11"/>
       <c r="M70" s="12"/>
       <c r="O70" s="7"/>
-      <c r="P70" s="8"/>
-      <c r="Q70" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="R70" s="10"/>
-      <c r="S70" s="11"/>
-      <c r="T70" s="12"/>
+      <c r="P70" s="17"/>
+      <c r="Q70" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="R70" s="19">
+        <v>2.0</v>
+      </c>
+      <c r="S70" s="28"/>
+      <c r="T70" s="33"/>
     </row>
     <row r="71">
       <c r="A71" s="7"/>
@@ -2453,13 +2470,13 @@
       <c r="L71" s="11"/>
       <c r="M71" s="12"/>
       <c r="O71" s="7"/>
-      <c r="P71" s="8"/>
-      <c r="Q71" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="R71" s="10"/>
-      <c r="S71" s="11"/>
-      <c r="T71" s="12"/>
+      <c r="P71" s="17"/>
+      <c r="Q71" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="R71" s="22"/>
+      <c r="S71" s="28"/>
+      <c r="T71" s="33"/>
     </row>
     <row r="72">
       <c r="A72" s="7"/>
@@ -2477,13 +2494,13 @@
       <c r="L72" s="11"/>
       <c r="M72" s="12"/>
       <c r="O72" s="7"/>
-      <c r="P72" s="8"/>
-      <c r="Q72" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="R72" s="16"/>
-      <c r="S72" s="11"/>
-      <c r="T72" s="12"/>
+      <c r="P72" s="17"/>
+      <c r="Q72" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="R72" s="25"/>
+      <c r="S72" s="28"/>
+      <c r="T72" s="33"/>
     </row>
     <row r="73">
       <c r="A73" s="7"/>
@@ -2503,15 +2520,13 @@
       <c r="L73" s="11"/>
       <c r="M73" s="12"/>
       <c r="O73" s="7"/>
-      <c r="P73" s="8"/>
-      <c r="Q73" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="R73" s="16">
-        <v>1.0</v>
-      </c>
-      <c r="S73" s="11"/>
-      <c r="T73" s="12"/>
+      <c r="P73" s="17"/>
+      <c r="Q73" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="R73" s="25"/>
+      <c r="S73" s="28"/>
+      <c r="T73" s="33"/>
     </row>
     <row r="74">
       <c r="A74" s="7"/>
@@ -2527,16 +2542,20 @@
       <c r="L74" s="11"/>
       <c r="M74" s="12"/>
       <c r="O74" s="7"/>
-      <c r="P74" s="8"/>
-      <c r="Q74" s="9"/>
-      <c r="R74" s="10"/>
-      <c r="S74" s="11"/>
-      <c r="T74" s="12"/>
+      <c r="P74" s="17"/>
+      <c r="Q74" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="R74" s="19">
+        <v>1.0</v>
+      </c>
+      <c r="S74" s="28"/>
+      <c r="T74" s="33"/>
     </row>
     <row r="75">
       <c r="A75" s="7"/>
       <c r="B75" s="14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C75" s="15" t="s">
         <v>8</v>
@@ -2553,11 +2572,11 @@
       <c r="L75" s="11"/>
       <c r="M75" s="12"/>
       <c r="O75" s="7"/>
-      <c r="P75" s="8"/>
-      <c r="Q75" s="9"/>
-      <c r="R75" s="10"/>
-      <c r="S75" s="11"/>
-      <c r="T75" s="12"/>
+      <c r="P75" s="17"/>
+      <c r="Q75" s="18"/>
+      <c r="R75" s="22"/>
+      <c r="S75" s="28"/>
+      <c r="T75" s="33"/>
     </row>
     <row r="76">
       <c r="A76" s="7"/>
@@ -2575,11 +2594,17 @@
       <c r="L76" s="11"/>
       <c r="M76" s="12"/>
       <c r="O76" s="7"/>
-      <c r="P76" s="8"/>
-      <c r="Q76" s="9"/>
-      <c r="R76" s="10"/>
-      <c r="S76" s="11"/>
-      <c r="T76" s="12"/>
+      <c r="P76" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q76" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="R76" s="19">
+        <v>4.0</v>
+      </c>
+      <c r="S76" s="28"/>
+      <c r="T76" s="33"/>
     </row>
     <row r="77">
       <c r="A77" s="7"/>
@@ -2597,11 +2622,15 @@
       <c r="L77" s="11"/>
       <c r="M77" s="12"/>
       <c r="O77" s="7"/>
-      <c r="P77" s="8"/>
-      <c r="Q77" s="9"/>
-      <c r="R77" s="10"/>
-      <c r="S77" s="11"/>
-      <c r="T77" s="12"/>
+      <c r="P77" s="17"/>
+      <c r="Q77" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="R77" s="19">
+        <v>3.0</v>
+      </c>
+      <c r="S77" s="28"/>
+      <c r="T77" s="33"/>
     </row>
     <row r="78">
       <c r="A78" s="7"/>
@@ -2619,11 +2648,13 @@
       <c r="L78" s="11"/>
       <c r="M78" s="12"/>
       <c r="O78" s="7"/>
-      <c r="P78" s="8"/>
-      <c r="Q78" s="9"/>
-      <c r="R78" s="10"/>
-      <c r="S78" s="11"/>
-      <c r="T78" s="12"/>
+      <c r="P78" s="17"/>
+      <c r="Q78" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="R78" s="22"/>
+      <c r="S78" s="28"/>
+      <c r="T78" s="33"/>
     </row>
     <row r="79">
       <c r="A79" s="7"/>
@@ -2643,11 +2674,13 @@
       <c r="L79" s="11"/>
       <c r="M79" s="12"/>
       <c r="O79" s="7"/>
-      <c r="P79" s="8"/>
-      <c r="Q79" s="9"/>
-      <c r="R79" s="10"/>
-      <c r="S79" s="11"/>
-      <c r="T79" s="12"/>
+      <c r="P79" s="17"/>
+      <c r="Q79" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="R79" s="22"/>
+      <c r="S79" s="28"/>
+      <c r="T79" s="33"/>
     </row>
     <row r="80">
       <c r="A80" s="7"/>
@@ -2665,11 +2698,13 @@
       <c r="L80" s="11"/>
       <c r="M80" s="12"/>
       <c r="O80" s="7"/>
-      <c r="P80" s="8"/>
-      <c r="Q80" s="9"/>
-      <c r="R80" s="10"/>
-      <c r="S80" s="11"/>
-      <c r="T80" s="12"/>
+      <c r="P80" s="17"/>
+      <c r="Q80" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="R80" s="22"/>
+      <c r="S80" s="28"/>
+      <c r="T80" s="33"/>
     </row>
     <row r="81">
       <c r="A81" s="7"/>
@@ -2687,11 +2722,13 @@
       <c r="L81" s="11"/>
       <c r="M81" s="12"/>
       <c r="O81" s="7"/>
-      <c r="P81" s="8"/>
-      <c r="Q81" s="9"/>
-      <c r="R81" s="10"/>
-      <c r="S81" s="11"/>
-      <c r="T81" s="12"/>
+      <c r="P81" s="17"/>
+      <c r="Q81" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="R81" s="22"/>
+      <c r="S81" s="28"/>
+      <c r="T81" s="33"/>
     </row>
     <row r="82">
       <c r="A82" s="7"/>
@@ -2709,11 +2746,15 @@
       <c r="L82" s="11"/>
       <c r="M82" s="12"/>
       <c r="O82" s="7"/>
-      <c r="P82" s="8"/>
-      <c r="Q82" s="9"/>
-      <c r="R82" s="10"/>
-      <c r="S82" s="11"/>
-      <c r="T82" s="12"/>
+      <c r="P82" s="17"/>
+      <c r="Q82" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="R82" s="19">
+        <v>2.0</v>
+      </c>
+      <c r="S82" s="28"/>
+      <c r="T82" s="33"/>
     </row>
     <row r="83">
       <c r="A83" s="7"/>
@@ -2731,11 +2772,13 @@
       <c r="L83" s="11"/>
       <c r="M83" s="12"/>
       <c r="O83" s="7"/>
-      <c r="P83" s="8"/>
-      <c r="Q83" s="9"/>
-      <c r="R83" s="10"/>
-      <c r="S83" s="11"/>
-      <c r="T83" s="12"/>
+      <c r="P83" s="17"/>
+      <c r="Q83" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="R83" s="22"/>
+      <c r="S83" s="28"/>
+      <c r="T83" s="33"/>
     </row>
     <row r="84">
       <c r="A84" s="7"/>
@@ -2753,11 +2796,13 @@
       <c r="L84" s="11"/>
       <c r="M84" s="12"/>
       <c r="O84" s="7"/>
-      <c r="P84" s="8"/>
-      <c r="Q84" s="9"/>
-      <c r="R84" s="10"/>
-      <c r="S84" s="11"/>
-      <c r="T84" s="12"/>
+      <c r="P84" s="17"/>
+      <c r="Q84" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="R84" s="22"/>
+      <c r="S84" s="28"/>
+      <c r="T84" s="33"/>
     </row>
     <row r="85">
       <c r="A85" s="7"/>
@@ -2777,11 +2822,13 @@
       <c r="L85" s="11"/>
       <c r="M85" s="12"/>
       <c r="O85" s="7"/>
-      <c r="P85" s="8"/>
-      <c r="Q85" s="9"/>
-      <c r="R85" s="10"/>
-      <c r="S85" s="11"/>
-      <c r="T85" s="12"/>
+      <c r="P85" s="17"/>
+      <c r="Q85" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="R85" s="22"/>
+      <c r="S85" s="28"/>
+      <c r="T85" s="33"/>
     </row>
     <row r="86">
       <c r="A86" s="7"/>
@@ -2797,16 +2844,20 @@
       <c r="L86" s="11"/>
       <c r="M86" s="12"/>
       <c r="O86" s="7"/>
-      <c r="P86" s="8"/>
-      <c r="Q86" s="9"/>
-      <c r="R86" s="10"/>
-      <c r="S86" s="11"/>
-      <c r="T86" s="12"/>
+      <c r="P86" s="17"/>
+      <c r="Q86" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="R86" s="19">
+        <v>1.0</v>
+      </c>
+      <c r="S86" s="28"/>
+      <c r="T86" s="33"/>
     </row>
     <row r="87">
       <c r="A87" s="7"/>
       <c r="B87" s="14" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C87" s="15" t="s">
         <v>8</v>
@@ -2823,11 +2874,11 @@
       <c r="L87" s="11"/>
       <c r="M87" s="12"/>
       <c r="O87" s="7"/>
-      <c r="P87" s="8"/>
-      <c r="Q87" s="9"/>
-      <c r="R87" s="10"/>
-      <c r="S87" s="11"/>
-      <c r="T87" s="12"/>
+      <c r="P87" s="17"/>
+      <c r="Q87" s="18"/>
+      <c r="R87" s="22"/>
+      <c r="S87" s="28"/>
+      <c r="T87" s="33"/>
     </row>
     <row r="88">
       <c r="A88" s="7"/>
@@ -2845,11 +2896,11 @@
       <c r="L88" s="11"/>
       <c r="M88" s="12"/>
       <c r="O88" s="7"/>
-      <c r="P88" s="8"/>
-      <c r="Q88" s="9"/>
-      <c r="R88" s="10"/>
-      <c r="S88" s="11"/>
-      <c r="T88" s="12"/>
+      <c r="P88" s="17"/>
+      <c r="Q88" s="18"/>
+      <c r="R88" s="22"/>
+      <c r="S88" s="28"/>
+      <c r="T88" s="33"/>
     </row>
     <row r="89">
       <c r="A89" s="7"/>
@@ -2867,17 +2918,17 @@
       <c r="L89" s="11"/>
       <c r="M89" s="12"/>
       <c r="O89" s="7"/>
-      <c r="P89" s="8"/>
-      <c r="Q89" s="9"/>
-      <c r="R89" s="10"/>
-      <c r="S89" s="11"/>
-      <c r="T89" s="12"/>
+      <c r="P89" s="17"/>
+      <c r="Q89" s="18"/>
+      <c r="R89" s="19"/>
+      <c r="S89" s="28"/>
+      <c r="T89" s="33"/>
     </row>
     <row r="90">
       <c r="A90" s="7"/>
       <c r="B90" s="8"/>
       <c r="C90" s="15" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="D90" s="16">
         <v>3.0</v>
@@ -2891,11 +2942,11 @@
       <c r="L90" s="11"/>
       <c r="M90" s="12"/>
       <c r="O90" s="7"/>
-      <c r="P90" s="8"/>
-      <c r="Q90" s="9"/>
-      <c r="R90" s="10"/>
-      <c r="S90" s="11"/>
-      <c r="T90" s="12"/>
+      <c r="P90" s="17"/>
+      <c r="Q90" s="18"/>
+      <c r="R90" s="22"/>
+      <c r="S90" s="28"/>
+      <c r="T90" s="33"/>
     </row>
     <row r="91">
       <c r="A91" s="7"/>
@@ -2915,11 +2966,11 @@
       <c r="L91" s="11"/>
       <c r="M91" s="12"/>
       <c r="O91" s="7"/>
-      <c r="P91" s="8"/>
-      <c r="Q91" s="9"/>
-      <c r="R91" s="10"/>
-      <c r="S91" s="11"/>
-      <c r="T91" s="12"/>
+      <c r="P91" s="17"/>
+      <c r="Q91" s="18"/>
+      <c r="R91" s="22"/>
+      <c r="S91" s="28"/>
+      <c r="T91" s="33"/>
     </row>
     <row r="92">
       <c r="A92" s="7"/>
@@ -2937,11 +2988,11 @@
       <c r="L92" s="11"/>
       <c r="M92" s="12"/>
       <c r="O92" s="7"/>
-      <c r="P92" s="8"/>
-      <c r="Q92" s="9"/>
-      <c r="R92" s="10"/>
-      <c r="S92" s="11"/>
-      <c r="T92" s="12"/>
+      <c r="P92" s="17"/>
+      <c r="Q92" s="18"/>
+      <c r="R92" s="22"/>
+      <c r="S92" s="28"/>
+      <c r="T92" s="33"/>
     </row>
     <row r="93">
       <c r="A93" s="7"/>
@@ -2959,11 +3010,11 @@
       <c r="L93" s="11"/>
       <c r="M93" s="12"/>
       <c r="O93" s="7"/>
-      <c r="P93" s="8"/>
-      <c r="Q93" s="9"/>
-      <c r="R93" s="10"/>
-      <c r="S93" s="11"/>
-      <c r="T93" s="12"/>
+      <c r="P93" s="17"/>
+      <c r="Q93" s="18"/>
+      <c r="R93" s="19"/>
+      <c r="S93" s="28"/>
+      <c r="T93" s="33"/>
     </row>
     <row r="94">
       <c r="A94" s="7"/>
@@ -3122,7 +3173,7 @@
     <row r="101">
       <c r="A101" s="7"/>
       <c r="B101" s="14" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="C101" s="15" t="s">
         <v>8</v>
@@ -3438,7 +3489,7 @@
     <row r="115">
       <c r="A115" s="7"/>
       <c r="B115" s="14" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="C115" s="15" t="s">
         <v>17</v>
@@ -3732,7 +3783,7 @@
     <row r="128">
       <c r="A128" s="7"/>
       <c r="B128" s="14" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C128" s="15" t="s">
         <v>17</v>
@@ -4026,7 +4077,7 @@
     <row r="141">
       <c r="A141" s="7"/>
       <c r="B141" s="14" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C141" s="15" t="s">
         <v>11</v>
@@ -4320,7 +4371,7 @@
     <row r="154">
       <c r="A154" s="7"/>
       <c r="B154" s="14" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="C154" s="15" t="s">
         <v>11</v>
@@ -4614,7 +4665,7 @@
     <row r="167">
       <c r="A167" s="7"/>
       <c r="B167" s="14" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="C167" s="15" t="s">
         <v>26</v>
@@ -4930,7 +4981,7 @@
     <row r="181">
       <c r="A181" s="7"/>
       <c r="B181" s="14" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="C181" s="15" t="s">
         <v>26</v>
@@ -5246,7 +5297,7 @@
     <row r="195">
       <c r="A195" s="7"/>
       <c r="B195" s="14" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C195" s="15" t="s">
         <v>27</v>
@@ -5255,7 +5306,7 @@
         <v>4.0</v>
       </c>
       <c r="E195" s="20" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="F195" s="21">
         <v>1.25</v>
@@ -5279,7 +5330,7 @@
       <c r="C196" s="15"/>
       <c r="D196" s="16"/>
       <c r="E196" s="20" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="F196" s="21">
         <v>1.25</v>
@@ -5303,7 +5354,7 @@
       <c r="C197" s="15"/>
       <c r="D197" s="16"/>
       <c r="E197" s="20" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="F197" s="21">
         <v>1.25</v>
@@ -5592,7 +5643,7 @@
     <row r="210">
       <c r="A210" s="7"/>
       <c r="B210" s="14" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C210" s="15" t="s">
         <v>27</v>
@@ -5601,7 +5652,7 @@
         <v>4.0</v>
       </c>
       <c r="E210" s="20" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="F210" s="21">
         <v>1.0</v>
@@ -5625,7 +5676,7 @@
       <c r="C211" s="15"/>
       <c r="D211" s="16"/>
       <c r="E211" s="20" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="F211" s="21">
         <v>1.0</v>
@@ -5649,7 +5700,7 @@
       <c r="C212" s="15"/>
       <c r="D212" s="16"/>
       <c r="E212" s="20" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="F212" s="21">
         <v>1.0</v>
@@ -5938,7 +5989,7 @@
     <row r="225">
       <c r="A225" s="7"/>
       <c r="B225" s="14" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="C225" s="15" t="s">
         <v>30</v>
@@ -6232,7 +6283,7 @@
     <row r="238">
       <c r="A238" s="7"/>
       <c r="B238" s="14" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C238" s="15" t="s">
         <v>30</v>
@@ -6526,7 +6577,7 @@
     <row r="251">
       <c r="A251" s="7"/>
       <c r="B251" s="14" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C251" s="15" t="s">
         <v>26</v>
@@ -6864,7 +6915,7 @@
     <row r="266">
       <c r="A266" s="7"/>
       <c r="B266" s="14" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C266" s="15" t="s">
         <v>26</v>
@@ -7202,7 +7253,7 @@
     <row r="281">
       <c r="A281" s="7"/>
       <c r="B281" s="14" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C281" s="15" t="s">
         <v>8</v>
@@ -7273,7 +7324,7 @@
       <c r="A284" s="7"/>
       <c r="B284" s="8"/>
       <c r="C284" s="15" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="D284" s="16">
         <v>3.0</v>
@@ -7297,7 +7348,7 @@
       <c r="A285" s="7"/>
       <c r="B285" s="8"/>
       <c r="C285" s="15" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="D285" s="16"/>
       <c r="E285" s="20" t="s">
@@ -7325,7 +7376,7 @@
       <c r="C286" s="15"/>
       <c r="D286" s="16"/>
       <c r="E286" s="20" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="F286" s="21">
         <v>1.0</v>
@@ -7480,7 +7531,7 @@
     <row r="293">
       <c r="A293" s="7"/>
       <c r="B293" s="14" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="C293" s="15" t="s">
         <v>8</v>
@@ -7575,7 +7626,7 @@
       <c r="A297" s="7"/>
       <c r="B297" s="8"/>
       <c r="C297" s="15" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="D297" s="16"/>
       <c r="E297" s="11"/>
@@ -7597,7 +7648,7 @@
       <c r="A298" s="7"/>
       <c r="B298" s="8"/>
       <c r="C298" s="15" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="D298" s="16"/>
       <c r="E298" s="20" t="s">
@@ -7625,7 +7676,7 @@
       <c r="C299" s="15"/>
       <c r="D299" s="16"/>
       <c r="E299" s="20" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="F299" s="21">
         <v>1.0</v>
@@ -7758,7 +7809,7 @@
     <row r="305">
       <c r="A305" s="7"/>
       <c r="B305" s="14" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="C305" s="15" t="s">
         <v>36</v>
@@ -7903,7 +7954,7 @@
       <c r="A311" s="7"/>
       <c r="B311" s="8"/>
       <c r="C311" s="15" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="D311" s="10"/>
       <c r="E311" s="20" t="s">
@@ -7931,7 +7982,7 @@
       <c r="C312" s="9"/>
       <c r="D312" s="10"/>
       <c r="E312" s="20" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="F312" s="21">
         <v>1.0</v>
@@ -8064,7 +8115,7 @@
     <row r="318">
       <c r="A318" s="7"/>
       <c r="B318" s="14" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="C318" s="15" t="s">
         <v>36</v>
@@ -8231,7 +8282,7 @@
       <c r="A325" s="7"/>
       <c r="B325" s="8"/>
       <c r="C325" s="15" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="D325" s="10"/>
       <c r="E325" s="20" t="s">
@@ -8259,7 +8310,7 @@
       <c r="C326" s="9"/>
       <c r="D326" s="10"/>
       <c r="E326" s="20" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="F326" s="21">
         <v>1.0</v>
@@ -8392,7 +8443,7 @@
     <row r="332">
       <c r="A332" s="7"/>
       <c r="B332" s="14" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="C332" s="15" t="s">
         <v>11</v>
@@ -8509,7 +8560,7 @@
       <c r="A337" s="7"/>
       <c r="B337" s="8"/>
       <c r="C337" s="15" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="D337" s="10"/>
       <c r="E337" s="20" t="s">
@@ -8537,7 +8588,7 @@
       <c r="C338" s="9"/>
       <c r="D338" s="10"/>
       <c r="E338" s="20" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="F338" s="21">
         <v>1.0</v>
@@ -8670,7 +8721,7 @@
     <row r="344">
       <c r="A344" s="7"/>
       <c r="B344" s="14" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="C344" s="15" t="s">
         <v>11</v>
@@ -8809,7 +8860,7 @@
       <c r="A350" s="7"/>
       <c r="B350" s="8"/>
       <c r="C350" s="15" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="D350" s="10"/>
       <c r="E350" s="20" t="s">
@@ -8837,7 +8888,7 @@
       <c r="C351" s="9"/>
       <c r="D351" s="10"/>
       <c r="E351" s="20" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="F351" s="21">
         <v>1.0</v>
@@ -8970,7 +9021,7 @@
     <row r="357">
       <c r="A357" s="7"/>
       <c r="B357" s="14" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="C357" s="15" t="s">
         <v>26</v>
@@ -9087,7 +9138,7 @@
       <c r="A362" s="7"/>
       <c r="B362" s="8"/>
       <c r="C362" s="15" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="D362" s="10"/>
       <c r="E362" s="20" t="s">
@@ -9115,7 +9166,7 @@
       <c r="C363" s="9"/>
       <c r="D363" s="10"/>
       <c r="E363" s="20" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="F363" s="21">
         <v>1.0</v>
@@ -9270,7 +9321,7 @@
     <row r="370">
       <c r="A370" s="7"/>
       <c r="B370" s="14" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C370" s="15" t="s">
         <v>26</v>
@@ -9409,7 +9460,7 @@
       <c r="A376" s="7"/>
       <c r="B376" s="8"/>
       <c r="C376" s="15" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="D376" s="10"/>
       <c r="E376" s="20" t="s">
@@ -9437,7 +9488,7 @@
       <c r="C377" s="9"/>
       <c r="D377" s="10"/>
       <c r="E377" s="20" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="F377" s="21">
         <v>1.0</v>
@@ -9548,16 +9599,16 @@
     <row r="382">
       <c r="A382" s="7"/>
       <c r="B382" s="14" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="C382" s="15" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="D382" s="16">
         <v>4.0</v>
       </c>
       <c r="E382" s="20" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="F382" s="21">
         <v>2.0</v>
@@ -9581,7 +9632,7 @@
       <c r="C383" s="9"/>
       <c r="D383" s="10"/>
       <c r="E383" s="20" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="F383" s="21">
         <v>2.0</v>
@@ -9603,15 +9654,15 @@
       <c r="A384" s="7"/>
       <c r="B384" s="8"/>
       <c r="C384" s="15" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="D384" s="16">
         <v>3.0</v>
       </c>
       <c r="E384" s="20" t="s">
-        <v>96</v>
-      </c>
-      <c r="F384" s="33">
+        <v>99</v>
+      </c>
+      <c r="F384" s="34">
         <v>43221.0</v>
       </c>
       <c r="H384" s="7"/>
@@ -9633,9 +9684,9 @@
       <c r="C385" s="9"/>
       <c r="D385" s="10"/>
       <c r="E385" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="F385" s="33">
+        <v>81</v>
+      </c>
+      <c r="F385" s="34">
         <v>43221.0</v>
       </c>
       <c r="H385" s="7"/>
@@ -9721,7 +9772,7 @@
       <c r="A389" s="7"/>
       <c r="B389" s="8"/>
       <c r="C389" s="15" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="D389" s="10"/>
       <c r="E389" s="20" t="s">
@@ -9749,7 +9800,7 @@
       <c r="C390" s="9"/>
       <c r="D390" s="10"/>
       <c r="E390" s="20" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="F390" s="21">
         <v>1.0</v>
@@ -9926,16 +9977,16 @@
     <row r="398">
       <c r="A398" s="7"/>
       <c r="B398" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="C398" s="15" t="s">
         <v>97</v>
-      </c>
-      <c r="C398" s="15" t="s">
-        <v>94</v>
       </c>
       <c r="D398" s="16">
         <v>4.0</v>
       </c>
       <c r="E398" s="20" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="F398" s="21">
         <v>2.0</v>
@@ -9959,7 +10010,7 @@
       <c r="C399" s="9"/>
       <c r="D399" s="10"/>
       <c r="E399" s="20" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="F399" s="21">
         <v>2.0</v>
@@ -9981,13 +10032,13 @@
       <c r="A400" s="7"/>
       <c r="B400" s="8"/>
       <c r="C400" s="15" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="D400" s="16">
         <v>3.0</v>
       </c>
       <c r="E400" s="20" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="F400" s="21">
         <v>1.5</v>
@@ -10011,7 +10062,7 @@
       <c r="C401" s="9"/>
       <c r="D401" s="10"/>
       <c r="E401" s="20" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="F401" s="21">
         <v>1.5</v>
@@ -10121,7 +10172,7 @@
       <c r="A406" s="7"/>
       <c r="B406" s="8"/>
       <c r="C406" s="15" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="D406" s="10"/>
       <c r="E406" s="20" t="s">
@@ -10149,7 +10200,7 @@
       <c r="C407" s="9"/>
       <c r="D407" s="10"/>
       <c r="E407" s="20" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="F407" s="21">
         <v>1.0</v>
@@ -10326,10 +10377,10 @@
     <row r="415">
       <c r="A415" s="7"/>
       <c r="B415" s="14" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="C415" s="15" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="D415" s="16">
         <v>4.0</v>
@@ -10353,7 +10404,7 @@
       <c r="A416" s="7"/>
       <c r="B416" s="8"/>
       <c r="C416" s="15" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="D416" s="16">
         <v>3.0</v>
@@ -10443,7 +10494,7 @@
       <c r="A420" s="7"/>
       <c r="B420" s="8"/>
       <c r="C420" s="15" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="D420" s="10"/>
       <c r="E420" s="20" t="s">
@@ -10471,7 +10522,7 @@
       <c r="C421" s="9"/>
       <c r="D421" s="10"/>
       <c r="E421" s="20" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="F421" s="21">
         <v>1.0</v>
@@ -10648,10 +10699,10 @@
     <row r="429">
       <c r="A429" s="7"/>
       <c r="B429" s="14" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="C429" s="15" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="D429" s="16">
         <v>4.0</v>
@@ -10675,7 +10726,7 @@
       <c r="A430" s="7"/>
       <c r="B430" s="8"/>
       <c r="C430" s="15" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="D430" s="16">
         <v>3.0</v>
@@ -10787,7 +10838,7 @@
       <c r="A435" s="7"/>
       <c r="B435" s="8"/>
       <c r="C435" s="15" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="D435" s="10"/>
       <c r="E435" s="20" t="s">
@@ -10815,7 +10866,7 @@
       <c r="C436" s="9"/>
       <c r="D436" s="10"/>
       <c r="E436" s="20" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="F436" s="21">
         <v>1.0</v>
@@ -10992,7 +11043,7 @@
     <row r="444">
       <c r="A444" s="7"/>
       <c r="B444" s="14" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="C444" s="15" t="s">
         <v>26</v>
@@ -11087,7 +11138,7 @@
       <c r="A448" s="7"/>
       <c r="B448" s="8"/>
       <c r="C448" s="15" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="D448" s="10"/>
       <c r="E448" s="20" t="s">
@@ -11115,7 +11166,7 @@
       <c r="C449" s="9"/>
       <c r="D449" s="10"/>
       <c r="E449" s="20" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="F449" s="21">
         <v>1.0</v>
@@ -11319,7 +11370,7 @@
       <c r="C458" s="18"/>
       <c r="D458" s="22"/>
       <c r="E458" s="28"/>
-      <c r="F458" s="34"/>
+      <c r="F458" s="33"/>
       <c r="H458" s="7"/>
       <c r="I458" s="8"/>
       <c r="J458" s="9"/>
@@ -11336,7 +11387,7 @@
     <row r="459">
       <c r="A459" s="7"/>
       <c r="B459" s="27" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="C459" s="18" t="s">
         <v>26</v>
@@ -11345,7 +11396,7 @@
         <v>4.0</v>
       </c>
       <c r="E459" s="28"/>
-      <c r="F459" s="34"/>
+      <c r="F459" s="33"/>
       <c r="H459" s="7"/>
       <c r="I459" s="8"/>
       <c r="J459" s="9"/>
@@ -11369,7 +11420,7 @@
         <v>3.0</v>
       </c>
       <c r="E460" s="28"/>
-      <c r="F460" s="34"/>
+      <c r="F460" s="33"/>
       <c r="H460" s="7"/>
       <c r="I460" s="8"/>
       <c r="J460" s="9"/>
@@ -11391,7 +11442,7 @@
       </c>
       <c r="D461" s="22"/>
       <c r="E461" s="28"/>
-      <c r="F461" s="34"/>
+      <c r="F461" s="33"/>
       <c r="H461" s="7"/>
       <c r="I461" s="8"/>
       <c r="J461" s="9"/>
@@ -11413,7 +11464,7 @@
       </c>
       <c r="D462" s="22"/>
       <c r="E462" s="28"/>
-      <c r="F462" s="34"/>
+      <c r="F462" s="33"/>
       <c r="H462" s="7"/>
       <c r="I462" s="8"/>
       <c r="J462" s="9"/>
@@ -11435,7 +11486,7 @@
       </c>
       <c r="D463" s="22"/>
       <c r="E463" s="28"/>
-      <c r="F463" s="34"/>
+      <c r="F463" s="33"/>
       <c r="H463" s="7"/>
       <c r="I463" s="8"/>
       <c r="J463" s="9"/>
@@ -11453,7 +11504,7 @@
       <c r="A464" s="7"/>
       <c r="B464" s="17"/>
       <c r="C464" s="18" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="D464" s="22"/>
       <c r="E464" s="28" t="s">
@@ -11481,7 +11532,7 @@
       <c r="C465" s="18"/>
       <c r="D465" s="22"/>
       <c r="E465" s="28" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="F465" s="29">
         <v>1.0</v>
@@ -11509,7 +11560,7 @@
         <v>2.0</v>
       </c>
       <c r="E466" s="28"/>
-      <c r="F466" s="34"/>
+      <c r="F466" s="33"/>
       <c r="H466" s="7"/>
       <c r="I466" s="8"/>
       <c r="J466" s="9"/>
@@ -11531,7 +11582,7 @@
       </c>
       <c r="D467" s="22"/>
       <c r="E467" s="28"/>
-      <c r="F467" s="34"/>
+      <c r="F467" s="33"/>
       <c r="H467" s="7"/>
       <c r="I467" s="8"/>
       <c r="J467" s="9"/>
@@ -11553,7 +11604,7 @@
       </c>
       <c r="D468" s="22"/>
       <c r="E468" s="28"/>
-      <c r="F468" s="34"/>
+      <c r="F468" s="33"/>
       <c r="H468" s="7"/>
       <c r="I468" s="8"/>
       <c r="J468" s="9"/>
@@ -11575,7 +11626,7 @@
       </c>
       <c r="D469" s="22"/>
       <c r="E469" s="28"/>
-      <c r="F469" s="34"/>
+      <c r="F469" s="33"/>
       <c r="H469" s="7"/>
       <c r="I469" s="8"/>
       <c r="J469" s="9"/>
@@ -11597,7 +11648,7 @@
       </c>
       <c r="D470" s="22"/>
       <c r="E470" s="28"/>
-      <c r="F470" s="34"/>
+      <c r="F470" s="33"/>
       <c r="H470" s="7"/>
       <c r="I470" s="8"/>
       <c r="J470" s="9"/>
@@ -11619,7 +11670,7 @@
       </c>
       <c r="D471" s="22"/>
       <c r="E471" s="28"/>
-      <c r="F471" s="34"/>
+      <c r="F471" s="33"/>
       <c r="H471" s="7"/>
       <c r="I471" s="8"/>
       <c r="J471" s="9"/>
@@ -11641,7 +11692,7 @@
       </c>
       <c r="D472" s="22"/>
       <c r="E472" s="28"/>
-      <c r="F472" s="34"/>
+      <c r="F472" s="33"/>
       <c r="H472" s="7"/>
       <c r="I472" s="8"/>
       <c r="J472" s="9"/>
@@ -11665,7 +11716,7 @@
         <v>1.0</v>
       </c>
       <c r="E473" s="28"/>
-      <c r="F473" s="34"/>
+      <c r="F473" s="33"/>
       <c r="H473" s="7"/>
       <c r="I473" s="8"/>
       <c r="J473" s="9"/>
@@ -11704,10 +11755,10 @@
         <v>9</v>
       </c>
       <c r="B475" s="14" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="C475" s="15" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="D475" s="16">
         <v>4.0</v>
@@ -11797,7 +11848,7 @@
       <c r="A479" s="7"/>
       <c r="B479" s="8"/>
       <c r="C479" s="15" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="D479" s="10"/>
       <c r="E479" s="20" t="s">
@@ -11847,7 +11898,7 @@
       <c r="A481" s="7"/>
       <c r="B481" s="8"/>
       <c r="C481" s="15" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="D481" s="10"/>
       <c r="E481" s="20" t="s">
@@ -11923,7 +11974,7 @@
       <c r="C484" s="9"/>
       <c r="D484" s="10"/>
       <c r="E484" s="20" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="F484" s="21">
         <v>1.0</v>

</xml_diff>

<commit_message>
v2.1.2: added Biologie to 3MF and 3CF
</commit_message>
<xml_diff>
--- a/assets/All Classes.xlsx
+++ b/assets/All Classes.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1276" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1278" uniqueCount="258">
   <si>
     <t>Macros</t>
   </si>
@@ -640,15 +640,15 @@
     <t>Langage Médias</t>
   </si>
   <si>
+    <t>Travail Personnel</t>
+  </si>
+  <si>
+    <t>Communication</t>
+  </si>
+  <si>
     <t>3MG</t>
   </si>
   <si>
-    <t>Travail Personnel</t>
-  </si>
-  <si>
-    <t>Communication</t>
-  </si>
-  <si>
     <t>Sciences</t>
   </si>
   <si>
@@ -667,12 +667,12 @@
     <t>2GSH</t>
   </si>
   <si>
+    <t>4GSO</t>
+  </si>
+  <si>
     <t>2CA</t>
   </si>
   <si>
-    <t>4GSO</t>
-  </si>
-  <si>
     <t>Histo/Civique</t>
   </si>
   <si>
@@ -763,10 +763,10 @@
     <t>3GSN</t>
   </si>
   <si>
+    <t>2GSN</t>
+  </si>
+  <si>
     <t>2CF</t>
-  </si>
-  <si>
-    <t>2GSN</t>
   </si>
   <si>
     <t>4GACV</t>
@@ -7591,7 +7591,7 @@
       <c r="A231" s="8"/>
       <c r="B231" s="9"/>
       <c r="C231" s="17" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="D231" s="18"/>
       <c r="E231" s="12"/>
@@ -7617,7 +7617,7 @@
       <c r="A232" s="8"/>
       <c r="B232" s="9"/>
       <c r="C232" s="17" t="s">
-        <v>31</v>
+        <v>55</v>
       </c>
       <c r="D232" s="18"/>
       <c r="E232" s="12"/>
@@ -7643,9 +7643,9 @@
       <c r="A233" s="8"/>
       <c r="B233" s="9"/>
       <c r="C233" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="D233" s="11"/>
+        <v>31</v>
+      </c>
+      <c r="D233" s="18"/>
       <c r="E233" s="12"/>
       <c r="F233" s="13"/>
       <c r="H233" s="8"/>
@@ -7671,7 +7671,7 @@
       <c r="A234" s="8"/>
       <c r="B234" s="9"/>
       <c r="C234" s="17" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D234" s="11"/>
       <c r="E234" s="12"/>
@@ -7699,7 +7699,7 @@
       <c r="A235" s="8"/>
       <c r="B235" s="9"/>
       <c r="C235" s="17" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D235" s="11"/>
       <c r="E235" s="12"/>
@@ -7725,11 +7725,9 @@
       <c r="A236" s="8"/>
       <c r="B236" s="9"/>
       <c r="C236" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="D236" s="18">
-        <v>1.0</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="D236" s="11"/>
       <c r="E236" s="12"/>
       <c r="F236" s="13"/>
       <c r="H236" s="8"/>
@@ -7752,8 +7750,12 @@
     <row r="237">
       <c r="A237" s="8"/>
       <c r="B237" s="9"/>
-      <c r="C237" s="10"/>
-      <c r="D237" s="11"/>
+      <c r="C237" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="D237" s="18">
+        <v>1.0</v>
+      </c>
       <c r="E237" s="12"/>
       <c r="F237" s="13"/>
       <c r="H237" s="8"/>
@@ -7775,15 +7777,9 @@
     </row>
     <row r="238">
       <c r="A238" s="8"/>
-      <c r="B238" s="16" t="s">
-        <v>198</v>
-      </c>
-      <c r="C238" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="D238" s="18">
-        <v>4.0</v>
-      </c>
+      <c r="B238" s="9"/>
+      <c r="C238" s="10"/>
+      <c r="D238" s="11"/>
       <c r="E238" s="12"/>
       <c r="F238" s="13"/>
       <c r="H238" s="8"/>
@@ -7809,12 +7805,14 @@
     </row>
     <row r="239">
       <c r="A239" s="8"/>
-      <c r="B239" s="9"/>
+      <c r="B239" s="16" t="s">
+        <v>198</v>
+      </c>
       <c r="C239" s="17" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="D239" s="18">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="E239" s="12"/>
       <c r="F239" s="13"/>
@@ -7837,9 +7835,11 @@
       <c r="A240" s="8"/>
       <c r="B240" s="9"/>
       <c r="C240" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="D240" s="11"/>
+        <v>24</v>
+      </c>
+      <c r="D240" s="18">
+        <v>3.0</v>
+      </c>
       <c r="E240" s="12"/>
       <c r="F240" s="13"/>
       <c r="H240" s="8"/>
@@ -7869,7 +7869,7 @@
       <c r="A241" s="8"/>
       <c r="B241" s="9"/>
       <c r="C241" s="17" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D241" s="11"/>
       <c r="E241" s="12"/>
@@ -7895,7 +7895,7 @@
       <c r="A242" s="8"/>
       <c r="B242" s="9"/>
       <c r="C242" s="17" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D242" s="11"/>
       <c r="E242" s="12"/>
@@ -7925,7 +7925,7 @@
       <c r="A243" s="8"/>
       <c r="B243" s="9"/>
       <c r="C243" s="17" t="s">
-        <v>51</v>
+        <v>26</v>
       </c>
       <c r="D243" s="11"/>
       <c r="E243" s="12"/>
@@ -7951,11 +7951,9 @@
       <c r="A244" s="8"/>
       <c r="B244" s="9"/>
       <c r="C244" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="D244" s="18">
-        <v>2.0</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="D244" s="11"/>
       <c r="E244" s="12"/>
       <c r="F244" s="13"/>
       <c r="H244" s="8"/>
@@ -7981,9 +7979,11 @@
       <c r="A245" s="8"/>
       <c r="B245" s="9"/>
       <c r="C245" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="D245" s="18"/>
+        <v>54</v>
+      </c>
+      <c r="D245" s="18">
+        <v>2.0</v>
+      </c>
       <c r="E245" s="12"/>
       <c r="F245" s="13"/>
       <c r="H245" s="8"/>
@@ -8007,7 +8007,7 @@
       <c r="A246" s="8"/>
       <c r="B246" s="9"/>
       <c r="C246" s="17" t="s">
-        <v>31</v>
+        <v>62</v>
       </c>
       <c r="D246" s="18"/>
       <c r="E246" s="12"/>
@@ -8033,9 +8033,9 @@
       <c r="A247" s="8"/>
       <c r="B247" s="9"/>
       <c r="C247" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="D247" s="11"/>
+        <v>55</v>
+      </c>
+      <c r="D247" s="18"/>
       <c r="E247" s="12"/>
       <c r="F247" s="13"/>
       <c r="H247" s="8"/>
@@ -8059,9 +8059,9 @@
       <c r="A248" s="8"/>
       <c r="B248" s="9"/>
       <c r="C248" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="D248" s="11"/>
+        <v>31</v>
+      </c>
+      <c r="D248" s="18"/>
       <c r="E248" s="12"/>
       <c r="F248" s="13"/>
       <c r="H248" s="8"/>
@@ -8085,11 +8085,9 @@
       <c r="A249" s="8"/>
       <c r="B249" s="9"/>
       <c r="C249" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="D249" s="18">
-        <v>1.0</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="D249" s="11"/>
       <c r="E249" s="12"/>
       <c r="F249" s="13"/>
       <c r="H249" s="8"/>
@@ -8112,7 +8110,9 @@
     <row r="250">
       <c r="A250" s="8"/>
       <c r="B250" s="9"/>
-      <c r="C250" s="10"/>
+      <c r="C250" s="17" t="s">
+        <v>36</v>
+      </c>
       <c r="D250" s="11"/>
       <c r="E250" s="12"/>
       <c r="F250" s="13"/>
@@ -8139,14 +8139,12 @@
     </row>
     <row r="251">
       <c r="A251" s="8"/>
-      <c r="B251" s="16" t="s">
-        <v>209</v>
-      </c>
+      <c r="B251" s="9"/>
       <c r="C251" s="17" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D251" s="18">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
       <c r="E251" s="12"/>
       <c r="F251" s="13"/>
@@ -8161,7 +8159,7 @@
       <c r="O251" s="8"/>
       <c r="P251" s="19"/>
       <c r="Q251" s="34" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="R251" s="26"/>
       <c r="S251" s="12"/>
@@ -8170,18 +8168,14 @@
     <row r="252">
       <c r="A252" s="8"/>
       <c r="B252" s="9"/>
-      <c r="C252" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="D252" s="18">
-        <v>3.0</v>
-      </c>
+      <c r="C252" s="10"/>
+      <c r="D252" s="11"/>
       <c r="E252" s="12"/>
       <c r="F252" s="13"/>
       <c r="H252" s="8"/>
       <c r="I252" s="19"/>
       <c r="J252" s="27" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="K252" s="26"/>
       <c r="L252" s="22"/>
@@ -8197,11 +8191,15 @@
     </row>
     <row r="253">
       <c r="A253" s="8"/>
-      <c r="B253" s="9"/>
+      <c r="B253" s="16" t="s">
+        <v>211</v>
+      </c>
       <c r="C253" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="D253" s="11"/>
+        <v>39</v>
+      </c>
+      <c r="D253" s="18">
+        <v>4.0</v>
+      </c>
       <c r="E253" s="12"/>
       <c r="F253" s="13"/>
       <c r="H253" s="8"/>
@@ -8225,9 +8223,11 @@
       <c r="A254" s="8"/>
       <c r="B254" s="9"/>
       <c r="C254" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="D254" s="11"/>
+        <v>24</v>
+      </c>
+      <c r="D254" s="18">
+        <v>3.0</v>
+      </c>
       <c r="E254" s="12"/>
       <c r="F254" s="13"/>
       <c r="H254" s="8"/>
@@ -8251,7 +8251,7 @@
       <c r="A255" s="8"/>
       <c r="B255" s="9"/>
       <c r="C255" s="17" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="D255" s="11"/>
       <c r="E255" s="12"/>
@@ -8279,11 +8279,9 @@
       <c r="A256" s="8"/>
       <c r="B256" s="9"/>
       <c r="C256" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="D256" s="18">
-        <v>2.0</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="D256" s="11"/>
       <c r="E256" s="12"/>
       <c r="F256" s="13"/>
       <c r="H256" s="8"/>
@@ -8305,9 +8303,9 @@
       <c r="A257" s="8"/>
       <c r="B257" s="9"/>
       <c r="C257" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="D257" s="18"/>
+        <v>26</v>
+      </c>
+      <c r="D257" s="11"/>
       <c r="E257" s="12"/>
       <c r="F257" s="13"/>
       <c r="H257" s="8"/>
@@ -8329,9 +8327,11 @@
       <c r="A258" s="8"/>
       <c r="B258" s="9"/>
       <c r="C258" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="D258" s="18"/>
+        <v>54</v>
+      </c>
+      <c r="D258" s="18">
+        <v>2.0</v>
+      </c>
       <c r="E258" s="12"/>
       <c r="F258" s="13"/>
       <c r="H258" s="8"/>
@@ -8353,7 +8353,7 @@
       <c r="A259" s="8"/>
       <c r="B259" s="9"/>
       <c r="C259" s="17" t="s">
-        <v>31</v>
+        <v>55</v>
       </c>
       <c r="D259" s="18"/>
       <c r="E259" s="12"/>
@@ -8377,9 +8377,9 @@
       <c r="A260" s="8"/>
       <c r="B260" s="9"/>
       <c r="C260" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="D260" s="11"/>
+        <v>62</v>
+      </c>
+      <c r="D260" s="18"/>
       <c r="E260" s="12"/>
       <c r="F260" s="13"/>
       <c r="H260" s="8"/>
@@ -8401,9 +8401,9 @@
       <c r="A261" s="8"/>
       <c r="B261" s="9"/>
       <c r="C261" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="D261" s="11"/>
+        <v>31</v>
+      </c>
+      <c r="D261" s="18"/>
       <c r="E261" s="12"/>
       <c r="F261" s="13"/>
       <c r="H261" s="8"/>
@@ -8425,7 +8425,7 @@
       <c r="A262" s="8"/>
       <c r="B262" s="9"/>
       <c r="C262" s="17" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="D262" s="11"/>
       <c r="E262" s="12"/>
@@ -8451,7 +8451,7 @@
       <c r="A263" s="8"/>
       <c r="B263" s="9"/>
       <c r="C263" s="17" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="D263" s="11"/>
       <c r="E263" s="12"/>
@@ -8475,11 +8475,9 @@
       <c r="A264" s="8"/>
       <c r="B264" s="9"/>
       <c r="C264" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="D264" s="18">
-        <v>1.0</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="D264" s="11"/>
       <c r="E264" s="12"/>
       <c r="F264" s="13"/>
       <c r="H264" s="8"/>
@@ -8500,7 +8498,9 @@
     <row r="265">
       <c r="A265" s="8"/>
       <c r="B265" s="9"/>
-      <c r="C265" s="10"/>
+      <c r="C265" s="17" t="s">
+        <v>33</v>
+      </c>
       <c r="D265" s="11"/>
       <c r="E265" s="12"/>
       <c r="F265" s="13"/>
@@ -8521,14 +8521,12 @@
     </row>
     <row r="266">
       <c r="A266" s="8"/>
-      <c r="B266" s="16" t="s">
-        <v>209</v>
-      </c>
+      <c r="B266" s="9"/>
       <c r="C266" s="17" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D266" s="18">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
       <c r="E266" s="12"/>
       <c r="F266" s="13"/>
@@ -8552,12 +8550,8 @@
     <row r="267">
       <c r="A267" s="8"/>
       <c r="B267" s="9"/>
-      <c r="C267" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="D267" s="18">
-        <v>3.0</v>
-      </c>
+      <c r="C267" s="10"/>
+      <c r="D267" s="11"/>
       <c r="E267" s="12"/>
       <c r="F267" s="13"/>
       <c r="H267" s="8"/>
@@ -8575,11 +8569,15 @@
     </row>
     <row r="268">
       <c r="A268" s="8"/>
-      <c r="B268" s="9"/>
+      <c r="B268" s="16" t="s">
+        <v>211</v>
+      </c>
       <c r="C268" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="D268" s="11"/>
+        <v>39</v>
+      </c>
+      <c r="D268" s="18">
+        <v>4.0</v>
+      </c>
       <c r="E268" s="12"/>
       <c r="F268" s="13"/>
       <c r="H268" s="8"/>
@@ -8605,9 +8603,11 @@
       <c r="A269" s="8"/>
       <c r="B269" s="9"/>
       <c r="C269" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="D269" s="11"/>
+        <v>24</v>
+      </c>
+      <c r="D269" s="18">
+        <v>3.0</v>
+      </c>
       <c r="E269" s="12"/>
       <c r="F269" s="13"/>
       <c r="H269" s="8"/>
@@ -8629,7 +8629,7 @@
       <c r="A270" s="8"/>
       <c r="B270" s="9"/>
       <c r="C270" s="17" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="D270" s="11"/>
       <c r="E270" s="12"/>
@@ -8653,9 +8653,9 @@
       <c r="A271" s="8"/>
       <c r="B271" s="9"/>
       <c r="C271" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="D271" s="18"/>
+        <v>22</v>
+      </c>
+      <c r="D271" s="11"/>
       <c r="E271" s="12"/>
       <c r="F271" s="13"/>
       <c r="H271" s="8"/>
@@ -8677,11 +8677,9 @@
       <c r="A272" s="8"/>
       <c r="B272" s="9"/>
       <c r="C272" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="D272" s="18">
-        <v>2.0</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="D272" s="11"/>
       <c r="E272" s="12"/>
       <c r="F272" s="13"/>
       <c r="H272" s="8"/>
@@ -8703,7 +8701,7 @@
       <c r="A273" s="8"/>
       <c r="B273" s="9"/>
       <c r="C273" s="17" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D273" s="18"/>
       <c r="E273" s="12"/>
@@ -8729,9 +8727,11 @@
       <c r="A274" s="8"/>
       <c r="B274" s="9"/>
       <c r="C274" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="D274" s="18"/>
+        <v>54</v>
+      </c>
+      <c r="D274" s="18">
+        <v>2.0</v>
+      </c>
       <c r="E274" s="12"/>
       <c r="F274" s="13"/>
       <c r="H274" s="8"/>
@@ -8753,9 +8753,9 @@
       <c r="A275" s="8"/>
       <c r="B275" s="9"/>
       <c r="C275" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="D275" s="11"/>
+        <v>55</v>
+      </c>
+      <c r="D275" s="18"/>
       <c r="E275" s="12"/>
       <c r="F275" s="13"/>
       <c r="H275" s="8"/>
@@ -8777,9 +8777,9 @@
       <c r="A276" s="8"/>
       <c r="B276" s="9"/>
       <c r="C276" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="D276" s="11"/>
+        <v>62</v>
+      </c>
+      <c r="D276" s="18"/>
       <c r="E276" s="12"/>
       <c r="F276" s="13"/>
       <c r="H276" s="8"/>
@@ -8801,7 +8801,7 @@
       <c r="A277" s="8"/>
       <c r="B277" s="9"/>
       <c r="C277" s="17" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D277" s="11"/>
       <c r="E277" s="12"/>
@@ -8825,7 +8825,7 @@
       <c r="A278" s="8"/>
       <c r="B278" s="9"/>
       <c r="C278" s="17" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="D278" s="11"/>
       <c r="E278" s="12"/>
@@ -8851,11 +8851,9 @@
       <c r="A279" s="8"/>
       <c r="B279" s="9"/>
       <c r="C279" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="D279" s="18">
-        <v>1.0</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="D279" s="11"/>
       <c r="E279" s="12"/>
       <c r="F279" s="13"/>
       <c r="H279" s="8"/>
@@ -8876,7 +8874,9 @@
     <row r="280">
       <c r="A280" s="8"/>
       <c r="B280" s="9"/>
-      <c r="C280" s="10"/>
+      <c r="C280" s="17" t="s">
+        <v>33</v>
+      </c>
       <c r="D280" s="11"/>
       <c r="E280" s="12"/>
       <c r="F280" s="13"/>
@@ -8899,14 +8899,12 @@
     </row>
     <row r="281">
       <c r="A281" s="8"/>
-      <c r="B281" s="16" t="s">
-        <v>218</v>
-      </c>
+      <c r="B281" s="9"/>
       <c r="C281" s="17" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="D281" s="18">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
       <c r="E281" s="12"/>
       <c r="F281" s="13"/>
@@ -8926,15 +8924,13 @@
     <row r="282">
       <c r="A282" s="8"/>
       <c r="B282" s="9"/>
-      <c r="C282" s="17" t="s">
-        <v>22</v>
-      </c>
+      <c r="C282" s="10"/>
       <c r="D282" s="11"/>
       <c r="E282" s="12"/>
       <c r="F282" s="13"/>
       <c r="H282" s="8"/>
       <c r="I282" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J282" s="27" t="s">
         <v>106</v>
@@ -8953,11 +8949,15 @@
     </row>
     <row r="283">
       <c r="A283" s="8"/>
-      <c r="B283" s="9"/>
+      <c r="B283" s="16" t="s">
+        <v>219</v>
+      </c>
       <c r="C283" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="D283" s="11"/>
+        <v>13</v>
+      </c>
+      <c r="D283" s="18">
+        <v>4.0</v>
+      </c>
       <c r="E283" s="12"/>
       <c r="F283" s="13"/>
       <c r="H283" s="8"/>
@@ -8981,11 +8981,9 @@
       <c r="A284" s="8"/>
       <c r="B284" s="9"/>
       <c r="C284" s="17" t="s">
-        <v>104</v>
-      </c>
-      <c r="D284" s="18">
-        <v>3.0</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="D284" s="11"/>
       <c r="E284" s="12"/>
       <c r="F284" s="13"/>
       <c r="H284" s="8"/>
@@ -9007,15 +9005,11 @@
       <c r="A285" s="8"/>
       <c r="B285" s="9"/>
       <c r="C285" s="17" t="s">
-        <v>220</v>
-      </c>
-      <c r="D285" s="18"/>
-      <c r="E285" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="F285" s="25">
-        <v>2.0</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="D285" s="11"/>
+      <c r="E285" s="12"/>
+      <c r="F285" s="13"/>
       <c r="H285" s="8"/>
       <c r="I285" s="19"/>
       <c r="J285" s="27" t="s">
@@ -9034,14 +9028,14 @@
     <row r="286">
       <c r="A286" s="8"/>
       <c r="B286" s="9"/>
-      <c r="C286" s="17"/>
-      <c r="D286" s="18"/>
-      <c r="E286" s="24" t="s">
-        <v>221</v>
-      </c>
-      <c r="F286" s="25">
-        <v>1.0</v>
-      </c>
+      <c r="C286" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="D286" s="18">
+        <v>3.0</v>
+      </c>
+      <c r="E286" s="12"/>
+      <c r="F286" s="13"/>
       <c r="H286" s="8"/>
       <c r="I286" s="19"/>
       <c r="J286" s="27" t="s">
@@ -9061,13 +9055,15 @@
       <c r="A287" s="8"/>
       <c r="B287" s="9"/>
       <c r="C287" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="D287" s="18">
+        <v>220</v>
+      </c>
+      <c r="D287" s="18"/>
+      <c r="E287" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="F287" s="25">
         <v>2.0</v>
       </c>
-      <c r="E287" s="12"/>
-      <c r="F287" s="13"/>
       <c r="H287" s="8"/>
       <c r="I287" s="19"/>
       <c r="J287" s="27" t="s">
@@ -9086,12 +9082,14 @@
     <row r="288">
       <c r="A288" s="8"/>
       <c r="B288" s="9"/>
-      <c r="C288" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="D288" s="11"/>
-      <c r="E288" s="12"/>
-      <c r="F288" s="13"/>
+      <c r="C288" s="17"/>
+      <c r="D288" s="18"/>
+      <c r="E288" s="24" t="s">
+        <v>221</v>
+      </c>
+      <c r="F288" s="25">
+        <v>1.0</v>
+      </c>
       <c r="H288" s="8"/>
       <c r="I288" s="19"/>
       <c r="J288" s="27" t="s">
@@ -9113,9 +9111,11 @@
       <c r="A289" s="8"/>
       <c r="B289" s="9"/>
       <c r="C289" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="D289" s="11"/>
+        <v>34</v>
+      </c>
+      <c r="D289" s="18">
+        <v>2.0</v>
+      </c>
       <c r="E289" s="12"/>
       <c r="F289" s="13"/>
       <c r="H289" s="8"/>
@@ -9137,7 +9137,7 @@
       <c r="A290" s="8"/>
       <c r="B290" s="9"/>
       <c r="C290" s="17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D290" s="11"/>
       <c r="E290" s="12"/>
@@ -9161,11 +9161,9 @@
       <c r="A291" s="8"/>
       <c r="B291" s="9"/>
       <c r="C291" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="D291" s="18">
-        <v>1.0</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="D291" s="11"/>
       <c r="E291" s="12"/>
       <c r="F291" s="13"/>
       <c r="H291" s="8"/>
@@ -9186,7 +9184,9 @@
     <row r="292">
       <c r="A292" s="8"/>
       <c r="B292" s="9"/>
-      <c r="C292" s="10"/>
+      <c r="C292" s="17" t="s">
+        <v>41</v>
+      </c>
       <c r="D292" s="11"/>
       <c r="E292" s="12"/>
       <c r="F292" s="13"/>
@@ -9207,14 +9207,12 @@
     </row>
     <row r="293">
       <c r="A293" s="8"/>
-      <c r="B293" s="16" t="s">
-        <v>222</v>
-      </c>
+      <c r="B293" s="9"/>
       <c r="C293" s="17" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="D293" s="18">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
       <c r="E293" s="12"/>
       <c r="F293" s="13"/>
@@ -9236,9 +9234,7 @@
     <row r="294">
       <c r="A294" s="8"/>
       <c r="B294" s="9"/>
-      <c r="C294" s="17" t="s">
-        <v>22</v>
-      </c>
+      <c r="C294" s="10"/>
       <c r="D294" s="11"/>
       <c r="E294" s="12"/>
       <c r="F294" s="13"/>
@@ -9261,11 +9257,15 @@
     </row>
     <row r="295">
       <c r="A295" s="8"/>
-      <c r="B295" s="9"/>
+      <c r="B295" s="16" t="s">
+        <v>222</v>
+      </c>
       <c r="C295" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="D295" s="11"/>
+        <v>13</v>
+      </c>
+      <c r="D295" s="18">
+        <v>4.0</v>
+      </c>
       <c r="E295" s="12"/>
       <c r="F295" s="13"/>
       <c r="H295" s="8"/>
@@ -9285,11 +9285,9 @@
       <c r="A296" s="8"/>
       <c r="B296" s="9"/>
       <c r="C296" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="D296" s="18">
-        <v>3.0</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="D296" s="11"/>
       <c r="E296" s="12"/>
       <c r="F296" s="13"/>
       <c r="H296" s="8"/>
@@ -9315,9 +9313,9 @@
       <c r="A297" s="8"/>
       <c r="B297" s="9"/>
       <c r="C297" s="17" t="s">
-        <v>104</v>
-      </c>
-      <c r="D297" s="18"/>
+        <v>26</v>
+      </c>
+      <c r="D297" s="11"/>
       <c r="E297" s="12"/>
       <c r="F297" s="13"/>
       <c r="H297" s="8"/>
@@ -9341,15 +9339,13 @@
       <c r="A298" s="8"/>
       <c r="B298" s="9"/>
       <c r="C298" s="17" t="s">
-        <v>220</v>
-      </c>
-      <c r="D298" s="18"/>
-      <c r="E298" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="F298" s="25">
-        <v>2.0</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="D298" s="18">
+        <v>3.0</v>
+      </c>
+      <c r="E298" s="12"/>
+      <c r="F298" s="13"/>
       <c r="H298" s="8"/>
       <c r="I298" s="19"/>
       <c r="J298" s="27" t="s">
@@ -9368,14 +9364,12 @@
     <row r="299">
       <c r="A299" s="8"/>
       <c r="B299" s="9"/>
-      <c r="C299" s="17"/>
+      <c r="C299" s="17" t="s">
+        <v>104</v>
+      </c>
       <c r="D299" s="18"/>
-      <c r="E299" s="24" t="s">
-        <v>221</v>
-      </c>
-      <c r="F299" s="25">
-        <v>1.0</v>
-      </c>
+      <c r="E299" s="12"/>
+      <c r="F299" s="13"/>
       <c r="H299" s="8"/>
       <c r="I299" s="19"/>
       <c r="J299" s="27" t="s">
@@ -9395,13 +9389,15 @@
       <c r="A300" s="8"/>
       <c r="B300" s="9"/>
       <c r="C300" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="D300" s="18">
+        <v>220</v>
+      </c>
+      <c r="D300" s="18"/>
+      <c r="E300" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="F300" s="25">
         <v>2.0</v>
       </c>
-      <c r="E300" s="12"/>
-      <c r="F300" s="13"/>
       <c r="H300" s="8"/>
       <c r="I300" s="19"/>
       <c r="J300" s="27" t="s">
@@ -9420,12 +9416,14 @@
     <row r="301">
       <c r="A301" s="8"/>
       <c r="B301" s="9"/>
-      <c r="C301" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="D301" s="11"/>
-      <c r="E301" s="12"/>
-      <c r="F301" s="13"/>
+      <c r="C301" s="17"/>
+      <c r="D301" s="18"/>
+      <c r="E301" s="24" t="s">
+        <v>221</v>
+      </c>
+      <c r="F301" s="25">
+        <v>1.0</v>
+      </c>
       <c r="H301" s="8"/>
       <c r="I301" s="19"/>
       <c r="J301" s="27" t="s">
@@ -9445,9 +9443,11 @@
       <c r="A302" s="8"/>
       <c r="B302" s="9"/>
       <c r="C302" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="D302" s="11"/>
+        <v>34</v>
+      </c>
+      <c r="D302" s="18">
+        <v>2.0</v>
+      </c>
       <c r="E302" s="12"/>
       <c r="F302" s="13"/>
       <c r="H302" s="8"/>
@@ -9471,11 +9471,9 @@
       <c r="A303" s="8"/>
       <c r="B303" s="9"/>
       <c r="C303" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="D303" s="18">
-        <v>1.0</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="D303" s="11"/>
       <c r="E303" s="12"/>
       <c r="F303" s="13"/>
       <c r="H303" s="8"/>
@@ -9496,7 +9494,9 @@
     <row r="304">
       <c r="A304" s="8"/>
       <c r="B304" s="9"/>
-      <c r="C304" s="10"/>
+      <c r="C304" s="17" t="s">
+        <v>38</v>
+      </c>
       <c r="D304" s="11"/>
       <c r="E304" s="12"/>
       <c r="F304" s="13"/>
@@ -9517,21 +9517,15 @@
     </row>
     <row r="305">
       <c r="A305" s="8"/>
-      <c r="B305" s="16" t="s">
-        <v>224</v>
-      </c>
+      <c r="B305" s="9"/>
       <c r="C305" s="17" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D305" s="18">
-        <v>4.0</v>
-      </c>
-      <c r="E305" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="F305" s="25">
-        <v>3.0</v>
-      </c>
+        <v>1.0</v>
+      </c>
+      <c r="E305" s="12"/>
+      <c r="F305" s="13"/>
       <c r="H305" s="8"/>
       <c r="I305" s="19"/>
       <c r="J305" s="27" t="s">
@@ -9552,12 +9546,8 @@
       <c r="B306" s="9"/>
       <c r="C306" s="10"/>
       <c r="D306" s="11"/>
-      <c r="E306" s="24" t="s">
-        <v>48</v>
-      </c>
-      <c r="F306" s="25">
-        <v>1.0</v>
-      </c>
+      <c r="E306" s="12"/>
+      <c r="F306" s="13"/>
       <c r="H306" s="8"/>
       <c r="I306" s="19"/>
       <c r="J306" s="27" t="s">
@@ -9575,15 +9565,21 @@
     </row>
     <row r="307">
       <c r="A307" s="8"/>
-      <c r="B307" s="9"/>
+      <c r="B307" s="16" t="s">
+        <v>224</v>
+      </c>
       <c r="C307" s="17" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="D307" s="18">
+        <v>4.0</v>
+      </c>
+      <c r="E307" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="F307" s="25">
         <v>3.0</v>
       </c>
-      <c r="E307" s="12"/>
-      <c r="F307" s="13"/>
       <c r="H307" s="8"/>
       <c r="I307" s="19"/>
       <c r="J307" s="27" t="s">
@@ -9604,12 +9600,14 @@
     <row r="308">
       <c r="A308" s="8"/>
       <c r="B308" s="9"/>
-      <c r="C308" s="17" t="s">
-        <v>22</v>
-      </c>
+      <c r="C308" s="10"/>
       <c r="D308" s="11"/>
-      <c r="E308" s="12"/>
-      <c r="F308" s="13"/>
+      <c r="E308" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="F308" s="25">
+        <v>1.0</v>
+      </c>
       <c r="H308" s="8"/>
       <c r="I308" s="19"/>
       <c r="J308" s="27"/>
@@ -9627,9 +9625,11 @@
       <c r="A309" s="8"/>
       <c r="B309" s="9"/>
       <c r="C309" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="D309" s="11"/>
+        <v>18</v>
+      </c>
+      <c r="D309" s="18">
+        <v>3.0</v>
+      </c>
       <c r="E309" s="12"/>
       <c r="F309" s="13"/>
       <c r="H309" s="8"/>
@@ -9655,7 +9655,7 @@
       <c r="A310" s="8"/>
       <c r="B310" s="9"/>
       <c r="C310" s="17" t="s">
-        <v>53</v>
+        <v>22</v>
       </c>
       <c r="D310" s="11"/>
       <c r="E310" s="12"/>
@@ -9679,15 +9679,11 @@
       <c r="A311" s="8"/>
       <c r="B311" s="9"/>
       <c r="C311" s="17" t="s">
-        <v>220</v>
+        <v>26</v>
       </c>
       <c r="D311" s="11"/>
-      <c r="E311" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="F311" s="25">
-        <v>2.0</v>
-      </c>
+      <c r="E311" s="12"/>
+      <c r="F311" s="13"/>
       <c r="H311" s="8"/>
       <c r="I311" s="19"/>
       <c r="J311" s="27" t="s">
@@ -9706,14 +9702,12 @@
     <row r="312">
       <c r="A312" s="8"/>
       <c r="B312" s="9"/>
-      <c r="C312" s="10"/>
+      <c r="C312" s="17" t="s">
+        <v>53</v>
+      </c>
       <c r="D312" s="11"/>
-      <c r="E312" s="24" t="s">
-        <v>221</v>
-      </c>
-      <c r="F312" s="25">
-        <v>1.0</v>
-      </c>
+      <c r="E312" s="12"/>
+      <c r="F312" s="13"/>
       <c r="H312" s="8"/>
       <c r="I312" s="19"/>
       <c r="J312" s="27" t="s">
@@ -9733,11 +9727,15 @@
       <c r="A313" s="8"/>
       <c r="B313" s="9"/>
       <c r="C313" s="17" t="s">
-        <v>54</v>
+        <v>220</v>
       </c>
       <c r="D313" s="11"/>
-      <c r="E313" s="12"/>
-      <c r="F313" s="13"/>
+      <c r="E313" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="F313" s="25">
+        <v>2.0</v>
+      </c>
       <c r="H313" s="8"/>
       <c r="I313" s="19"/>
       <c r="J313" s="27" t="s">
@@ -9756,12 +9754,14 @@
     <row r="314">
       <c r="A314" s="8"/>
       <c r="B314" s="9"/>
-      <c r="C314" s="17" t="s">
-        <v>55</v>
-      </c>
+      <c r="C314" s="10"/>
       <c r="D314" s="11"/>
-      <c r="E314" s="12"/>
-      <c r="F314" s="13"/>
+      <c r="E314" s="24" t="s">
+        <v>221</v>
+      </c>
+      <c r="F314" s="25">
+        <v>1.0</v>
+      </c>
       <c r="H314" s="8"/>
       <c r="I314" s="19"/>
       <c r="J314" s="27" t="s">
@@ -9781,11 +9781,9 @@
       <c r="A315" s="8"/>
       <c r="B315" s="9"/>
       <c r="C315" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="D315" s="18">
-        <v>2.0</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="D315" s="11"/>
       <c r="E315" s="12"/>
       <c r="F315" s="13"/>
       <c r="H315" s="8"/>
@@ -9807,11 +9805,9 @@
       <c r="A316" s="8"/>
       <c r="B316" s="9"/>
       <c r="C316" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="D316" s="18">
-        <v>1.0</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="D316" s="11"/>
       <c r="E316" s="12"/>
       <c r="F316" s="13"/>
       <c r="H316" s="8"/>
@@ -9832,8 +9828,12 @@
     <row r="317">
       <c r="A317" s="8"/>
       <c r="B317" s="9"/>
-      <c r="C317" s="10"/>
-      <c r="D317" s="11"/>
+      <c r="C317" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="D317" s="18">
+        <v>2.0</v>
+      </c>
       <c r="E317" s="12"/>
       <c r="F317" s="13"/>
       <c r="H317" s="8"/>
@@ -9855,21 +9855,15 @@
     </row>
     <row r="318">
       <c r="A318" s="8"/>
-      <c r="B318" s="16" t="s">
-        <v>226</v>
-      </c>
+      <c r="B318" s="9"/>
       <c r="C318" s="17" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D318" s="18">
-        <v>4.0</v>
-      </c>
-      <c r="E318" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="F318" s="25">
-        <v>3.0</v>
-      </c>
+        <v>1.0</v>
+      </c>
+      <c r="E318" s="12"/>
+      <c r="F318" s="13"/>
       <c r="H318" s="8"/>
       <c r="I318" s="33"/>
       <c r="J318" s="27" t="s">
@@ -9890,12 +9884,8 @@
       <c r="B319" s="9"/>
       <c r="C319" s="10"/>
       <c r="D319" s="11"/>
-      <c r="E319" s="24" t="s">
-        <v>48</v>
-      </c>
-      <c r="F319" s="25">
-        <v>1.0</v>
-      </c>
+      <c r="E319" s="12"/>
+      <c r="F319" s="13"/>
       <c r="H319" s="8"/>
       <c r="I319" s="19"/>
       <c r="J319" s="27" t="s">
@@ -9913,15 +9903,21 @@
     </row>
     <row r="320">
       <c r="A320" s="8"/>
-      <c r="B320" s="9"/>
+      <c r="B320" s="16" t="s">
+        <v>226</v>
+      </c>
       <c r="C320" s="17" t="s">
-        <v>68</v>
+        <v>46</v>
       </c>
       <c r="D320" s="18">
+        <v>4.0</v>
+      </c>
+      <c r="E320" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="F320" s="25">
         <v>3.0</v>
       </c>
-      <c r="E320" s="12"/>
-      <c r="F320" s="13"/>
       <c r="H320" s="8"/>
       <c r="I320" s="19"/>
       <c r="J320" s="27" t="s">
@@ -9942,12 +9938,14 @@
     <row r="321">
       <c r="A321" s="8"/>
       <c r="B321" s="9"/>
-      <c r="C321" s="17" t="s">
-        <v>22</v>
-      </c>
+      <c r="C321" s="10"/>
       <c r="D321" s="11"/>
-      <c r="E321" s="12"/>
-      <c r="F321" s="13"/>
+      <c r="E321" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="F321" s="25">
+        <v>1.0</v>
+      </c>
       <c r="H321" s="8"/>
       <c r="I321" s="19"/>
       <c r="J321" s="27" t="s">
@@ -9967,9 +9965,11 @@
       <c r="A322" s="8"/>
       <c r="B322" s="9"/>
       <c r="C322" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="D322" s="11"/>
+        <v>68</v>
+      </c>
+      <c r="D322" s="18">
+        <v>3.0</v>
+      </c>
       <c r="E322" s="12"/>
       <c r="F322" s="13"/>
       <c r="H322" s="8"/>
@@ -9989,7 +9989,7 @@
       <c r="A323" s="8"/>
       <c r="B323" s="9"/>
       <c r="C323" s="17" t="s">
-        <v>51</v>
+        <v>22</v>
       </c>
       <c r="D323" s="11"/>
       <c r="E323" s="12"/>
@@ -10017,7 +10017,7 @@
       <c r="A324" s="8"/>
       <c r="B324" s="9"/>
       <c r="C324" s="17" t="s">
-        <v>53</v>
+        <v>26</v>
       </c>
       <c r="D324" s="11"/>
       <c r="E324" s="12"/>
@@ -10041,15 +10041,11 @@
       <c r="A325" s="8"/>
       <c r="B325" s="9"/>
       <c r="C325" s="17" t="s">
-        <v>220</v>
+        <v>51</v>
       </c>
       <c r="D325" s="11"/>
-      <c r="E325" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="F325" s="25">
-        <v>2.0</v>
-      </c>
+      <c r="E325" s="12"/>
+      <c r="F325" s="13"/>
       <c r="H325" s="8"/>
       <c r="I325" s="19"/>
       <c r="J325" s="27" t="s">
@@ -10068,14 +10064,12 @@
     <row r="326">
       <c r="A326" s="8"/>
       <c r="B326" s="9"/>
-      <c r="C326" s="10"/>
+      <c r="C326" s="17" t="s">
+        <v>53</v>
+      </c>
       <c r="D326" s="11"/>
-      <c r="E326" s="24" t="s">
-        <v>221</v>
-      </c>
-      <c r="F326" s="25">
-        <v>1.0</v>
-      </c>
+      <c r="E326" s="12"/>
+      <c r="F326" s="13"/>
       <c r="H326" s="8"/>
       <c r="I326" s="19"/>
       <c r="J326" s="27" t="s">
@@ -10097,11 +10091,15 @@
       <c r="A327" s="8"/>
       <c r="B327" s="9"/>
       <c r="C327" s="17" t="s">
-        <v>54</v>
+        <v>220</v>
       </c>
       <c r="D327" s="11"/>
-      <c r="E327" s="12"/>
-      <c r="F327" s="13"/>
+      <c r="E327" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="F327" s="25">
+        <v>2.0</v>
+      </c>
       <c r="H327" s="8"/>
       <c r="I327" s="19"/>
       <c r="J327" s="27" t="s">
@@ -10120,12 +10118,14 @@
     <row r="328">
       <c r="A328" s="8"/>
       <c r="B328" s="9"/>
-      <c r="C328" s="17" t="s">
-        <v>55</v>
-      </c>
+      <c r="C328" s="10"/>
       <c r="D328" s="11"/>
-      <c r="E328" s="12"/>
-      <c r="F328" s="13"/>
+      <c r="E328" s="24" t="s">
+        <v>221</v>
+      </c>
+      <c r="F328" s="25">
+        <v>1.0</v>
+      </c>
       <c r="H328" s="8"/>
       <c r="I328" s="19"/>
       <c r="J328" s="27" t="s">
@@ -10145,11 +10145,9 @@
       <c r="A329" s="8"/>
       <c r="B329" s="9"/>
       <c r="C329" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="D329" s="18">
-        <v>2.0</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="D329" s="11"/>
       <c r="E329" s="12"/>
       <c r="F329" s="13"/>
       <c r="H329" s="8"/>
@@ -10171,11 +10169,9 @@
       <c r="A330" s="8"/>
       <c r="B330" s="9"/>
       <c r="C330" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="D330" s="18">
-        <v>1.0</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="D330" s="11"/>
       <c r="E330" s="12"/>
       <c r="F330" s="13"/>
       <c r="H330" s="8"/>
@@ -10196,8 +10192,12 @@
     <row r="331">
       <c r="A331" s="8"/>
       <c r="B331" s="9"/>
-      <c r="C331" s="10"/>
-      <c r="D331" s="11"/>
+      <c r="C331" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="D331" s="18">
+        <v>2.0</v>
+      </c>
       <c r="E331" s="12"/>
       <c r="F331" s="13"/>
       <c r="H331" s="8"/>
@@ -10217,14 +10217,12 @@
     </row>
     <row r="332">
       <c r="A332" s="8"/>
-      <c r="B332" s="16" t="s">
-        <v>232</v>
-      </c>
+      <c r="B332" s="9"/>
       <c r="C332" s="17" t="s">
-        <v>62</v>
+        <v>42</v>
       </c>
       <c r="D332" s="18">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
       <c r="E332" s="12"/>
       <c r="F332" s="13"/>
@@ -10248,12 +10246,8 @@
     <row r="333">
       <c r="A333" s="8"/>
       <c r="B333" s="9"/>
-      <c r="C333" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="D333" s="18">
-        <v>3.0</v>
-      </c>
+      <c r="C333" s="10"/>
+      <c r="D333" s="11"/>
       <c r="E333" s="12"/>
       <c r="F333" s="13"/>
       <c r="H333" s="8"/>
@@ -10273,11 +10267,15 @@
     </row>
     <row r="334">
       <c r="A334" s="8"/>
-      <c r="B334" s="9"/>
+      <c r="B334" s="16" t="s">
+        <v>232</v>
+      </c>
       <c r="C334" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="D334" s="11"/>
+        <v>62</v>
+      </c>
+      <c r="D334" s="18">
+        <v>4.0</v>
+      </c>
       <c r="E334" s="12"/>
       <c r="F334" s="13"/>
       <c r="H334" s="8"/>
@@ -10299,9 +10297,11 @@
       <c r="A335" s="8"/>
       <c r="B335" s="9"/>
       <c r="C335" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="D335" s="11"/>
+        <v>68</v>
+      </c>
+      <c r="D335" s="18">
+        <v>3.0</v>
+      </c>
       <c r="E335" s="12"/>
       <c r="F335" s="13"/>
       <c r="H335" s="8"/>
@@ -10325,7 +10325,7 @@
       <c r="A336" s="8"/>
       <c r="B336" s="9"/>
       <c r="C336" s="17" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D336" s="11"/>
       <c r="E336" s="12"/>
@@ -10347,15 +10347,11 @@
       <c r="A337" s="8"/>
       <c r="B337" s="9"/>
       <c r="C337" s="17" t="s">
-        <v>220</v>
+        <v>26</v>
       </c>
       <c r="D337" s="11"/>
-      <c r="E337" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="F337" s="25">
-        <v>2.0</v>
-      </c>
+      <c r="E337" s="12"/>
+      <c r="F337" s="13"/>
       <c r="H337" s="8"/>
       <c r="I337" s="19" t="s">
         <v>233</v>
@@ -10378,14 +10374,12 @@
     <row r="338">
       <c r="A338" s="8"/>
       <c r="B338" s="9"/>
-      <c r="C338" s="10"/>
+      <c r="C338" s="17" t="s">
+        <v>24</v>
+      </c>
       <c r="D338" s="11"/>
-      <c r="E338" s="24" t="s">
-        <v>221</v>
-      </c>
-      <c r="F338" s="25">
-        <v>1.0</v>
-      </c>
+      <c r="E338" s="12"/>
+      <c r="F338" s="13"/>
       <c r="H338" s="8"/>
       <c r="I338" s="19"/>
       <c r="J338" s="27" t="s">
@@ -10405,11 +10399,15 @@
       <c r="A339" s="8"/>
       <c r="B339" s="9"/>
       <c r="C339" s="17" t="s">
-        <v>54</v>
+        <v>220</v>
       </c>
       <c r="D339" s="11"/>
-      <c r="E339" s="12"/>
-      <c r="F339" s="13"/>
+      <c r="E339" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="F339" s="25">
+        <v>2.0</v>
+      </c>
       <c r="H339" s="8"/>
       <c r="I339" s="19"/>
       <c r="J339" s="27" t="s">
@@ -10428,12 +10426,14 @@
     <row r="340">
       <c r="A340" s="8"/>
       <c r="B340" s="9"/>
-      <c r="C340" s="17" t="s">
-        <v>55</v>
-      </c>
+      <c r="C340" s="10"/>
       <c r="D340" s="11"/>
-      <c r="E340" s="12"/>
-      <c r="F340" s="13"/>
+      <c r="E340" s="24" t="s">
+        <v>221</v>
+      </c>
+      <c r="F340" s="25">
+        <v>1.0</v>
+      </c>
       <c r="H340" s="8"/>
       <c r="I340" s="19"/>
       <c r="J340" s="27" t="s">
@@ -10455,11 +10455,9 @@
       <c r="A341" s="8"/>
       <c r="B341" s="9"/>
       <c r="C341" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="D341" s="18">
-        <v>2.0</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="D341" s="11"/>
       <c r="E341" s="12"/>
       <c r="F341" s="13"/>
       <c r="H341" s="8"/>
@@ -10481,11 +10479,9 @@
       <c r="A342" s="8"/>
       <c r="B342" s="9"/>
       <c r="C342" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="D342" s="18">
-        <v>1.0</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="D342" s="11"/>
       <c r="E342" s="12"/>
       <c r="F342" s="13"/>
       <c r="H342" s="8"/>
@@ -10506,8 +10502,12 @@
     <row r="343">
       <c r="A343" s="8"/>
       <c r="B343" s="9"/>
-      <c r="C343" s="10"/>
-      <c r="D343" s="11"/>
+      <c r="C343" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="D343" s="18">
+        <v>2.0</v>
+      </c>
       <c r="E343" s="12"/>
       <c r="F343" s="13"/>
       <c r="H343" s="8"/>
@@ -10527,14 +10527,12 @@
     </row>
     <row r="344">
       <c r="A344" s="8"/>
-      <c r="B344" s="16" t="s">
-        <v>234</v>
-      </c>
+      <c r="B344" s="9"/>
       <c r="C344" s="17" t="s">
-        <v>62</v>
+        <v>42</v>
       </c>
       <c r="D344" s="18">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
       <c r="E344" s="12"/>
       <c r="F344" s="13"/>
@@ -10556,12 +10554,8 @@
     <row r="345">
       <c r="A345" s="8"/>
       <c r="B345" s="9"/>
-      <c r="C345" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="D345" s="18">
-        <v>3.0</v>
-      </c>
+      <c r="C345" s="10"/>
+      <c r="D345" s="11"/>
       <c r="E345" s="12"/>
       <c r="F345" s="13"/>
       <c r="H345" s="8"/>
@@ -10581,11 +10575,15 @@
     </row>
     <row r="346">
       <c r="A346" s="8"/>
-      <c r="B346" s="9"/>
+      <c r="B346" s="16" t="s">
+        <v>234</v>
+      </c>
       <c r="C346" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="D346" s="11"/>
+        <v>62</v>
+      </c>
+      <c r="D346" s="18">
+        <v>4.0</v>
+      </c>
       <c r="E346" s="12"/>
       <c r="F346" s="13"/>
       <c r="H346" s="8"/>
@@ -10609,9 +10607,11 @@
       <c r="A347" s="8"/>
       <c r="B347" s="9"/>
       <c r="C347" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="D347" s="11"/>
+        <v>68</v>
+      </c>
+      <c r="D347" s="18">
+        <v>3.0</v>
+      </c>
       <c r="E347" s="12"/>
       <c r="F347" s="13"/>
       <c r="H347" s="8"/>
@@ -10633,7 +10633,7 @@
       <c r="A348" s="8"/>
       <c r="B348" s="9"/>
       <c r="C348" s="17" t="s">
-        <v>51</v>
+        <v>22</v>
       </c>
       <c r="D348" s="11"/>
       <c r="E348" s="12"/>
@@ -10657,7 +10657,7 @@
       <c r="A349" s="8"/>
       <c r="B349" s="9"/>
       <c r="C349" s="17" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D349" s="11"/>
       <c r="E349" s="12"/>
@@ -10683,15 +10683,11 @@
       <c r="A350" s="8"/>
       <c r="B350" s="9"/>
       <c r="C350" s="17" t="s">
-        <v>220</v>
+        <v>51</v>
       </c>
       <c r="D350" s="11"/>
-      <c r="E350" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="F350" s="25">
-        <v>2.0</v>
-      </c>
+      <c r="E350" s="12"/>
+      <c r="F350" s="13"/>
       <c r="H350" s="8"/>
       <c r="I350" s="19"/>
       <c r="J350" s="27"/>
@@ -10708,14 +10704,12 @@
     <row r="351">
       <c r="A351" s="8"/>
       <c r="B351" s="9"/>
-      <c r="C351" s="10"/>
+      <c r="C351" s="17" t="s">
+        <v>24</v>
+      </c>
       <c r="D351" s="11"/>
-      <c r="E351" s="24" t="s">
-        <v>221</v>
-      </c>
-      <c r="F351" s="25">
-        <v>1.0</v>
-      </c>
+      <c r="E351" s="12"/>
+      <c r="F351" s="13"/>
       <c r="H351" s="8"/>
       <c r="I351" s="19" t="s">
         <v>235</v>
@@ -10739,11 +10733,15 @@
       <c r="A352" s="8"/>
       <c r="B352" s="9"/>
       <c r="C352" s="17" t="s">
-        <v>54</v>
+        <v>220</v>
       </c>
       <c r="D352" s="11"/>
-      <c r="E352" s="12"/>
-      <c r="F352" s="13"/>
+      <c r="E352" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="F352" s="25">
+        <v>2.0</v>
+      </c>
       <c r="H352" s="8"/>
       <c r="I352" s="19"/>
       <c r="J352" s="27" t="s">
@@ -10762,12 +10760,14 @@
     <row r="353">
       <c r="A353" s="8"/>
       <c r="B353" s="9"/>
-      <c r="C353" s="17" t="s">
-        <v>55</v>
-      </c>
+      <c r="C353" s="10"/>
       <c r="D353" s="11"/>
-      <c r="E353" s="12"/>
-      <c r="F353" s="13"/>
+      <c r="E353" s="24" t="s">
+        <v>221</v>
+      </c>
+      <c r="F353" s="25">
+        <v>1.0</v>
+      </c>
       <c r="H353" s="8"/>
       <c r="I353" s="19"/>
       <c r="J353" s="27" t="s">
@@ -10787,11 +10787,9 @@
       <c r="A354" s="8"/>
       <c r="B354" s="9"/>
       <c r="C354" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="D354" s="18">
-        <v>2.0</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="D354" s="11"/>
       <c r="E354" s="12"/>
       <c r="F354" s="13"/>
       <c r="H354" s="8"/>
@@ -10815,11 +10813,9 @@
       <c r="A355" s="8"/>
       <c r="B355" s="9"/>
       <c r="C355" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="D355" s="18">
-        <v>1.0</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="D355" s="11"/>
       <c r="E355" s="12"/>
       <c r="F355" s="13"/>
       <c r="H355" s="8"/>
@@ -10840,8 +10836,12 @@
     <row r="356">
       <c r="A356" s="8"/>
       <c r="B356" s="9"/>
-      <c r="C356" s="10"/>
-      <c r="D356" s="11"/>
+      <c r="C356" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="D356" s="18">
+        <v>2.0</v>
+      </c>
       <c r="E356" s="12"/>
       <c r="F356" s="13"/>
       <c r="H356" s="8"/>
@@ -10861,14 +10861,12 @@
     </row>
     <row r="357">
       <c r="A357" s="8"/>
-      <c r="B357" s="16" t="s">
-        <v>236</v>
-      </c>
+      <c r="B357" s="9"/>
       <c r="C357" s="17" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D357" s="18">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
       <c r="E357" s="12"/>
       <c r="F357" s="13"/>
@@ -10890,12 +10888,8 @@
     <row r="358">
       <c r="A358" s="8"/>
       <c r="B358" s="9"/>
-      <c r="C358" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="D358" s="18">
-        <v>3.0</v>
-      </c>
+      <c r="C358" s="10"/>
+      <c r="D358" s="11"/>
       <c r="E358" s="12"/>
       <c r="F358" s="13"/>
       <c r="H358" s="8"/>
@@ -10915,11 +10909,15 @@
     </row>
     <row r="359">
       <c r="A359" s="8"/>
-      <c r="B359" s="9"/>
+      <c r="B359" s="16" t="s">
+        <v>236</v>
+      </c>
       <c r="C359" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="D359" s="11"/>
+        <v>39</v>
+      </c>
+      <c r="D359" s="18">
+        <v>4.0</v>
+      </c>
       <c r="E359" s="12"/>
       <c r="F359" s="13"/>
       <c r="H359" s="8"/>
@@ -10943,9 +10941,11 @@
       <c r="A360" s="8"/>
       <c r="B360" s="9"/>
       <c r="C360" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="D360" s="11"/>
+        <v>68</v>
+      </c>
+      <c r="D360" s="18">
+        <v>3.0</v>
+      </c>
       <c r="E360" s="12"/>
       <c r="F360" s="13"/>
       <c r="H360" s="8"/>
@@ -10967,7 +10967,7 @@
       <c r="A361" s="8"/>
       <c r="B361" s="9"/>
       <c r="C361" s="17" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D361" s="11"/>
       <c r="E361" s="12"/>
@@ -10991,15 +10991,11 @@
       <c r="A362" s="8"/>
       <c r="B362" s="9"/>
       <c r="C362" s="17" t="s">
-        <v>220</v>
+        <v>26</v>
       </c>
       <c r="D362" s="11"/>
-      <c r="E362" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="F362" s="25">
-        <v>2.0</v>
-      </c>
+      <c r="E362" s="12"/>
+      <c r="F362" s="13"/>
       <c r="H362" s="8"/>
       <c r="I362" s="19"/>
       <c r="J362" s="27" t="s">
@@ -11020,14 +11016,12 @@
     <row r="363">
       <c r="A363" s="8"/>
       <c r="B363" s="9"/>
-      <c r="C363" s="10"/>
+      <c r="C363" s="17" t="s">
+        <v>24</v>
+      </c>
       <c r="D363" s="11"/>
-      <c r="E363" s="24" t="s">
-        <v>221</v>
-      </c>
-      <c r="F363" s="25">
-        <v>1.0</v>
-      </c>
+      <c r="E363" s="12"/>
+      <c r="F363" s="13"/>
       <c r="H363" s="8"/>
       <c r="I363" s="19"/>
       <c r="J363" s="27"/>
@@ -11045,11 +11039,15 @@
       <c r="A364" s="8"/>
       <c r="B364" s="9"/>
       <c r="C364" s="17" t="s">
-        <v>67</v>
+        <v>220</v>
       </c>
       <c r="D364" s="11"/>
-      <c r="E364" s="12"/>
-      <c r="F364" s="13"/>
+      <c r="E364" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="F364" s="25">
+        <v>2.0</v>
+      </c>
       <c r="H364" s="8"/>
       <c r="I364" s="19" t="s">
         <v>237</v>
@@ -11072,14 +11070,14 @@
     <row r="365">
       <c r="A365" s="8"/>
       <c r="B365" s="9"/>
-      <c r="C365" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="D365" s="18">
-        <v>2.0</v>
-      </c>
-      <c r="E365" s="12"/>
-      <c r="F365" s="13"/>
+      <c r="C365" s="10"/>
+      <c r="D365" s="11"/>
+      <c r="E365" s="24" t="s">
+        <v>221</v>
+      </c>
+      <c r="F365" s="25">
+        <v>1.0</v>
+      </c>
       <c r="H365" s="8"/>
       <c r="I365" s="19"/>
       <c r="J365" s="27" t="s">
@@ -11099,9 +11097,9 @@
       <c r="A366" s="8"/>
       <c r="B366" s="9"/>
       <c r="C366" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="D366" s="18"/>
+        <v>67</v>
+      </c>
+      <c r="D366" s="11"/>
       <c r="E366" s="12"/>
       <c r="F366" s="13"/>
       <c r="H366" s="8"/>
@@ -11123,9 +11121,11 @@
       <c r="A367" s="8"/>
       <c r="B367" s="9"/>
       <c r="C367" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="D367" s="18"/>
+        <v>41</v>
+      </c>
+      <c r="D367" s="18">
+        <v>2.0</v>
+      </c>
       <c r="E367" s="12"/>
       <c r="F367" s="13"/>
       <c r="H367" s="8"/>
@@ -11149,11 +11149,9 @@
       <c r="A368" s="8"/>
       <c r="B368" s="9"/>
       <c r="C368" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="D368" s="18">
-        <v>1.0</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="D368" s="18"/>
       <c r="E368" s="12"/>
       <c r="F368" s="13"/>
       <c r="H368" s="8"/>
@@ -11174,8 +11172,10 @@
     <row r="369">
       <c r="A369" s="8"/>
       <c r="B369" s="9"/>
-      <c r="C369" s="10"/>
-      <c r="D369" s="11"/>
+      <c r="C369" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D369" s="18"/>
       <c r="E369" s="12"/>
       <c r="F369" s="13"/>
       <c r="H369" s="8"/>
@@ -11195,14 +11195,12 @@
     </row>
     <row r="370">
       <c r="A370" s="8"/>
-      <c r="B370" s="16" t="s">
-        <v>238</v>
-      </c>
+      <c r="B370" s="9"/>
       <c r="C370" s="17" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D370" s="18">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
       <c r="E370" s="12"/>
       <c r="F370" s="13"/>
@@ -11224,12 +11222,8 @@
     <row r="371">
       <c r="A371" s="8"/>
       <c r="B371" s="9"/>
-      <c r="C371" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="D371" s="18">
-        <v>3.0</v>
-      </c>
+      <c r="C371" s="10"/>
+      <c r="D371" s="11"/>
       <c r="E371" s="12"/>
       <c r="F371" s="13"/>
       <c r="H371" s="8"/>
@@ -11249,11 +11243,15 @@
     </row>
     <row r="372">
       <c r="A372" s="8"/>
-      <c r="B372" s="9"/>
+      <c r="B372" s="16" t="s">
+        <v>238</v>
+      </c>
       <c r="C372" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="D372" s="11"/>
+        <v>39</v>
+      </c>
+      <c r="D372" s="18">
+        <v>4.0</v>
+      </c>
       <c r="E372" s="12"/>
       <c r="F372" s="13"/>
       <c r="H372" s="8"/>
@@ -11277,9 +11275,11 @@
       <c r="A373" s="8"/>
       <c r="B373" s="9"/>
       <c r="C373" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="D373" s="11"/>
+        <v>68</v>
+      </c>
+      <c r="D373" s="18">
+        <v>3.0</v>
+      </c>
       <c r="E373" s="12"/>
       <c r="F373" s="13"/>
       <c r="H373" s="8"/>
@@ -11301,7 +11301,7 @@
       <c r="A374" s="8"/>
       <c r="B374" s="9"/>
       <c r="C374" s="17" t="s">
-        <v>51</v>
+        <v>22</v>
       </c>
       <c r="D374" s="11"/>
       <c r="E374" s="12"/>
@@ -11325,7 +11325,7 @@
       <c r="A375" s="8"/>
       <c r="B375" s="9"/>
       <c r="C375" s="17" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D375" s="11"/>
       <c r="E375" s="12"/>
@@ -11351,15 +11351,11 @@
       <c r="A376" s="8"/>
       <c r="B376" s="9"/>
       <c r="C376" s="17" t="s">
-        <v>220</v>
+        <v>51</v>
       </c>
       <c r="D376" s="11"/>
-      <c r="E376" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="F376" s="25">
-        <v>2.0</v>
-      </c>
+      <c r="E376" s="12"/>
+      <c r="F376" s="13"/>
       <c r="H376" s="8"/>
       <c r="I376" s="19"/>
       <c r="J376" s="27"/>
@@ -11376,14 +11372,12 @@
     <row r="377">
       <c r="A377" s="8"/>
       <c r="B377" s="9"/>
-      <c r="C377" s="10"/>
+      <c r="C377" s="17" t="s">
+        <v>24</v>
+      </c>
       <c r="D377" s="11"/>
-      <c r="E377" s="24" t="s">
-        <v>221</v>
-      </c>
-      <c r="F377" s="25">
-        <v>1.0</v>
-      </c>
+      <c r="E377" s="12"/>
+      <c r="F377" s="13"/>
       <c r="H377" s="8"/>
       <c r="I377" s="19" t="s">
         <v>239</v>
@@ -11407,11 +11401,15 @@
       <c r="A378" s="8"/>
       <c r="B378" s="9"/>
       <c r="C378" s="17" t="s">
-        <v>67</v>
+        <v>220</v>
       </c>
       <c r="D378" s="11"/>
-      <c r="E378" s="12"/>
-      <c r="F378" s="13"/>
+      <c r="E378" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="F378" s="25">
+        <v>2.0</v>
+      </c>
       <c r="H378" s="8"/>
       <c r="I378" s="19"/>
       <c r="J378" s="27" t="s">
@@ -11430,14 +11428,14 @@
     <row r="379">
       <c r="A379" s="8"/>
       <c r="B379" s="9"/>
-      <c r="C379" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="D379" s="18">
-        <v>2.0</v>
-      </c>
-      <c r="E379" s="12"/>
-      <c r="F379" s="13"/>
+      <c r="C379" s="10"/>
+      <c r="D379" s="11"/>
+      <c r="E379" s="24" t="s">
+        <v>221</v>
+      </c>
+      <c r="F379" s="25">
+        <v>1.0</v>
+      </c>
       <c r="H379" s="8"/>
       <c r="I379" s="19"/>
       <c r="J379" s="27" t="s">
@@ -11457,11 +11455,9 @@
       <c r="A380" s="8"/>
       <c r="B380" s="9"/>
       <c r="C380" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="D380" s="18">
-        <v>1.0</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="D380" s="11"/>
       <c r="E380" s="12"/>
       <c r="F380" s="13"/>
       <c r="H380" s="8"/>
@@ -11484,8 +11480,12 @@
     <row r="381">
       <c r="A381" s="8"/>
       <c r="B381" s="9"/>
-      <c r="C381" s="10"/>
-      <c r="D381" s="11"/>
+      <c r="C381" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="D381" s="18">
+        <v>2.0</v>
+      </c>
       <c r="E381" s="12"/>
       <c r="F381" s="13"/>
       <c r="H381" s="8"/>
@@ -11505,21 +11505,15 @@
     </row>
     <row r="382">
       <c r="A382" s="8"/>
-      <c r="B382" s="16" t="s">
-        <v>240</v>
-      </c>
+      <c r="B382" s="9"/>
       <c r="C382" s="17" t="s">
-        <v>241</v>
+        <v>42</v>
       </c>
       <c r="D382" s="18">
-        <v>4.0</v>
-      </c>
-      <c r="E382" s="24" t="s">
-        <v>84</v>
-      </c>
-      <c r="F382" s="25">
-        <v>2.0</v>
-      </c>
+        <v>1.0</v>
+      </c>
+      <c r="E382" s="12"/>
+      <c r="F382" s="13"/>
       <c r="H382" s="8"/>
       <c r="I382" s="19"/>
       <c r="J382" s="27" t="s">
@@ -11540,12 +11534,8 @@
       <c r="B383" s="9"/>
       <c r="C383" s="10"/>
       <c r="D383" s="11"/>
-      <c r="E383" s="24" t="s">
-        <v>177</v>
-      </c>
-      <c r="F383" s="25">
-        <v>2.0</v>
-      </c>
+      <c r="E383" s="12"/>
+      <c r="F383" s="13"/>
       <c r="H383" s="8"/>
       <c r="I383" s="19"/>
       <c r="J383" s="27" t="s">
@@ -11563,18 +11553,20 @@
     </row>
     <row r="384">
       <c r="A384" s="8"/>
-      <c r="B384" s="9"/>
+      <c r="B384" s="16" t="s">
+        <v>240</v>
+      </c>
       <c r="C384" s="17" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D384" s="18">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="E384" s="24" t="s">
-        <v>243</v>
+        <v>84</v>
       </c>
       <c r="F384" s="25">
-        <v>1.5</v>
+        <v>2.0</v>
       </c>
       <c r="H384" s="8"/>
       <c r="I384" s="19"/>
@@ -11597,10 +11589,10 @@
       <c r="C385" s="10"/>
       <c r="D385" s="11"/>
       <c r="E385" s="24" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F385" s="25">
-        <v>1.5</v>
+        <v>2.0</v>
       </c>
       <c r="H385" s="8"/>
       <c r="I385" s="19"/>
@@ -11621,11 +11613,17 @@
       <c r="A386" s="8"/>
       <c r="B386" s="9"/>
       <c r="C386" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="D386" s="11"/>
-      <c r="E386" s="12"/>
-      <c r="F386" s="13"/>
+        <v>242</v>
+      </c>
+      <c r="D386" s="18">
+        <v>3.0</v>
+      </c>
+      <c r="E386" s="24" t="s">
+        <v>243</v>
+      </c>
+      <c r="F386" s="25">
+        <v>1.5</v>
+      </c>
       <c r="H386" s="8"/>
       <c r="I386" s="33"/>
       <c r="J386" s="27" t="s">
@@ -11644,12 +11642,14 @@
     <row r="387">
       <c r="A387" s="8"/>
       <c r="B387" s="9"/>
-      <c r="C387" s="17" t="s">
-        <v>22</v>
-      </c>
+      <c r="C387" s="10"/>
       <c r="D387" s="11"/>
-      <c r="E387" s="12"/>
-      <c r="F387" s="13"/>
+      <c r="E387" s="24" t="s">
+        <v>178</v>
+      </c>
+      <c r="F387" s="25">
+        <v>1.5</v>
+      </c>
       <c r="H387" s="8"/>
       <c r="I387" s="19"/>
       <c r="J387" s="27" t="s">
@@ -11671,7 +11671,7 @@
       <c r="A388" s="8"/>
       <c r="B388" s="9"/>
       <c r="C388" s="17" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="D388" s="11"/>
       <c r="E388" s="12"/>
@@ -11697,15 +11697,11 @@
       <c r="A389" s="8"/>
       <c r="B389" s="9"/>
       <c r="C389" s="17" t="s">
-        <v>220</v>
+        <v>22</v>
       </c>
       <c r="D389" s="11"/>
-      <c r="E389" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="F389" s="25">
-        <v>2.0</v>
-      </c>
+      <c r="E389" s="12"/>
+      <c r="F389" s="13"/>
       <c r="H389" s="8"/>
       <c r="I389" s="19"/>
       <c r="J389" s="27"/>
@@ -11722,14 +11718,12 @@
     <row r="390">
       <c r="A390" s="8"/>
       <c r="B390" s="9"/>
-      <c r="C390" s="10"/>
+      <c r="C390" s="17" t="s">
+        <v>26</v>
+      </c>
       <c r="D390" s="11"/>
-      <c r="E390" s="24" t="s">
-        <v>221</v>
-      </c>
-      <c r="F390" s="25">
-        <v>1.0</v>
-      </c>
+      <c r="E390" s="12"/>
+      <c r="F390" s="13"/>
       <c r="H390" s="8"/>
       <c r="I390" s="19" t="s">
         <v>244</v>
@@ -11753,13 +11747,15 @@
       <c r="A391" s="8"/>
       <c r="B391" s="9"/>
       <c r="C391" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="D391" s="18">
+        <v>220</v>
+      </c>
+      <c r="D391" s="11"/>
+      <c r="E391" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="F391" s="25">
         <v>2.0</v>
       </c>
-      <c r="E391" s="12"/>
-      <c r="F391" s="13"/>
       <c r="H391" s="8"/>
       <c r="I391" s="19"/>
       <c r="J391" s="27" t="s">
@@ -11778,12 +11774,14 @@
     <row r="392">
       <c r="A392" s="8"/>
       <c r="B392" s="9"/>
-      <c r="C392" s="17" t="s">
-        <v>39</v>
-      </c>
+      <c r="C392" s="10"/>
       <c r="D392" s="11"/>
-      <c r="E392" s="12"/>
-      <c r="F392" s="13"/>
+      <c r="E392" s="24" t="s">
+        <v>221</v>
+      </c>
+      <c r="F392" s="25">
+        <v>1.0</v>
+      </c>
       <c r="H392" s="8"/>
       <c r="I392" s="19"/>
       <c r="J392" s="27" t="s">
@@ -11803,9 +11801,11 @@
       <c r="A393" s="8"/>
       <c r="B393" s="9"/>
       <c r="C393" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="D393" s="11"/>
+        <v>24</v>
+      </c>
+      <c r="D393" s="18">
+        <v>2.0</v>
+      </c>
       <c r="E393" s="12"/>
       <c r="F393" s="13"/>
       <c r="H393" s="8"/>
@@ -11829,7 +11829,7 @@
       <c r="A394" s="8"/>
       <c r="B394" s="9"/>
       <c r="C394" s="17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D394" s="11"/>
       <c r="E394" s="12"/>
@@ -11853,7 +11853,7 @@
       <c r="A395" s="8"/>
       <c r="B395" s="9"/>
       <c r="C395" s="17" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="D395" s="11"/>
       <c r="E395" s="12"/>
@@ -11877,11 +11877,9 @@
       <c r="A396" s="8"/>
       <c r="B396" s="9"/>
       <c r="C396" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="D396" s="18">
-        <v>1.0</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="D396" s="11"/>
       <c r="E396" s="12"/>
       <c r="F396" s="13"/>
       <c r="H396" s="8"/>
@@ -11902,7 +11900,9 @@
     <row r="397">
       <c r="A397" s="8"/>
       <c r="B397" s="9"/>
-      <c r="C397" s="10"/>
+      <c r="C397" s="17" t="s">
+        <v>41</v>
+      </c>
       <c r="D397" s="11"/>
       <c r="E397" s="12"/>
       <c r="F397" s="13"/>
@@ -11923,21 +11923,15 @@
     </row>
     <row r="398">
       <c r="A398" s="8"/>
-      <c r="B398" s="16" t="s">
-        <v>245</v>
-      </c>
+      <c r="B398" s="9"/>
       <c r="C398" s="17" t="s">
-        <v>241</v>
+        <v>42</v>
       </c>
       <c r="D398" s="18">
-        <v>4.0</v>
-      </c>
-      <c r="E398" s="24" t="s">
-        <v>84</v>
-      </c>
-      <c r="F398" s="25">
-        <v>2.0</v>
-      </c>
+        <v>1.0</v>
+      </c>
+      <c r="E398" s="12"/>
+      <c r="F398" s="13"/>
       <c r="H398" s="8"/>
       <c r="I398" s="19"/>
       <c r="J398" s="20" t="s">
@@ -11958,12 +11952,8 @@
       <c r="B399" s="9"/>
       <c r="C399" s="10"/>
       <c r="D399" s="11"/>
-      <c r="E399" s="24" t="s">
-        <v>177</v>
-      </c>
-      <c r="F399" s="25">
-        <v>2.0</v>
-      </c>
+      <c r="E399" s="12"/>
+      <c r="F399" s="13"/>
       <c r="H399" s="8"/>
       <c r="I399" s="33"/>
       <c r="J399" s="27" t="s">
@@ -11983,18 +11973,20 @@
     </row>
     <row r="400">
       <c r="A400" s="8"/>
-      <c r="B400" s="9"/>
+      <c r="B400" s="16" t="s">
+        <v>245</v>
+      </c>
       <c r="C400" s="17" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D400" s="18">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="E400" s="24" t="s">
-        <v>243</v>
+        <v>84</v>
       </c>
       <c r="F400" s="25">
-        <v>1.5</v>
+        <v>2.0</v>
       </c>
       <c r="H400" s="8"/>
       <c r="I400" s="19"/>
@@ -12017,10 +12009,10 @@
       <c r="C401" s="10"/>
       <c r="D401" s="11"/>
       <c r="E401" s="24" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F401" s="25">
-        <v>1.5</v>
+        <v>2.0</v>
       </c>
       <c r="H401" s="8"/>
       <c r="I401" s="19"/>
@@ -12041,11 +12033,17 @@
       <c r="A402" s="8"/>
       <c r="B402" s="9"/>
       <c r="C402" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="D402" s="11"/>
-      <c r="E402" s="12"/>
-      <c r="F402" s="13"/>
+        <v>242</v>
+      </c>
+      <c r="D402" s="18">
+        <v>3.0</v>
+      </c>
+      <c r="E402" s="24" t="s">
+        <v>243</v>
+      </c>
+      <c r="F402" s="25">
+        <v>1.5</v>
+      </c>
       <c r="H402" s="8"/>
       <c r="I402" s="19"/>
       <c r="J402" s="27" t="s">
@@ -12066,12 +12064,14 @@
     <row r="403">
       <c r="A403" s="8"/>
       <c r="B403" s="9"/>
-      <c r="C403" s="17" t="s">
-        <v>22</v>
-      </c>
+      <c r="C403" s="10"/>
       <c r="D403" s="11"/>
-      <c r="E403" s="12"/>
-      <c r="F403" s="13"/>
+      <c r="E403" s="24" t="s">
+        <v>178</v>
+      </c>
+      <c r="F403" s="25">
+        <v>1.5</v>
+      </c>
       <c r="H403" s="8"/>
       <c r="I403" s="19"/>
       <c r="J403" s="27"/>
@@ -12089,7 +12089,7 @@
       <c r="A404" s="8"/>
       <c r="B404" s="9"/>
       <c r="C404" s="17" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="D404" s="11"/>
       <c r="E404" s="12"/>
@@ -12117,7 +12117,7 @@
       <c r="A405" s="8"/>
       <c r="B405" s="9"/>
       <c r="C405" s="17" t="s">
-        <v>51</v>
+        <v>22</v>
       </c>
       <c r="D405" s="11"/>
       <c r="E405" s="12"/>
@@ -12141,15 +12141,11 @@
       <c r="A406" s="8"/>
       <c r="B406" s="9"/>
       <c r="C406" s="17" t="s">
-        <v>220</v>
+        <v>26</v>
       </c>
       <c r="D406" s="11"/>
-      <c r="E406" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="F406" s="25">
-        <v>2.0</v>
-      </c>
+      <c r="E406" s="12"/>
+      <c r="F406" s="13"/>
       <c r="H406" s="8"/>
       <c r="I406" s="19"/>
       <c r="J406" s="27" t="s">
@@ -12168,14 +12164,12 @@
     <row r="407">
       <c r="A407" s="8"/>
       <c r="B407" s="9"/>
-      <c r="C407" s="10"/>
+      <c r="C407" s="17" t="s">
+        <v>51</v>
+      </c>
       <c r="D407" s="11"/>
-      <c r="E407" s="24" t="s">
-        <v>221</v>
-      </c>
-      <c r="F407" s="25">
-        <v>1.0</v>
-      </c>
+      <c r="E407" s="12"/>
+      <c r="F407" s="13"/>
       <c r="H407" s="8"/>
       <c r="I407" s="19"/>
       <c r="J407" s="27" t="s">
@@ -12195,13 +12189,15 @@
       <c r="A408" s="8"/>
       <c r="B408" s="9"/>
       <c r="C408" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="D408" s="18">
+        <v>220</v>
+      </c>
+      <c r="D408" s="11"/>
+      <c r="E408" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="F408" s="25">
         <v>2.0</v>
       </c>
-      <c r="E408" s="12"/>
-      <c r="F408" s="13"/>
       <c r="H408" s="8"/>
       <c r="I408" s="19"/>
       <c r="J408" s="27" t="s">
@@ -12222,12 +12218,14 @@
     <row r="409">
       <c r="A409" s="8"/>
       <c r="B409" s="9"/>
-      <c r="C409" s="17" t="s">
-        <v>39</v>
-      </c>
+      <c r="C409" s="10"/>
       <c r="D409" s="11"/>
-      <c r="E409" s="12"/>
-      <c r="F409" s="13"/>
+      <c r="E409" s="24" t="s">
+        <v>221</v>
+      </c>
+      <c r="F409" s="25">
+        <v>1.0</v>
+      </c>
       <c r="H409" s="8"/>
       <c r="I409" s="19"/>
       <c r="J409" s="27" t="s">
@@ -12247,9 +12245,11 @@
       <c r="A410" s="8"/>
       <c r="B410" s="9"/>
       <c r="C410" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="D410" s="11"/>
+        <v>24</v>
+      </c>
+      <c r="D410" s="18">
+        <v>2.0</v>
+      </c>
       <c r="E410" s="12"/>
       <c r="F410" s="13"/>
       <c r="H410" s="8"/>
@@ -12271,7 +12271,7 @@
       <c r="A411" s="8"/>
       <c r="B411" s="9"/>
       <c r="C411" s="17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D411" s="11"/>
       <c r="E411" s="12"/>
@@ -12297,7 +12297,7 @@
       <c r="A412" s="8"/>
       <c r="B412" s="9"/>
       <c r="C412" s="17" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="D412" s="11"/>
       <c r="E412" s="12"/>
@@ -12321,11 +12321,9 @@
       <c r="A413" s="8"/>
       <c r="B413" s="9"/>
       <c r="C413" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="D413" s="18">
-        <v>1.0</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="D413" s="11"/>
       <c r="E413" s="12"/>
       <c r="F413" s="13"/>
       <c r="H413" s="8"/>
@@ -12346,7 +12344,9 @@
     <row r="414">
       <c r="A414" s="8"/>
       <c r="B414" s="9"/>
-      <c r="C414" s="10"/>
+      <c r="C414" s="17" t="s">
+        <v>41</v>
+      </c>
       <c r="D414" s="11"/>
       <c r="E414" s="12"/>
       <c r="F414" s="13"/>
@@ -12367,14 +12367,12 @@
     </row>
     <row r="415">
       <c r="A415" s="8"/>
-      <c r="B415" s="16" t="s">
-        <v>248</v>
-      </c>
+      <c r="B415" s="9"/>
       <c r="C415" s="17" t="s">
-        <v>95</v>
+        <v>42</v>
       </c>
       <c r="D415" s="18">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
       <c r="E415" s="12"/>
       <c r="F415" s="13"/>
@@ -12398,12 +12396,8 @@
     <row r="416">
       <c r="A416" s="8"/>
       <c r="B416" s="9"/>
-      <c r="C416" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="D416" s="18">
-        <v>3.0</v>
-      </c>
+      <c r="C416" s="10"/>
+      <c r="D416" s="11"/>
       <c r="E416" s="12"/>
       <c r="F416" s="13"/>
       <c r="H416" s="8"/>
@@ -12421,11 +12415,15 @@
     </row>
     <row r="417">
       <c r="A417" s="8"/>
-      <c r="B417" s="9"/>
+      <c r="B417" s="16" t="s">
+        <v>248</v>
+      </c>
       <c r="C417" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="D417" s="11"/>
+        <v>95</v>
+      </c>
+      <c r="D417" s="18">
+        <v>4.0</v>
+      </c>
       <c r="E417" s="12"/>
       <c r="F417" s="13"/>
       <c r="H417" s="8"/>
@@ -12451,9 +12449,11 @@
       <c r="A418" s="8"/>
       <c r="B418" s="9"/>
       <c r="C418" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="D418" s="11"/>
+        <v>97</v>
+      </c>
+      <c r="D418" s="18">
+        <v>3.0</v>
+      </c>
       <c r="E418" s="12"/>
       <c r="F418" s="13"/>
       <c r="H418" s="8"/>
@@ -12475,7 +12475,7 @@
       <c r="A419" s="8"/>
       <c r="B419" s="9"/>
       <c r="C419" s="17" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="D419" s="11"/>
       <c r="E419" s="12"/>
@@ -12499,15 +12499,11 @@
       <c r="A420" s="8"/>
       <c r="B420" s="9"/>
       <c r="C420" s="17" t="s">
-        <v>220</v>
+        <v>22</v>
       </c>
       <c r="D420" s="11"/>
-      <c r="E420" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="F420" s="25">
-        <v>2.0</v>
-      </c>
+      <c r="E420" s="12"/>
+      <c r="F420" s="13"/>
       <c r="H420" s="8"/>
       <c r="I420" s="19"/>
       <c r="J420" s="27" t="s">
@@ -12526,14 +12522,12 @@
     <row r="421">
       <c r="A421" s="8"/>
       <c r="B421" s="9"/>
-      <c r="C421" s="10"/>
+      <c r="C421" s="17" t="s">
+        <v>26</v>
+      </c>
       <c r="D421" s="11"/>
-      <c r="E421" s="24" t="s">
-        <v>221</v>
-      </c>
-      <c r="F421" s="25">
-        <v>1.0</v>
-      </c>
+      <c r="E421" s="12"/>
+      <c r="F421" s="13"/>
       <c r="H421" s="8"/>
       <c r="I421" s="19"/>
       <c r="J421" s="27" t="s">
@@ -12555,13 +12549,15 @@
       <c r="A422" s="8"/>
       <c r="B422" s="9"/>
       <c r="C422" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="D422" s="18">
+        <v>220</v>
+      </c>
+      <c r="D422" s="11"/>
+      <c r="E422" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="F422" s="25">
         <v>2.0</v>
       </c>
-      <c r="E422" s="12"/>
-      <c r="F422" s="13"/>
       <c r="H422" s="8"/>
       <c r="I422" s="19"/>
       <c r="J422" s="27" t="s">
@@ -12580,12 +12576,14 @@
     <row r="423">
       <c r="A423" s="8"/>
       <c r="B423" s="9"/>
-      <c r="C423" s="17" t="s">
-        <v>39</v>
-      </c>
+      <c r="C423" s="10"/>
       <c r="D423" s="11"/>
-      <c r="E423" s="12"/>
-      <c r="F423" s="13"/>
+      <c r="E423" s="24" t="s">
+        <v>221</v>
+      </c>
+      <c r="F423" s="25">
+        <v>1.0</v>
+      </c>
       <c r="H423" s="8"/>
       <c r="I423" s="19"/>
       <c r="J423" s="27" t="s">
@@ -12605,9 +12603,11 @@
       <c r="A424" s="8"/>
       <c r="B424" s="9"/>
       <c r="C424" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="D424" s="11"/>
+        <v>24</v>
+      </c>
+      <c r="D424" s="18">
+        <v>2.0</v>
+      </c>
       <c r="E424" s="12"/>
       <c r="F424" s="13"/>
       <c r="H424" s="8"/>
@@ -12631,7 +12631,7 @@
       <c r="A425" s="8"/>
       <c r="B425" s="9"/>
       <c r="C425" s="17" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D425" s="11"/>
       <c r="E425" s="12"/>
@@ -12655,7 +12655,7 @@
       <c r="A426" s="8"/>
       <c r="B426" s="9"/>
       <c r="C426" s="17" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="D426" s="11"/>
       <c r="E426" s="12"/>
@@ -12679,11 +12679,9 @@
       <c r="A427" s="8"/>
       <c r="B427" s="9"/>
       <c r="C427" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="D427" s="18">
-        <v>1.0</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="D427" s="11"/>
       <c r="E427" s="12"/>
       <c r="F427" s="13"/>
       <c r="H427" s="8"/>
@@ -12704,7 +12702,9 @@
     <row r="428">
       <c r="A428" s="8"/>
       <c r="B428" s="9"/>
-      <c r="C428" s="10"/>
+      <c r="C428" s="17" t="s">
+        <v>41</v>
+      </c>
       <c r="D428" s="11"/>
       <c r="E428" s="12"/>
       <c r="F428" s="13"/>
@@ -12727,14 +12727,12 @@
     </row>
     <row r="429">
       <c r="A429" s="8"/>
-      <c r="B429" s="16" t="s">
-        <v>250</v>
-      </c>
+      <c r="B429" s="9"/>
       <c r="C429" s="17" t="s">
-        <v>95</v>
+        <v>42</v>
       </c>
       <c r="D429" s="18">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
       <c r="E429" s="12"/>
       <c r="F429" s="13"/>
@@ -12754,17 +12752,13 @@
     <row r="430">
       <c r="A430" s="8"/>
       <c r="B430" s="9"/>
-      <c r="C430" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="D430" s="18">
-        <v>3.0</v>
-      </c>
+      <c r="C430" s="10"/>
+      <c r="D430" s="11"/>
       <c r="E430" s="12"/>
       <c r="F430" s="13"/>
       <c r="H430" s="8"/>
       <c r="I430" s="19" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="J430" s="27" t="s">
         <v>62</v>
@@ -12783,11 +12777,15 @@
     </row>
     <row r="431">
       <c r="A431" s="8"/>
-      <c r="B431" s="9"/>
+      <c r="B431" s="16" t="s">
+        <v>251</v>
+      </c>
       <c r="C431" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="D431" s="11"/>
+        <v>95</v>
+      </c>
+      <c r="D431" s="18">
+        <v>4.0</v>
+      </c>
       <c r="E431" s="12"/>
       <c r="F431" s="13"/>
       <c r="H431" s="8"/>
@@ -12809,9 +12807,11 @@
       <c r="A432" s="8"/>
       <c r="B432" s="9"/>
       <c r="C432" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="D432" s="11"/>
+        <v>97</v>
+      </c>
+      <c r="D432" s="18">
+        <v>3.0</v>
+      </c>
       <c r="E432" s="12"/>
       <c r="F432" s="13"/>
       <c r="H432" s="8"/>
@@ -12833,7 +12833,7 @@
       <c r="A433" s="8"/>
       <c r="B433" s="9"/>
       <c r="C433" s="17" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="D433" s="11"/>
       <c r="E433" s="12"/>
@@ -12857,7 +12857,7 @@
       <c r="A434" s="8"/>
       <c r="B434" s="9"/>
       <c r="C434" s="17" t="s">
-        <v>51</v>
+        <v>22</v>
       </c>
       <c r="D434" s="11"/>
       <c r="E434" s="12"/>
@@ -12883,15 +12883,11 @@
       <c r="A435" s="8"/>
       <c r="B435" s="9"/>
       <c r="C435" s="17" t="s">
-        <v>220</v>
+        <v>26</v>
       </c>
       <c r="D435" s="11"/>
-      <c r="E435" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="F435" s="25">
-        <v>2.0</v>
-      </c>
+      <c r="E435" s="12"/>
+      <c r="F435" s="13"/>
       <c r="H435" s="8"/>
       <c r="I435" s="19"/>
       <c r="J435" s="27" t="s">
@@ -12910,14 +12906,12 @@
     <row r="436">
       <c r="A436" s="8"/>
       <c r="B436" s="9"/>
-      <c r="C436" s="10"/>
+      <c r="C436" s="17" t="s">
+        <v>51</v>
+      </c>
       <c r="D436" s="11"/>
-      <c r="E436" s="24" t="s">
-        <v>221</v>
-      </c>
-      <c r="F436" s="25">
-        <v>1.0</v>
-      </c>
+      <c r="E436" s="12"/>
+      <c r="F436" s="13"/>
       <c r="H436" s="8"/>
       <c r="I436" s="19"/>
       <c r="J436" s="27" t="s">
@@ -12937,13 +12931,15 @@
       <c r="A437" s="8"/>
       <c r="B437" s="9"/>
       <c r="C437" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="D437" s="18">
+        <v>220</v>
+      </c>
+      <c r="D437" s="11"/>
+      <c r="E437" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="F437" s="25">
         <v>2.0</v>
       </c>
-      <c r="E437" s="12"/>
-      <c r="F437" s="13"/>
       <c r="H437" s="8"/>
       <c r="I437" s="19"/>
       <c r="J437" s="27" t="s">
@@ -12962,12 +12958,14 @@
     <row r="438">
       <c r="A438" s="8"/>
       <c r="B438" s="9"/>
-      <c r="C438" s="17" t="s">
-        <v>39</v>
-      </c>
+      <c r="C438" s="10"/>
       <c r="D438" s="11"/>
-      <c r="E438" s="12"/>
-      <c r="F438" s="13"/>
+      <c r="E438" s="24" t="s">
+        <v>221</v>
+      </c>
+      <c r="F438" s="25">
+        <v>1.0</v>
+      </c>
       <c r="H438" s="8"/>
       <c r="I438" s="19"/>
       <c r="J438" s="20" t="s">
@@ -12989,9 +12987,11 @@
       <c r="A439" s="8"/>
       <c r="B439" s="9"/>
       <c r="C439" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="D439" s="11"/>
+        <v>24</v>
+      </c>
+      <c r="D439" s="18">
+        <v>2.0</v>
+      </c>
       <c r="E439" s="12"/>
       <c r="F439" s="13"/>
       <c r="H439" s="8"/>
@@ -13013,7 +13013,7 @@
       <c r="A440" s="8"/>
       <c r="B440" s="9"/>
       <c r="C440" s="17" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D440" s="11"/>
       <c r="E440" s="12"/>
@@ -13037,7 +13037,7 @@
       <c r="A441" s="8"/>
       <c r="B441" s="9"/>
       <c r="C441" s="17" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="D441" s="11"/>
       <c r="E441" s="12"/>
@@ -13063,11 +13063,9 @@
       <c r="A442" s="8"/>
       <c r="B442" s="9"/>
       <c r="C442" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="D442" s="18">
-        <v>1.0</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="D442" s="11"/>
       <c r="E442" s="12"/>
       <c r="F442" s="13"/>
       <c r="H442" s="8"/>
@@ -13086,7 +13084,9 @@
     <row r="443">
       <c r="A443" s="8"/>
       <c r="B443" s="9"/>
-      <c r="C443" s="10"/>
+      <c r="C443" s="17" t="s">
+        <v>41</v>
+      </c>
       <c r="D443" s="11"/>
       <c r="E443" s="12"/>
       <c r="F443" s="13"/>
@@ -13111,14 +13111,12 @@
     </row>
     <row r="444">
       <c r="A444" s="8"/>
-      <c r="B444" s="16" t="s">
-        <v>253</v>
-      </c>
+      <c r="B444" s="9"/>
       <c r="C444" s="17" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D444" s="18">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
       <c r="E444" s="12"/>
       <c r="F444" s="13"/>
@@ -13142,12 +13140,8 @@
     <row r="445">
       <c r="A445" s="8"/>
       <c r="B445" s="9"/>
-      <c r="C445" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="D445" s="18">
-        <v>3.0</v>
-      </c>
+      <c r="C445" s="10"/>
+      <c r="D445" s="11"/>
       <c r="E445" s="12"/>
       <c r="F445" s="13"/>
       <c r="H445" s="8"/>
@@ -13167,11 +13161,15 @@
     </row>
     <row r="446">
       <c r="A446" s="8"/>
-      <c r="B446" s="9"/>
+      <c r="B446" s="16" t="s">
+        <v>253</v>
+      </c>
       <c r="C446" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="D446" s="11"/>
+        <v>39</v>
+      </c>
+      <c r="D446" s="18">
+        <v>4.0</v>
+      </c>
       <c r="E446" s="12"/>
       <c r="F446" s="13"/>
       <c r="H446" s="8"/>
@@ -13193,9 +13191,11 @@
       <c r="A447" s="8"/>
       <c r="B447" s="9"/>
       <c r="C447" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="D447" s="11"/>
+        <v>68</v>
+      </c>
+      <c r="D447" s="18">
+        <v>3.0</v>
+      </c>
       <c r="E447" s="12"/>
       <c r="F447" s="13"/>
       <c r="H447" s="8"/>
@@ -13217,15 +13217,11 @@
       <c r="A448" s="8"/>
       <c r="B448" s="9"/>
       <c r="C448" s="17" t="s">
-        <v>220</v>
+        <v>22</v>
       </c>
       <c r="D448" s="11"/>
-      <c r="E448" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="F448" s="25">
-        <v>2.0</v>
-      </c>
+      <c r="E448" s="12"/>
+      <c r="F448" s="13"/>
       <c r="H448" s="8"/>
       <c r="I448" s="19"/>
       <c r="J448" s="27" t="s">
@@ -13244,14 +13240,12 @@
     <row r="449">
       <c r="A449" s="8"/>
       <c r="B449" s="9"/>
-      <c r="C449" s="10"/>
+      <c r="C449" s="17" t="s">
+        <v>26</v>
+      </c>
       <c r="D449" s="11"/>
-      <c r="E449" s="24" t="s">
-        <v>221</v>
-      </c>
-      <c r="F449" s="25">
-        <v>1.0</v>
-      </c>
+      <c r="E449" s="12"/>
+      <c r="F449" s="13"/>
       <c r="H449" s="8"/>
       <c r="I449" s="19"/>
       <c r="J449" s="34" t="s">
@@ -13271,13 +13265,15 @@
       <c r="A450" s="8"/>
       <c r="B450" s="9"/>
       <c r="C450" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="D450" s="18">
+        <v>220</v>
+      </c>
+      <c r="D450" s="11"/>
+      <c r="E450" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="F450" s="25">
         <v>2.0</v>
       </c>
-      <c r="E450" s="12"/>
-      <c r="F450" s="13"/>
       <c r="H450" s="8"/>
       <c r="I450" s="19"/>
       <c r="J450" s="27" t="s">
@@ -13296,12 +13292,14 @@
     <row r="451">
       <c r="A451" s="8"/>
       <c r="B451" s="9"/>
-      <c r="C451" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="D451" s="18"/>
-      <c r="E451" s="12"/>
-      <c r="F451" s="13"/>
+      <c r="C451" s="10"/>
+      <c r="D451" s="11"/>
+      <c r="E451" s="24" t="s">
+        <v>221</v>
+      </c>
+      <c r="F451" s="25">
+        <v>1.0</v>
+      </c>
       <c r="H451" s="8"/>
       <c r="I451" s="19"/>
       <c r="J451" s="27" t="s">
@@ -13323,9 +13321,11 @@
       <c r="A452" s="8"/>
       <c r="B452" s="9"/>
       <c r="C452" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="D452" s="18"/>
+        <v>67</v>
+      </c>
+      <c r="D452" s="18">
+        <v>2.0</v>
+      </c>
       <c r="E452" s="12"/>
       <c r="F452" s="13"/>
       <c r="H452" s="8"/>
@@ -13347,7 +13347,7 @@
       <c r="A453" s="8"/>
       <c r="B453" s="9"/>
       <c r="C453" s="17" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="D453" s="18"/>
       <c r="E453" s="12"/>
@@ -13371,7 +13371,7 @@
       <c r="A454" s="8"/>
       <c r="B454" s="9"/>
       <c r="C454" s="17" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="D454" s="18"/>
       <c r="E454" s="12"/>
@@ -13395,7 +13395,7 @@
       <c r="A455" s="8"/>
       <c r="B455" s="9"/>
       <c r="C455" s="17" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D455" s="18"/>
       <c r="E455" s="12"/>
@@ -13421,7 +13421,7 @@
       <c r="A456" s="8"/>
       <c r="B456" s="9"/>
       <c r="C456" s="17" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D456" s="18"/>
       <c r="E456" s="12"/>
@@ -13443,11 +13443,9 @@
       <c r="A457" s="8"/>
       <c r="B457" s="9"/>
       <c r="C457" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="D457" s="18">
-        <v>1.0</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="D457" s="18"/>
       <c r="E457" s="12"/>
       <c r="F457" s="13"/>
       <c r="H457" s="8"/>
@@ -13471,11 +13469,13 @@
     </row>
     <row r="458">
       <c r="A458" s="8"/>
-      <c r="B458" s="19"/>
-      <c r="C458" s="20"/>
-      <c r="D458" s="26"/>
-      <c r="E458" s="22"/>
-      <c r="F458" s="23"/>
+      <c r="B458" s="9"/>
+      <c r="C458" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="D458" s="18"/>
+      <c r="E458" s="12"/>
+      <c r="F458" s="13"/>
       <c r="H458" s="8"/>
       <c r="I458" s="19"/>
       <c r="J458" s="27" t="s">
@@ -13495,17 +13495,15 @@
     </row>
     <row r="459">
       <c r="A459" s="8"/>
-      <c r="B459" s="32" t="s">
-        <v>256</v>
-      </c>
-      <c r="C459" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="D459" s="21">
-        <v>4.0</v>
-      </c>
-      <c r="E459" s="22"/>
-      <c r="F459" s="23"/>
+      <c r="B459" s="9"/>
+      <c r="C459" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="D459" s="18">
+        <v>1.0</v>
+      </c>
+      <c r="E459" s="12"/>
+      <c r="F459" s="13"/>
       <c r="H459" s="8"/>
       <c r="I459" s="19"/>
       <c r="J459" s="27" t="s">
@@ -13524,12 +13522,8 @@
     <row r="460">
       <c r="A460" s="8"/>
       <c r="B460" s="19"/>
-      <c r="C460" s="20" t="s">
-        <v>68</v>
-      </c>
-      <c r="D460" s="21">
-        <v>3.0</v>
-      </c>
+      <c r="C460" s="20"/>
+      <c r="D460" s="26"/>
       <c r="E460" s="22"/>
       <c r="F460" s="23"/>
       <c r="H460" s="8"/>
@@ -13549,11 +13543,15 @@
     </row>
     <row r="461">
       <c r="A461" s="8"/>
-      <c r="B461" s="19"/>
+      <c r="B461" s="32" t="s">
+        <v>256</v>
+      </c>
       <c r="C461" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="D461" s="26"/>
+        <v>39</v>
+      </c>
+      <c r="D461" s="21">
+        <v>4.0</v>
+      </c>
       <c r="E461" s="22"/>
       <c r="F461" s="23"/>
       <c r="H461" s="8"/>
@@ -13575,9 +13573,11 @@
       <c r="A462" s="8"/>
       <c r="B462" s="19"/>
       <c r="C462" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="D462" s="26"/>
+        <v>68</v>
+      </c>
+      <c r="D462" s="21">
+        <v>3.0</v>
+      </c>
       <c r="E462" s="22"/>
       <c r="F462" s="23"/>
       <c r="H462" s="8"/>
@@ -13598,8 +13598,8 @@
     <row r="463">
       <c r="A463" s="8"/>
       <c r="B463" s="19"/>
-      <c r="C463" s="35" t="s">
-        <v>51</v>
+      <c r="C463" s="20" t="s">
+        <v>22</v>
       </c>
       <c r="D463" s="26"/>
       <c r="E463" s="22"/>
@@ -13623,15 +13623,11 @@
       <c r="A464" s="8"/>
       <c r="B464" s="19"/>
       <c r="C464" s="20" t="s">
-        <v>220</v>
+        <v>26</v>
       </c>
       <c r="D464" s="26"/>
-      <c r="E464" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="F464" s="30">
-        <v>2.0</v>
-      </c>
+      <c r="E464" s="22"/>
+      <c r="F464" s="23"/>
       <c r="H464" s="8"/>
       <c r="I464" s="19"/>
       <c r="J464" s="27" t="s">
@@ -13650,14 +13646,12 @@
     <row r="465">
       <c r="A465" s="8"/>
       <c r="B465" s="19"/>
-      <c r="C465" s="20"/>
+      <c r="C465" s="35" t="s">
+        <v>51</v>
+      </c>
       <c r="D465" s="26"/>
-      <c r="E465" s="22" t="s">
-        <v>221</v>
-      </c>
-      <c r="F465" s="30">
-        <v>1.0</v>
-      </c>
+      <c r="E465" s="22"/>
+      <c r="F465" s="23"/>
       <c r="H465" s="8"/>
       <c r="I465" s="19"/>
       <c r="J465" s="27" t="s">
@@ -13679,13 +13673,15 @@
       <c r="A466" s="8"/>
       <c r="B466" s="19"/>
       <c r="C466" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="D466" s="21">
+        <v>220</v>
+      </c>
+      <c r="D466" s="26"/>
+      <c r="E466" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="F466" s="30">
         <v>2.0</v>
       </c>
-      <c r="E466" s="22"/>
-      <c r="F466" s="23"/>
       <c r="H466" s="8"/>
       <c r="I466" s="19"/>
       <c r="J466" s="27" t="s">
@@ -13704,12 +13700,14 @@
     <row r="467">
       <c r="A467" s="8"/>
       <c r="B467" s="19"/>
-      <c r="C467" s="20" t="s">
-        <v>34</v>
-      </c>
+      <c r="C467" s="20"/>
       <c r="D467" s="26"/>
-      <c r="E467" s="22"/>
-      <c r="F467" s="23"/>
+      <c r="E467" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="F467" s="30">
+        <v>1.0</v>
+      </c>
       <c r="H467" s="8"/>
       <c r="I467" s="19"/>
       <c r="J467" s="27" t="s">
@@ -13729,9 +13727,11 @@
       <c r="A468" s="8"/>
       <c r="B468" s="19"/>
       <c r="C468" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="D468" s="26"/>
+        <v>67</v>
+      </c>
+      <c r="D468" s="21">
+        <v>2.0</v>
+      </c>
       <c r="E468" s="22"/>
       <c r="F468" s="23"/>
       <c r="H468" s="8"/>
@@ -13753,7 +13753,7 @@
       <c r="A469" s="8"/>
       <c r="B469" s="19"/>
       <c r="C469" s="20" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="D469" s="26"/>
       <c r="E469" s="22"/>
@@ -13779,7 +13779,7 @@
       <c r="A470" s="8"/>
       <c r="B470" s="19"/>
       <c r="C470" s="20" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="D470" s="26"/>
       <c r="E470" s="22"/>
@@ -13801,7 +13801,7 @@
       <c r="A471" s="8"/>
       <c r="B471" s="19"/>
       <c r="C471" s="20" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D471" s="26"/>
       <c r="E471" s="22"/>
@@ -13829,7 +13829,7 @@
       <c r="A472" s="8"/>
       <c r="B472" s="19"/>
       <c r="C472" s="20" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D472" s="26"/>
       <c r="E472" s="22"/>
@@ -13853,11 +13853,9 @@
       <c r="A473" s="8"/>
       <c r="B473" s="19"/>
       <c r="C473" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="D473" s="21">
-        <v>1.0</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="D473" s="26"/>
       <c r="E473" s="22"/>
       <c r="F473" s="23"/>
       <c r="H473" s="8"/>
@@ -13879,11 +13877,13 @@
     </row>
     <row r="474">
       <c r="A474" s="8"/>
-      <c r="B474" s="9"/>
-      <c r="C474" s="10"/>
-      <c r="D474" s="11"/>
-      <c r="E474" s="12"/>
-      <c r="F474" s="13"/>
+      <c r="B474" s="19"/>
+      <c r="C474" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D474" s="26"/>
+      <c r="E474" s="22"/>
+      <c r="F474" s="23"/>
       <c r="H474" s="15"/>
       <c r="I474" s="19"/>
       <c r="J474" s="27" t="s">
@@ -13900,12 +13900,16 @@
       <c r="T474" s="13"/>
     </row>
     <row r="475">
-      <c r="A475" s="15"/>
-      <c r="B475" s="16"/>
-      <c r="C475" s="17"/>
-      <c r="D475" s="18"/>
-      <c r="E475" s="12"/>
-      <c r="F475" s="13"/>
+      <c r="A475" s="8"/>
+      <c r="B475" s="19"/>
+      <c r="C475" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="D475" s="21">
+        <v>1.0</v>
+      </c>
+      <c r="E475" s="22"/>
+      <c r="F475" s="23"/>
       <c r="H475" s="8"/>
       <c r="I475" s="19"/>
       <c r="J475" s="27" t="s">
@@ -13924,7 +13928,7 @@
     <row r="476">
       <c r="A476" s="8"/>
       <c r="B476" s="9"/>
-      <c r="C476" s="17"/>
+      <c r="C476" s="10"/>
       <c r="D476" s="11"/>
       <c r="E476" s="12"/>
       <c r="F476" s="13"/>
@@ -14021,7 +14025,7 @@
       <c r="H480" s="8"/>
       <c r="I480" s="19"/>
       <c r="J480" s="34" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="K480" s="26"/>
       <c r="L480" s="22"/>

</xml_diff>

<commit_message>
Added Philo and Geo to 2MC and organized the assets folder
</commit_message>
<xml_diff>
--- a/assets/All Classes.xlsx
+++ b/assets/All Classes.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1278" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1280" uniqueCount="258">
   <si>
     <t>Macros</t>
   </si>
@@ -757,10 +757,10 @@
     <t>EduCitoyen</t>
   </si>
   <si>
+    <t>3GSN</t>
+  </si>
+  <si>
     <t>2MF</t>
-  </si>
-  <si>
-    <t>3GSN</t>
   </si>
   <si>
     <t>2GSN</t>
@@ -895,7 +895,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1004,6 +1004,9 @@
     <xf borderId="0" fillId="13" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="8" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -11504,16 +11507,14 @@
       <c r="T381" s="13"/>
     </row>
     <row r="382">
-      <c r="A382" s="8"/>
-      <c r="B382" s="9"/>
+      <c r="A382" s="40"/>
+      <c r="B382" s="19"/>
       <c r="C382" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="D382" s="18">
-        <v>1.0</v>
-      </c>
-      <c r="E382" s="12"/>
-      <c r="F382" s="13"/>
+        <v>72</v>
+      </c>
+      <c r="D382" s="21"/>
+      <c r="E382" s="22"/>
+      <c r="F382" s="23"/>
       <c r="H382" s="8"/>
       <c r="I382" s="19"/>
       <c r="J382" s="27" t="s">
@@ -11530,12 +11531,14 @@
       <c r="T382" s="13"/>
     </row>
     <row r="383">
-      <c r="A383" s="8"/>
-      <c r="B383" s="9"/>
-      <c r="C383" s="10"/>
-      <c r="D383" s="11"/>
-      <c r="E383" s="12"/>
-      <c r="F383" s="13"/>
+      <c r="A383" s="40"/>
+      <c r="B383" s="19"/>
+      <c r="C383" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D383" s="21"/>
+      <c r="E383" s="22"/>
+      <c r="F383" s="23"/>
       <c r="H383" s="8"/>
       <c r="I383" s="19"/>
       <c r="J383" s="27" t="s">
@@ -11553,21 +11556,15 @@
     </row>
     <row r="384">
       <c r="A384" s="8"/>
-      <c r="B384" s="16" t="s">
-        <v>240</v>
-      </c>
+      <c r="B384" s="9"/>
       <c r="C384" s="17" t="s">
-        <v>241</v>
+        <v>42</v>
       </c>
       <c r="D384" s="18">
-        <v>4.0</v>
-      </c>
-      <c r="E384" s="24" t="s">
-        <v>84</v>
-      </c>
-      <c r="F384" s="25">
-        <v>2.0</v>
-      </c>
+        <v>1.0</v>
+      </c>
+      <c r="E384" s="12"/>
+      <c r="F384" s="13"/>
       <c r="H384" s="8"/>
       <c r="I384" s="19"/>
       <c r="J384" s="27" t="s">
@@ -11588,12 +11585,8 @@
       <c r="B385" s="9"/>
       <c r="C385" s="10"/>
       <c r="D385" s="11"/>
-      <c r="E385" s="24" t="s">
-        <v>177</v>
-      </c>
-      <c r="F385" s="25">
-        <v>2.0</v>
-      </c>
+      <c r="E385" s="12"/>
+      <c r="F385" s="13"/>
       <c r="H385" s="8"/>
       <c r="I385" s="19"/>
       <c r="J385" s="20" t="s">
@@ -11611,18 +11604,20 @@
     </row>
     <row r="386">
       <c r="A386" s="8"/>
-      <c r="B386" s="9"/>
+      <c r="B386" s="16" t="s">
+        <v>240</v>
+      </c>
       <c r="C386" s="17" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D386" s="18">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="E386" s="24" t="s">
-        <v>243</v>
+        <v>84</v>
       </c>
       <c r="F386" s="25">
-        <v>1.5</v>
+        <v>2.0</v>
       </c>
       <c r="H386" s="8"/>
       <c r="I386" s="33"/>
@@ -11645,10 +11640,10 @@
       <c r="C387" s="10"/>
       <c r="D387" s="11"/>
       <c r="E387" s="24" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F387" s="25">
-        <v>1.5</v>
+        <v>2.0</v>
       </c>
       <c r="H387" s="8"/>
       <c r="I387" s="19"/>
@@ -11671,11 +11666,17 @@
       <c r="A388" s="8"/>
       <c r="B388" s="9"/>
       <c r="C388" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="D388" s="11"/>
-      <c r="E388" s="12"/>
-      <c r="F388" s="13"/>
+        <v>242</v>
+      </c>
+      <c r="D388" s="18">
+        <v>3.0</v>
+      </c>
+      <c r="E388" s="24" t="s">
+        <v>243</v>
+      </c>
+      <c r="F388" s="25">
+        <v>1.5</v>
+      </c>
       <c r="H388" s="8"/>
       <c r="I388" s="19"/>
       <c r="J388" s="27" t="s">
@@ -11696,12 +11697,14 @@
     <row r="389">
       <c r="A389" s="8"/>
       <c r="B389" s="9"/>
-      <c r="C389" s="17" t="s">
-        <v>22</v>
-      </c>
+      <c r="C389" s="10"/>
       <c r="D389" s="11"/>
-      <c r="E389" s="12"/>
-      <c r="F389" s="13"/>
+      <c r="E389" s="24" t="s">
+        <v>178</v>
+      </c>
+      <c r="F389" s="25">
+        <v>1.5</v>
+      </c>
       <c r="H389" s="8"/>
       <c r="I389" s="19"/>
       <c r="J389" s="27"/>
@@ -11719,7 +11722,7 @@
       <c r="A390" s="8"/>
       <c r="B390" s="9"/>
       <c r="C390" s="17" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="D390" s="11"/>
       <c r="E390" s="12"/>
@@ -11747,15 +11750,11 @@
       <c r="A391" s="8"/>
       <c r="B391" s="9"/>
       <c r="C391" s="17" t="s">
-        <v>220</v>
+        <v>22</v>
       </c>
       <c r="D391" s="11"/>
-      <c r="E391" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="F391" s="25">
-        <v>2.0</v>
-      </c>
+      <c r="E391" s="12"/>
+      <c r="F391" s="13"/>
       <c r="H391" s="8"/>
       <c r="I391" s="19"/>
       <c r="J391" s="27" t="s">
@@ -11774,14 +11773,12 @@
     <row r="392">
       <c r="A392" s="8"/>
       <c r="B392" s="9"/>
-      <c r="C392" s="10"/>
+      <c r="C392" s="17" t="s">
+        <v>26</v>
+      </c>
       <c r="D392" s="11"/>
-      <c r="E392" s="24" t="s">
-        <v>221</v>
-      </c>
-      <c r="F392" s="25">
-        <v>1.0</v>
-      </c>
+      <c r="E392" s="12"/>
+      <c r="F392" s="13"/>
       <c r="H392" s="8"/>
       <c r="I392" s="19"/>
       <c r="J392" s="27" t="s">
@@ -11801,13 +11798,15 @@
       <c r="A393" s="8"/>
       <c r="B393" s="9"/>
       <c r="C393" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="D393" s="18">
+        <v>220</v>
+      </c>
+      <c r="D393" s="11"/>
+      <c r="E393" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="F393" s="25">
         <v>2.0</v>
       </c>
-      <c r="E393" s="12"/>
-      <c r="F393" s="13"/>
       <c r="H393" s="8"/>
       <c r="I393" s="19"/>
       <c r="J393" s="27" t="s">
@@ -11828,12 +11827,14 @@
     <row r="394">
       <c r="A394" s="8"/>
       <c r="B394" s="9"/>
-      <c r="C394" s="17" t="s">
-        <v>39</v>
-      </c>
+      <c r="C394" s="10"/>
       <c r="D394" s="11"/>
-      <c r="E394" s="12"/>
-      <c r="F394" s="13"/>
+      <c r="E394" s="24" t="s">
+        <v>221</v>
+      </c>
+      <c r="F394" s="25">
+        <v>1.0</v>
+      </c>
       <c r="H394" s="8"/>
       <c r="I394" s="19"/>
       <c r="J394" s="27" t="s">
@@ -11853,9 +11854,11 @@
       <c r="A395" s="8"/>
       <c r="B395" s="9"/>
       <c r="C395" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="D395" s="11"/>
+        <v>24</v>
+      </c>
+      <c r="D395" s="18">
+        <v>2.0</v>
+      </c>
       <c r="E395" s="12"/>
       <c r="F395" s="13"/>
       <c r="H395" s="8"/>
@@ -11877,7 +11880,7 @@
       <c r="A396" s="8"/>
       <c r="B396" s="9"/>
       <c r="C396" s="17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D396" s="11"/>
       <c r="E396" s="12"/>
@@ -11901,7 +11904,7 @@
       <c r="A397" s="8"/>
       <c r="B397" s="9"/>
       <c r="C397" s="17" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="D397" s="11"/>
       <c r="E397" s="12"/>
@@ -11925,11 +11928,9 @@
       <c r="A398" s="8"/>
       <c r="B398" s="9"/>
       <c r="C398" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="D398" s="18">
-        <v>1.0</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="D398" s="11"/>
       <c r="E398" s="12"/>
       <c r="F398" s="13"/>
       <c r="H398" s="8"/>
@@ -11950,7 +11951,9 @@
     <row r="399">
       <c r="A399" s="8"/>
       <c r="B399" s="9"/>
-      <c r="C399" s="10"/>
+      <c r="C399" s="17" t="s">
+        <v>41</v>
+      </c>
       <c r="D399" s="11"/>
       <c r="E399" s="12"/>
       <c r="F399" s="13"/>
@@ -11973,21 +11976,15 @@
     </row>
     <row r="400">
       <c r="A400" s="8"/>
-      <c r="B400" s="16" t="s">
-        <v>245</v>
-      </c>
+      <c r="B400" s="9"/>
       <c r="C400" s="17" t="s">
-        <v>241</v>
+        <v>42</v>
       </c>
       <c r="D400" s="18">
-        <v>4.0</v>
-      </c>
-      <c r="E400" s="24" t="s">
-        <v>84</v>
-      </c>
-      <c r="F400" s="25">
-        <v>2.0</v>
-      </c>
+        <v>1.0</v>
+      </c>
+      <c r="E400" s="12"/>
+      <c r="F400" s="13"/>
       <c r="H400" s="8"/>
       <c r="I400" s="19"/>
       <c r="J400" s="27" t="s">
@@ -12008,12 +12005,8 @@
       <c r="B401" s="9"/>
       <c r="C401" s="10"/>
       <c r="D401" s="11"/>
-      <c r="E401" s="24" t="s">
-        <v>177</v>
-      </c>
-      <c r="F401" s="25">
-        <v>2.0</v>
-      </c>
+      <c r="E401" s="12"/>
+      <c r="F401" s="13"/>
       <c r="H401" s="8"/>
       <c r="I401" s="19"/>
       <c r="J401" s="27" t="s">
@@ -12031,18 +12024,20 @@
     </row>
     <row r="402">
       <c r="A402" s="8"/>
-      <c r="B402" s="9"/>
+      <c r="B402" s="16" t="s">
+        <v>245</v>
+      </c>
       <c r="C402" s="17" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D402" s="18">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="E402" s="24" t="s">
-        <v>243</v>
+        <v>84</v>
       </c>
       <c r="F402" s="25">
-        <v>1.5</v>
+        <v>2.0</v>
       </c>
       <c r="H402" s="8"/>
       <c r="I402" s="19"/>
@@ -12067,10 +12062,10 @@
       <c r="C403" s="10"/>
       <c r="D403" s="11"/>
       <c r="E403" s="24" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F403" s="25">
-        <v>1.5</v>
+        <v>2.0</v>
       </c>
       <c r="H403" s="8"/>
       <c r="I403" s="19"/>
@@ -12089,11 +12084,17 @@
       <c r="A404" s="8"/>
       <c r="B404" s="9"/>
       <c r="C404" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="D404" s="11"/>
-      <c r="E404" s="12"/>
-      <c r="F404" s="13"/>
+        <v>242</v>
+      </c>
+      <c r="D404" s="18">
+        <v>3.0</v>
+      </c>
+      <c r="E404" s="24" t="s">
+        <v>243</v>
+      </c>
+      <c r="F404" s="25">
+        <v>1.5</v>
+      </c>
       <c r="H404" s="8"/>
       <c r="I404" s="19" t="s">
         <v>246</v>
@@ -12116,12 +12117,14 @@
     <row r="405">
       <c r="A405" s="8"/>
       <c r="B405" s="9"/>
-      <c r="C405" s="17" t="s">
-        <v>22</v>
-      </c>
+      <c r="C405" s="10"/>
       <c r="D405" s="11"/>
-      <c r="E405" s="12"/>
-      <c r="F405" s="13"/>
+      <c r="E405" s="24" t="s">
+        <v>178</v>
+      </c>
+      <c r="F405" s="25">
+        <v>1.5</v>
+      </c>
       <c r="H405" s="8"/>
       <c r="I405" s="19"/>
       <c r="J405" s="27" t="s">
@@ -12141,7 +12144,7 @@
       <c r="A406" s="8"/>
       <c r="B406" s="9"/>
       <c r="C406" s="17" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="D406" s="11"/>
       <c r="E406" s="12"/>
@@ -12165,7 +12168,7 @@
       <c r="A407" s="8"/>
       <c r="B407" s="9"/>
       <c r="C407" s="17" t="s">
-        <v>51</v>
+        <v>22</v>
       </c>
       <c r="D407" s="11"/>
       <c r="E407" s="12"/>
@@ -12189,15 +12192,11 @@
       <c r="A408" s="8"/>
       <c r="B408" s="9"/>
       <c r="C408" s="17" t="s">
-        <v>220</v>
+        <v>26</v>
       </c>
       <c r="D408" s="11"/>
-      <c r="E408" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="F408" s="25">
-        <v>2.0</v>
-      </c>
+      <c r="E408" s="12"/>
+      <c r="F408" s="13"/>
       <c r="H408" s="8"/>
       <c r="I408" s="19"/>
       <c r="J408" s="27" t="s">
@@ -12218,14 +12217,12 @@
     <row r="409">
       <c r="A409" s="8"/>
       <c r="B409" s="9"/>
-      <c r="C409" s="10"/>
+      <c r="C409" s="17" t="s">
+        <v>51</v>
+      </c>
       <c r="D409" s="11"/>
-      <c r="E409" s="24" t="s">
-        <v>221</v>
-      </c>
-      <c r="F409" s="25">
-        <v>1.0</v>
-      </c>
+      <c r="E409" s="12"/>
+      <c r="F409" s="13"/>
       <c r="H409" s="8"/>
       <c r="I409" s="19"/>
       <c r="J409" s="27" t="s">
@@ -12245,13 +12242,15 @@
       <c r="A410" s="8"/>
       <c r="B410" s="9"/>
       <c r="C410" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="D410" s="18">
+        <v>220</v>
+      </c>
+      <c r="D410" s="11"/>
+      <c r="E410" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="F410" s="25">
         <v>2.0</v>
       </c>
-      <c r="E410" s="12"/>
-      <c r="F410" s="13"/>
       <c r="H410" s="8"/>
       <c r="I410" s="19"/>
       <c r="J410" s="27" t="s">
@@ -12270,12 +12269,14 @@
     <row r="411">
       <c r="A411" s="8"/>
       <c r="B411" s="9"/>
-      <c r="C411" s="17" t="s">
-        <v>39</v>
-      </c>
+      <c r="C411" s="10"/>
       <c r="D411" s="11"/>
-      <c r="E411" s="12"/>
-      <c r="F411" s="13"/>
+      <c r="E411" s="24" t="s">
+        <v>221</v>
+      </c>
+      <c r="F411" s="25">
+        <v>1.0</v>
+      </c>
       <c r="H411" s="8"/>
       <c r="I411" s="19"/>
       <c r="J411" s="27" t="s">
@@ -12297,9 +12298,11 @@
       <c r="A412" s="8"/>
       <c r="B412" s="9"/>
       <c r="C412" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="D412" s="11"/>
+        <v>24</v>
+      </c>
+      <c r="D412" s="18">
+        <v>2.0</v>
+      </c>
       <c r="E412" s="12"/>
       <c r="F412" s="13"/>
       <c r="H412" s="8"/>
@@ -12321,7 +12324,7 @@
       <c r="A413" s="8"/>
       <c r="B413" s="9"/>
       <c r="C413" s="17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D413" s="11"/>
       <c r="E413" s="12"/>
@@ -12345,7 +12348,7 @@
       <c r="A414" s="8"/>
       <c r="B414" s="9"/>
       <c r="C414" s="17" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="D414" s="11"/>
       <c r="E414" s="12"/>
@@ -12369,11 +12372,9 @@
       <c r="A415" s="8"/>
       <c r="B415" s="9"/>
       <c r="C415" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="D415" s="18">
-        <v>1.0</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="D415" s="11"/>
       <c r="E415" s="12"/>
       <c r="F415" s="13"/>
       <c r="H415" s="8"/>
@@ -12396,7 +12397,9 @@
     <row r="416">
       <c r="A416" s="8"/>
       <c r="B416" s="9"/>
-      <c r="C416" s="10"/>
+      <c r="C416" s="17" t="s">
+        <v>41</v>
+      </c>
       <c r="D416" s="11"/>
       <c r="E416" s="12"/>
       <c r="F416" s="13"/>
@@ -12415,20 +12418,18 @@
     </row>
     <row r="417">
       <c r="A417" s="8"/>
-      <c r="B417" s="16" t="s">
-        <v>248</v>
-      </c>
+      <c r="B417" s="9"/>
       <c r="C417" s="17" t="s">
-        <v>95</v>
+        <v>42</v>
       </c>
       <c r="D417" s="18">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
       <c r="E417" s="12"/>
       <c r="F417" s="13"/>
       <c r="H417" s="8"/>
       <c r="I417" s="19" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="J417" s="27" t="s">
         <v>62</v>
@@ -12448,12 +12449,8 @@
     <row r="418">
       <c r="A418" s="8"/>
       <c r="B418" s="9"/>
-      <c r="C418" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="D418" s="18">
-        <v>3.0</v>
-      </c>
+      <c r="C418" s="10"/>
+      <c r="D418" s="11"/>
       <c r="E418" s="12"/>
       <c r="F418" s="13"/>
       <c r="H418" s="8"/>
@@ -12473,11 +12470,15 @@
     </row>
     <row r="419">
       <c r="A419" s="8"/>
-      <c r="B419" s="9"/>
+      <c r="B419" s="16" t="s">
+        <v>249</v>
+      </c>
       <c r="C419" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="D419" s="11"/>
+        <v>95</v>
+      </c>
+      <c r="D419" s="18">
+        <v>4.0</v>
+      </c>
       <c r="E419" s="12"/>
       <c r="F419" s="13"/>
       <c r="H419" s="8"/>
@@ -12499,9 +12500,11 @@
       <c r="A420" s="8"/>
       <c r="B420" s="9"/>
       <c r="C420" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="D420" s="11"/>
+        <v>97</v>
+      </c>
+      <c r="D420" s="18">
+        <v>3.0</v>
+      </c>
       <c r="E420" s="12"/>
       <c r="F420" s="13"/>
       <c r="H420" s="8"/>
@@ -12523,7 +12526,7 @@
       <c r="A421" s="8"/>
       <c r="B421" s="9"/>
       <c r="C421" s="17" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="D421" s="11"/>
       <c r="E421" s="12"/>
@@ -12549,15 +12552,11 @@
       <c r="A422" s="8"/>
       <c r="B422" s="9"/>
       <c r="C422" s="17" t="s">
-        <v>220</v>
+        <v>22</v>
       </c>
       <c r="D422" s="11"/>
-      <c r="E422" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="F422" s="25">
-        <v>2.0</v>
-      </c>
+      <c r="E422" s="12"/>
+      <c r="F422" s="13"/>
       <c r="H422" s="8"/>
       <c r="I422" s="19"/>
       <c r="J422" s="27" t="s">
@@ -12576,14 +12575,12 @@
     <row r="423">
       <c r="A423" s="8"/>
       <c r="B423" s="9"/>
-      <c r="C423" s="10"/>
+      <c r="C423" s="17" t="s">
+        <v>26</v>
+      </c>
       <c r="D423" s="11"/>
-      <c r="E423" s="24" t="s">
-        <v>221</v>
-      </c>
-      <c r="F423" s="25">
-        <v>1.0</v>
-      </c>
+      <c r="E423" s="12"/>
+      <c r="F423" s="13"/>
       <c r="H423" s="8"/>
       <c r="I423" s="19"/>
       <c r="J423" s="27" t="s">
@@ -12603,13 +12600,15 @@
       <c r="A424" s="8"/>
       <c r="B424" s="9"/>
       <c r="C424" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="D424" s="18">
+        <v>220</v>
+      </c>
+      <c r="D424" s="11"/>
+      <c r="E424" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="F424" s="25">
         <v>2.0</v>
       </c>
-      <c r="E424" s="12"/>
-      <c r="F424" s="13"/>
       <c r="H424" s="8"/>
       <c r="I424" s="19"/>
       <c r="J424" s="27" t="s">
@@ -12630,12 +12629,14 @@
     <row r="425">
       <c r="A425" s="8"/>
       <c r="B425" s="9"/>
-      <c r="C425" s="17" t="s">
-        <v>39</v>
-      </c>
+      <c r="C425" s="10"/>
       <c r="D425" s="11"/>
-      <c r="E425" s="12"/>
-      <c r="F425" s="13"/>
+      <c r="E425" s="24" t="s">
+        <v>221</v>
+      </c>
+      <c r="F425" s="25">
+        <v>1.0</v>
+      </c>
       <c r="H425" s="8"/>
       <c r="I425" s="19"/>
       <c r="J425" s="20" t="s">
@@ -12655,9 +12656,11 @@
       <c r="A426" s="8"/>
       <c r="B426" s="9"/>
       <c r="C426" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="D426" s="11"/>
+        <v>24</v>
+      </c>
+      <c r="D426" s="18">
+        <v>2.0</v>
+      </c>
       <c r="E426" s="12"/>
       <c r="F426" s="13"/>
       <c r="H426" s="8"/>
@@ -12679,7 +12682,7 @@
       <c r="A427" s="8"/>
       <c r="B427" s="9"/>
       <c r="C427" s="17" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D427" s="11"/>
       <c r="E427" s="12"/>
@@ -12703,7 +12706,7 @@
       <c r="A428" s="8"/>
       <c r="B428" s="9"/>
       <c r="C428" s="17" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="D428" s="11"/>
       <c r="E428" s="12"/>
@@ -12729,11 +12732,9 @@
       <c r="A429" s="8"/>
       <c r="B429" s="9"/>
       <c r="C429" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="D429" s="18">
-        <v>1.0</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="D429" s="11"/>
       <c r="E429" s="12"/>
       <c r="F429" s="13"/>
       <c r="H429" s="8"/>
@@ -12752,7 +12753,9 @@
     <row r="430">
       <c r="A430" s="8"/>
       <c r="B430" s="9"/>
-      <c r="C430" s="10"/>
+      <c r="C430" s="17" t="s">
+        <v>41</v>
+      </c>
       <c r="D430" s="11"/>
       <c r="E430" s="12"/>
       <c r="F430" s="13"/>
@@ -12777,14 +12780,12 @@
     </row>
     <row r="431">
       <c r="A431" s="8"/>
-      <c r="B431" s="16" t="s">
-        <v>251</v>
-      </c>
+      <c r="B431" s="9"/>
       <c r="C431" s="17" t="s">
-        <v>95</v>
+        <v>42</v>
       </c>
       <c r="D431" s="18">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
       <c r="E431" s="12"/>
       <c r="F431" s="13"/>
@@ -12806,12 +12807,8 @@
     <row r="432">
       <c r="A432" s="8"/>
       <c r="B432" s="9"/>
-      <c r="C432" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="D432" s="18">
-        <v>3.0</v>
-      </c>
+      <c r="C432" s="10"/>
+      <c r="D432" s="11"/>
       <c r="E432" s="12"/>
       <c r="F432" s="13"/>
       <c r="H432" s="8"/>
@@ -12831,11 +12828,15 @@
     </row>
     <row r="433">
       <c r="A433" s="8"/>
-      <c r="B433" s="9"/>
+      <c r="B433" s="16" t="s">
+        <v>251</v>
+      </c>
       <c r="C433" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="D433" s="11"/>
+        <v>95</v>
+      </c>
+      <c r="D433" s="18">
+        <v>4.0</v>
+      </c>
       <c r="E433" s="12"/>
       <c r="F433" s="13"/>
       <c r="H433" s="8"/>
@@ -12857,9 +12858,11 @@
       <c r="A434" s="8"/>
       <c r="B434" s="9"/>
       <c r="C434" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="D434" s="11"/>
+        <v>97</v>
+      </c>
+      <c r="D434" s="18">
+        <v>3.0</v>
+      </c>
       <c r="E434" s="12"/>
       <c r="F434" s="13"/>
       <c r="H434" s="8"/>
@@ -12883,7 +12886,7 @@
       <c r="A435" s="8"/>
       <c r="B435" s="9"/>
       <c r="C435" s="17" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="D435" s="11"/>
       <c r="E435" s="12"/>
@@ -12907,7 +12910,7 @@
       <c r="A436" s="8"/>
       <c r="B436" s="9"/>
       <c r="C436" s="17" t="s">
-        <v>51</v>
+        <v>22</v>
       </c>
       <c r="D436" s="11"/>
       <c r="E436" s="12"/>
@@ -12931,15 +12934,11 @@
       <c r="A437" s="8"/>
       <c r="B437" s="9"/>
       <c r="C437" s="17" t="s">
-        <v>220</v>
+        <v>26</v>
       </c>
       <c r="D437" s="11"/>
-      <c r="E437" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="F437" s="25">
-        <v>2.0</v>
-      </c>
+      <c r="E437" s="12"/>
+      <c r="F437" s="13"/>
       <c r="H437" s="8"/>
       <c r="I437" s="19"/>
       <c r="J437" s="27" t="s">
@@ -12958,14 +12957,12 @@
     <row r="438">
       <c r="A438" s="8"/>
       <c r="B438" s="9"/>
-      <c r="C438" s="10"/>
+      <c r="C438" s="17" t="s">
+        <v>51</v>
+      </c>
       <c r="D438" s="11"/>
-      <c r="E438" s="24" t="s">
-        <v>221</v>
-      </c>
-      <c r="F438" s="25">
-        <v>1.0</v>
-      </c>
+      <c r="E438" s="12"/>
+      <c r="F438" s="13"/>
       <c r="H438" s="8"/>
       <c r="I438" s="19"/>
       <c r="J438" s="20" t="s">
@@ -12987,13 +12984,15 @@
       <c r="A439" s="8"/>
       <c r="B439" s="9"/>
       <c r="C439" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="D439" s="18">
+        <v>220</v>
+      </c>
+      <c r="D439" s="11"/>
+      <c r="E439" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="F439" s="25">
         <v>2.0</v>
       </c>
-      <c r="E439" s="12"/>
-      <c r="F439" s="13"/>
       <c r="H439" s="8"/>
       <c r="I439" s="33"/>
       <c r="J439" s="27" t="s">
@@ -13012,12 +13011,14 @@
     <row r="440">
       <c r="A440" s="8"/>
       <c r="B440" s="9"/>
-      <c r="C440" s="17" t="s">
-        <v>39</v>
-      </c>
+      <c r="C440" s="10"/>
       <c r="D440" s="11"/>
-      <c r="E440" s="12"/>
-      <c r="F440" s="13"/>
+      <c r="E440" s="24" t="s">
+        <v>221</v>
+      </c>
+      <c r="F440" s="25">
+        <v>1.0</v>
+      </c>
       <c r="H440" s="8"/>
       <c r="I440" s="19"/>
       <c r="J440" s="27" t="s">
@@ -13037,9 +13038,11 @@
       <c r="A441" s="8"/>
       <c r="B441" s="9"/>
       <c r="C441" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="D441" s="11"/>
+        <v>24</v>
+      </c>
+      <c r="D441" s="18">
+        <v>2.0</v>
+      </c>
       <c r="E441" s="12"/>
       <c r="F441" s="13"/>
       <c r="H441" s="8"/>
@@ -13063,7 +13066,7 @@
       <c r="A442" s="8"/>
       <c r="B442" s="9"/>
       <c r="C442" s="17" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D442" s="11"/>
       <c r="E442" s="12"/>
@@ -13085,7 +13088,7 @@
       <c r="A443" s="8"/>
       <c r="B443" s="9"/>
       <c r="C443" s="17" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="D443" s="11"/>
       <c r="E443" s="12"/>
@@ -13113,11 +13116,9 @@
       <c r="A444" s="8"/>
       <c r="B444" s="9"/>
       <c r="C444" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="D444" s="18">
-        <v>1.0</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="D444" s="11"/>
       <c r="E444" s="12"/>
       <c r="F444" s="13"/>
       <c r="H444" s="8"/>
@@ -13140,7 +13141,9 @@
     <row r="445">
       <c r="A445" s="8"/>
       <c r="B445" s="9"/>
-      <c r="C445" s="10"/>
+      <c r="C445" s="17" t="s">
+        <v>41</v>
+      </c>
       <c r="D445" s="11"/>
       <c r="E445" s="12"/>
       <c r="F445" s="13"/>
@@ -13161,14 +13164,12 @@
     </row>
     <row r="446">
       <c r="A446" s="8"/>
-      <c r="B446" s="16" t="s">
-        <v>253</v>
-      </c>
+      <c r="B446" s="9"/>
       <c r="C446" s="17" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D446" s="18">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
       <c r="E446" s="12"/>
       <c r="F446" s="13"/>
@@ -13190,12 +13191,8 @@
     <row r="447">
       <c r="A447" s="8"/>
       <c r="B447" s="9"/>
-      <c r="C447" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="D447" s="18">
-        <v>3.0</v>
-      </c>
+      <c r="C447" s="10"/>
+      <c r="D447" s="11"/>
       <c r="E447" s="12"/>
       <c r="F447" s="13"/>
       <c r="H447" s="8"/>
@@ -13215,11 +13212,15 @@
     </row>
     <row r="448">
       <c r="A448" s="8"/>
-      <c r="B448" s="9"/>
+      <c r="B448" s="16" t="s">
+        <v>253</v>
+      </c>
       <c r="C448" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="D448" s="11"/>
+        <v>39</v>
+      </c>
+      <c r="D448" s="18">
+        <v>4.0</v>
+      </c>
       <c r="E448" s="12"/>
       <c r="F448" s="13"/>
       <c r="H448" s="8"/>
@@ -13241,9 +13242,11 @@
       <c r="A449" s="8"/>
       <c r="B449" s="9"/>
       <c r="C449" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="D449" s="11"/>
+        <v>68</v>
+      </c>
+      <c r="D449" s="18">
+        <v>3.0</v>
+      </c>
       <c r="E449" s="12"/>
       <c r="F449" s="13"/>
       <c r="H449" s="8"/>
@@ -13265,15 +13268,11 @@
       <c r="A450" s="8"/>
       <c r="B450" s="9"/>
       <c r="C450" s="17" t="s">
-        <v>220</v>
+        <v>22</v>
       </c>
       <c r="D450" s="11"/>
-      <c r="E450" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="F450" s="25">
-        <v>2.0</v>
-      </c>
+      <c r="E450" s="12"/>
+      <c r="F450" s="13"/>
       <c r="H450" s="8"/>
       <c r="I450" s="19"/>
       <c r="J450" s="27" t="s">
@@ -13292,14 +13291,12 @@
     <row r="451">
       <c r="A451" s="8"/>
       <c r="B451" s="9"/>
-      <c r="C451" s="10"/>
+      <c r="C451" s="17" t="s">
+        <v>26</v>
+      </c>
       <c r="D451" s="11"/>
-      <c r="E451" s="24" t="s">
-        <v>221</v>
-      </c>
-      <c r="F451" s="25">
-        <v>1.0</v>
-      </c>
+      <c r="E451" s="12"/>
+      <c r="F451" s="13"/>
       <c r="H451" s="8"/>
       <c r="I451" s="19"/>
       <c r="J451" s="27" t="s">
@@ -13321,13 +13318,15 @@
       <c r="A452" s="8"/>
       <c r="B452" s="9"/>
       <c r="C452" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="D452" s="18">
+        <v>220</v>
+      </c>
+      <c r="D452" s="11"/>
+      <c r="E452" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="F452" s="25">
         <v>2.0</v>
       </c>
-      <c r="E452" s="12"/>
-      <c r="F452" s="13"/>
       <c r="H452" s="8"/>
       <c r="I452" s="19"/>
       <c r="J452" s="27" t="s">
@@ -13346,12 +13345,14 @@
     <row r="453">
       <c r="A453" s="8"/>
       <c r="B453" s="9"/>
-      <c r="C453" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="D453" s="18"/>
-      <c r="E453" s="12"/>
-      <c r="F453" s="13"/>
+      <c r="C453" s="10"/>
+      <c r="D453" s="11"/>
+      <c r="E453" s="24" t="s">
+        <v>221</v>
+      </c>
+      <c r="F453" s="25">
+        <v>1.0</v>
+      </c>
       <c r="H453" s="8"/>
       <c r="I453" s="19"/>
       <c r="J453" s="20" t="s">
@@ -13371,9 +13372,11 @@
       <c r="A454" s="8"/>
       <c r="B454" s="9"/>
       <c r="C454" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="D454" s="18"/>
+        <v>67</v>
+      </c>
+      <c r="D454" s="18">
+        <v>2.0</v>
+      </c>
       <c r="E454" s="12"/>
       <c r="F454" s="13"/>
       <c r="H454" s="8"/>
@@ -13395,7 +13398,7 @@
       <c r="A455" s="8"/>
       <c r="B455" s="9"/>
       <c r="C455" s="17" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="D455" s="18"/>
       <c r="E455" s="12"/>
@@ -13421,7 +13424,7 @@
       <c r="A456" s="8"/>
       <c r="B456" s="9"/>
       <c r="C456" s="17" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="D456" s="18"/>
       <c r="E456" s="12"/>
@@ -13443,7 +13446,7 @@
       <c r="A457" s="8"/>
       <c r="B457" s="9"/>
       <c r="C457" s="17" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D457" s="18"/>
       <c r="E457" s="12"/>
@@ -13471,7 +13474,7 @@
       <c r="A458" s="8"/>
       <c r="B458" s="9"/>
       <c r="C458" s="17" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D458" s="18"/>
       <c r="E458" s="12"/>
@@ -13497,11 +13500,9 @@
       <c r="A459" s="8"/>
       <c r="B459" s="9"/>
       <c r="C459" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="D459" s="18">
-        <v>1.0</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="D459" s="18"/>
       <c r="E459" s="12"/>
       <c r="F459" s="13"/>
       <c r="H459" s="8"/>
@@ -13521,11 +13522,13 @@
     </row>
     <row r="460">
       <c r="A460" s="8"/>
-      <c r="B460" s="19"/>
-      <c r="C460" s="20"/>
-      <c r="D460" s="26"/>
-      <c r="E460" s="22"/>
-      <c r="F460" s="23"/>
+      <c r="B460" s="9"/>
+      <c r="C460" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="D460" s="18"/>
+      <c r="E460" s="12"/>
+      <c r="F460" s="13"/>
       <c r="H460" s="8"/>
       <c r="I460" s="19"/>
       <c r="J460" s="27" t="s">
@@ -13543,17 +13546,15 @@
     </row>
     <row r="461">
       <c r="A461" s="8"/>
-      <c r="B461" s="32" t="s">
-        <v>256</v>
-      </c>
-      <c r="C461" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="D461" s="21">
-        <v>4.0</v>
-      </c>
-      <c r="E461" s="22"/>
-      <c r="F461" s="23"/>
+      <c r="B461" s="9"/>
+      <c r="C461" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="D461" s="18">
+        <v>1.0</v>
+      </c>
+      <c r="E461" s="12"/>
+      <c r="F461" s="13"/>
       <c r="H461" s="8"/>
       <c r="I461" s="19"/>
       <c r="J461" s="27" t="s">
@@ -13572,12 +13573,8 @@
     <row r="462">
       <c r="A462" s="8"/>
       <c r="B462" s="19"/>
-      <c r="C462" s="20" t="s">
-        <v>68</v>
-      </c>
-      <c r="D462" s="21">
-        <v>3.0</v>
-      </c>
+      <c r="C462" s="20"/>
+      <c r="D462" s="26"/>
       <c r="E462" s="22"/>
       <c r="F462" s="23"/>
       <c r="H462" s="8"/>
@@ -13597,11 +13594,15 @@
     </row>
     <row r="463">
       <c r="A463" s="8"/>
-      <c r="B463" s="19"/>
+      <c r="B463" s="32" t="s">
+        <v>256</v>
+      </c>
       <c r="C463" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="D463" s="26"/>
+        <v>39</v>
+      </c>
+      <c r="D463" s="21">
+        <v>4.0</v>
+      </c>
       <c r="E463" s="22"/>
       <c r="F463" s="23"/>
       <c r="H463" s="8"/>
@@ -13623,9 +13624,11 @@
       <c r="A464" s="8"/>
       <c r="B464" s="19"/>
       <c r="C464" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="D464" s="26"/>
+        <v>68</v>
+      </c>
+      <c r="D464" s="21">
+        <v>3.0</v>
+      </c>
       <c r="E464" s="22"/>
       <c r="F464" s="23"/>
       <c r="H464" s="8"/>
@@ -13646,8 +13649,8 @@
     <row r="465">
       <c r="A465" s="8"/>
       <c r="B465" s="19"/>
-      <c r="C465" s="35" t="s">
-        <v>51</v>
+      <c r="C465" s="20" t="s">
+        <v>22</v>
       </c>
       <c r="D465" s="26"/>
       <c r="E465" s="22"/>
@@ -13673,15 +13676,11 @@
       <c r="A466" s="8"/>
       <c r="B466" s="19"/>
       <c r="C466" s="20" t="s">
-        <v>220</v>
+        <v>26</v>
       </c>
       <c r="D466" s="26"/>
-      <c r="E466" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="F466" s="30">
-        <v>2.0</v>
-      </c>
+      <c r="E466" s="22"/>
+      <c r="F466" s="23"/>
       <c r="H466" s="8"/>
       <c r="I466" s="19"/>
       <c r="J466" s="27" t="s">
@@ -13700,14 +13699,12 @@
     <row r="467">
       <c r="A467" s="8"/>
       <c r="B467" s="19"/>
-      <c r="C467" s="20"/>
+      <c r="C467" s="35" t="s">
+        <v>51</v>
+      </c>
       <c r="D467" s="26"/>
-      <c r="E467" s="22" t="s">
-        <v>221</v>
-      </c>
-      <c r="F467" s="30">
-        <v>1.0</v>
-      </c>
+      <c r="E467" s="22"/>
+      <c r="F467" s="23"/>
       <c r="H467" s="8"/>
       <c r="I467" s="19"/>
       <c r="J467" s="27" t="s">
@@ -13727,13 +13724,15 @@
       <c r="A468" s="8"/>
       <c r="B468" s="19"/>
       <c r="C468" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="D468" s="21">
+        <v>220</v>
+      </c>
+      <c r="D468" s="26"/>
+      <c r="E468" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="F468" s="30">
         <v>2.0</v>
       </c>
-      <c r="E468" s="22"/>
-      <c r="F468" s="23"/>
       <c r="H468" s="8"/>
       <c r="I468" s="19"/>
       <c r="J468" s="20" t="s">
@@ -13752,12 +13751,14 @@
     <row r="469">
       <c r="A469" s="8"/>
       <c r="B469" s="19"/>
-      <c r="C469" s="20" t="s">
-        <v>34</v>
-      </c>
+      <c r="C469" s="20"/>
       <c r="D469" s="26"/>
-      <c r="E469" s="22"/>
-      <c r="F469" s="23"/>
+      <c r="E469" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="F469" s="30">
+        <v>1.0</v>
+      </c>
       <c r="H469" s="8"/>
       <c r="I469" s="33"/>
       <c r="J469" s="27" t="s">
@@ -13779,9 +13780,11 @@
       <c r="A470" s="8"/>
       <c r="B470" s="19"/>
       <c r="C470" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="D470" s="26"/>
+        <v>67</v>
+      </c>
+      <c r="D470" s="21">
+        <v>2.0</v>
+      </c>
       <c r="E470" s="22"/>
       <c r="F470" s="23"/>
       <c r="H470" s="8"/>
@@ -13801,7 +13804,7 @@
       <c r="A471" s="8"/>
       <c r="B471" s="19"/>
       <c r="C471" s="20" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="D471" s="26"/>
       <c r="E471" s="22"/>
@@ -13829,7 +13832,7 @@
       <c r="A472" s="8"/>
       <c r="B472" s="19"/>
       <c r="C472" s="20" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="D472" s="26"/>
       <c r="E472" s="22"/>
@@ -13853,7 +13856,7 @@
       <c r="A473" s="8"/>
       <c r="B473" s="19"/>
       <c r="C473" s="20" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D473" s="26"/>
       <c r="E473" s="22"/>
@@ -13879,7 +13882,7 @@
       <c r="A474" s="8"/>
       <c r="B474" s="19"/>
       <c r="C474" s="20" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D474" s="26"/>
       <c r="E474" s="22"/>
@@ -13903,11 +13906,9 @@
       <c r="A475" s="8"/>
       <c r="B475" s="19"/>
       <c r="C475" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="D475" s="21">
-        <v>1.0</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="D475" s="26"/>
       <c r="E475" s="22"/>
       <c r="F475" s="23"/>
       <c r="H475" s="8"/>
@@ -13927,11 +13928,13 @@
     </row>
     <row r="476">
       <c r="A476" s="8"/>
-      <c r="B476" s="9"/>
-      <c r="C476" s="10"/>
-      <c r="D476" s="11"/>
-      <c r="E476" s="12"/>
-      <c r="F476" s="13"/>
+      <c r="B476" s="19"/>
+      <c r="C476" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D476" s="26"/>
+      <c r="E476" s="22"/>
+      <c r="F476" s="23"/>
       <c r="H476" s="8"/>
       <c r="I476" s="19"/>
       <c r="J476" s="27" t="s">
@@ -13949,11 +13952,15 @@
     </row>
     <row r="477">
       <c r="A477" s="8"/>
-      <c r="B477" s="9"/>
-      <c r="C477" s="17"/>
-      <c r="D477" s="11"/>
-      <c r="E477" s="12"/>
-      <c r="F477" s="13"/>
+      <c r="B477" s="19"/>
+      <c r="C477" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="D477" s="21">
+        <v>1.0</v>
+      </c>
+      <c r="E477" s="22"/>
+      <c r="F477" s="23"/>
       <c r="H477" s="8"/>
       <c r="I477" s="19"/>
       <c r="J477" s="34" t="s">

</xml_diff>

<commit_message>
Added section i and wrote down how to update classes
</commit_message>
<xml_diff>
--- a/assets/All Classes.xlsx
+++ b/assets/All Classes.xlsx
@@ -11,26 +11,26 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1280" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1320" uniqueCount="272">
+  <si>
+    <t>ClassNames</t>
+  </si>
+  <si>
+    <t>SubjectName</t>
+  </si>
+  <si>
+    <t>SubjectCoef</t>
+  </si>
+  <si>
+    <t>CombiName</t>
+  </si>
+  <si>
+    <t>CombiCoef</t>
+  </si>
   <si>
     <t>Macros</t>
   </si>
   <si>
-    <t>ClassNames</t>
-  </si>
-  <si>
-    <t>SubjectName</t>
-  </si>
-  <si>
-    <t>SubjectCoef</t>
-  </si>
-  <si>
-    <t>CombiName</t>
-  </si>
-  <si>
-    <t>CombiCoef</t>
-  </si>
-  <si>
     <t>skipped class</t>
   </si>
   <si>
@@ -658,12 +658,36 @@
     <t>ConProf 1</t>
   </si>
   <si>
+    <t>1I</t>
+  </si>
+  <si>
+    <t>Mathé 1</t>
+  </si>
+  <si>
     <t>ConProf 2</t>
   </si>
   <si>
+    <t>Mathé 2</t>
+  </si>
+  <si>
+    <t>Média</t>
+  </si>
+  <si>
+    <t>Pogrammation</t>
+  </si>
+  <si>
+    <t>AmInf</t>
+  </si>
+  <si>
+    <t>MaiOuv</t>
+  </si>
+  <si>
     <t>ConSci</t>
   </si>
   <si>
+    <t>EduPys</t>
+  </si>
+  <si>
     <t>2GSH</t>
   </si>
   <si>
@@ -785,6 +809,24 @@
   </si>
   <si>
     <t>2GACV</t>
+  </si>
+  <si>
+    <t>3I</t>
+  </si>
+  <si>
+    <t>Programmation</t>
+  </si>
+  <si>
+    <t>Design graphique</t>
+  </si>
+  <si>
+    <t>TechIn</t>
+  </si>
+  <si>
+    <t>ComMed</t>
+  </si>
+  <si>
+    <t>2I</t>
   </si>
 </sst>
 </file>
@@ -1038,59 +1080,57 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="1"/>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="M1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="O1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="R1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="S1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="T1" s="6" t="s">
         <v>4</v>
-      </c>
-      <c r="T1" s="6" t="s">
-        <v>5</v>
       </c>
       <c r="V1" s="7" t="s">
         <v>6</v>
@@ -8296,11 +8336,21 @@
       <c r="L256" s="22"/>
       <c r="M256" s="23"/>
       <c r="O256" s="8"/>
-      <c r="P256" s="9"/>
-      <c r="Q256" s="10"/>
-      <c r="R256" s="11"/>
-      <c r="S256" s="12"/>
-      <c r="T256" s="13"/>
+      <c r="P256" s="19" t="s">
+        <v>215</v>
+      </c>
+      <c r="Q256" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="R256" s="21">
+        <v>3.0</v>
+      </c>
+      <c r="S256" s="22" t="s">
+        <v>216</v>
+      </c>
+      <c r="T256" s="30">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="257">
       <c r="A257" s="8"/>
@@ -8314,17 +8364,21 @@
       <c r="H257" s="8"/>
       <c r="I257" s="19"/>
       <c r="J257" s="27" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="K257" s="26"/>
       <c r="L257" s="22"/>
       <c r="M257" s="23"/>
       <c r="O257" s="8"/>
-      <c r="P257" s="9"/>
-      <c r="Q257" s="10"/>
-      <c r="R257" s="11"/>
-      <c r="S257" s="12"/>
-      <c r="T257" s="13"/>
+      <c r="P257" s="19"/>
+      <c r="Q257" s="20"/>
+      <c r="R257" s="26"/>
+      <c r="S257" s="22" t="s">
+        <v>218</v>
+      </c>
+      <c r="T257" s="30">
+        <v>2.0</v>
+      </c>
     </row>
     <row r="258">
       <c r="A258" s="8"/>
@@ -8346,11 +8400,13 @@
       <c r="L258" s="22"/>
       <c r="M258" s="23"/>
       <c r="O258" s="8"/>
-      <c r="P258" s="9"/>
-      <c r="Q258" s="10"/>
-      <c r="R258" s="11"/>
-      <c r="S258" s="12"/>
-      <c r="T258" s="13"/>
+      <c r="P258" s="19"/>
+      <c r="Q258" s="20" t="s">
+        <v>219</v>
+      </c>
+      <c r="R258" s="26"/>
+      <c r="S258" s="22"/>
+      <c r="T258" s="23"/>
     </row>
     <row r="259">
       <c r="A259" s="8"/>
@@ -8370,11 +8426,13 @@
       <c r="L259" s="22"/>
       <c r="M259" s="23"/>
       <c r="O259" s="8"/>
-      <c r="P259" s="9"/>
-      <c r="Q259" s="10"/>
-      <c r="R259" s="11"/>
-      <c r="S259" s="12"/>
-      <c r="T259" s="13"/>
+      <c r="P259" s="19"/>
+      <c r="Q259" s="20" t="s">
+        <v>220</v>
+      </c>
+      <c r="R259" s="26"/>
+      <c r="S259" s="22"/>
+      <c r="T259" s="23"/>
     </row>
     <row r="260">
       <c r="A260" s="8"/>
@@ -8394,11 +8452,13 @@
       <c r="L260" s="22"/>
       <c r="M260" s="23"/>
       <c r="O260" s="8"/>
-      <c r="P260" s="9"/>
-      <c r="Q260" s="10"/>
-      <c r="R260" s="11"/>
-      <c r="S260" s="12"/>
-      <c r="T260" s="13"/>
+      <c r="P260" s="19"/>
+      <c r="Q260" s="20" t="s">
+        <v>221</v>
+      </c>
+      <c r="R260" s="26"/>
+      <c r="S260" s="22"/>
+      <c r="T260" s="23"/>
     </row>
     <row r="261">
       <c r="A261" s="8"/>
@@ -8418,11 +8478,15 @@
       <c r="L261" s="22"/>
       <c r="M261" s="23"/>
       <c r="O261" s="8"/>
-      <c r="P261" s="9"/>
-      <c r="Q261" s="10"/>
-      <c r="R261" s="11"/>
-      <c r="S261" s="12"/>
-      <c r="T261" s="13"/>
+      <c r="P261" s="19"/>
+      <c r="Q261" s="20" t="s">
+        <v>222</v>
+      </c>
+      <c r="R261" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="S261" s="22"/>
+      <c r="T261" s="23"/>
     </row>
     <row r="262">
       <c r="A262" s="8"/>
@@ -8444,11 +8508,13 @@
       <c r="L262" s="22"/>
       <c r="M262" s="23"/>
       <c r="O262" s="8"/>
-      <c r="P262" s="9"/>
-      <c r="Q262" s="10"/>
-      <c r="R262" s="11"/>
-      <c r="S262" s="12"/>
-      <c r="T262" s="13"/>
+      <c r="P262" s="19"/>
+      <c r="Q262" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="R262" s="26"/>
+      <c r="S262" s="22"/>
+      <c r="T262" s="23"/>
     </row>
     <row r="263">
       <c r="A263" s="8"/>
@@ -8468,11 +8534,13 @@
       <c r="L263" s="22"/>
       <c r="M263" s="23"/>
       <c r="O263" s="8"/>
-      <c r="P263" s="9"/>
-      <c r="Q263" s="10"/>
-      <c r="R263" s="11"/>
-      <c r="S263" s="12"/>
-      <c r="T263" s="13"/>
+      <c r="P263" s="19"/>
+      <c r="Q263" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="R263" s="26"/>
+      <c r="S263" s="22"/>
+      <c r="T263" s="23"/>
     </row>
     <row r="264">
       <c r="A264" s="8"/>
@@ -8492,11 +8560,13 @@
       <c r="L264" s="22"/>
       <c r="M264" s="23"/>
       <c r="O264" s="8"/>
-      <c r="P264" s="9"/>
-      <c r="Q264" s="10"/>
-      <c r="R264" s="11"/>
-      <c r="S264" s="12"/>
-      <c r="T264" s="13"/>
+      <c r="P264" s="19"/>
+      <c r="Q264" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="R264" s="26"/>
+      <c r="S264" s="22"/>
+      <c r="T264" s="23"/>
     </row>
     <row r="265">
       <c r="A265" s="8"/>
@@ -8510,17 +8580,21 @@
       <c r="H265" s="8"/>
       <c r="I265" s="19"/>
       <c r="J265" s="27" t="s">
-        <v>216</v>
+        <v>223</v>
       </c>
       <c r="K265" s="28"/>
       <c r="L265" s="22"/>
       <c r="M265" s="23"/>
       <c r="O265" s="8"/>
-      <c r="P265" s="9"/>
-      <c r="Q265" s="10"/>
-      <c r="R265" s="11"/>
-      <c r="S265" s="12"/>
-      <c r="T265" s="13"/>
+      <c r="P265" s="19"/>
+      <c r="Q265" s="20" t="s">
+        <v>224</v>
+      </c>
+      <c r="R265" s="21">
+        <v>1.0</v>
+      </c>
+      <c r="S265" s="22"/>
+      <c r="T265" s="23"/>
     </row>
     <row r="266">
       <c r="A266" s="8"/>
@@ -8585,7 +8659,7 @@
       <c r="F268" s="13"/>
       <c r="H268" s="8"/>
       <c r="I268" s="19" t="s">
-        <v>217</v>
+        <v>225</v>
       </c>
       <c r="J268" s="27" t="s">
         <v>140</v>
@@ -8933,7 +9007,7 @@
       <c r="F282" s="13"/>
       <c r="H282" s="8"/>
       <c r="I282" s="19" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="J282" s="27" t="s">
         <v>106</v>
@@ -8953,7 +9027,7 @@
     <row r="283">
       <c r="A283" s="8"/>
       <c r="B283" s="16" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
       <c r="C283" s="17" t="s">
         <v>13</v>
@@ -9058,7 +9132,7 @@
       <c r="A287" s="8"/>
       <c r="B287" s="9"/>
       <c r="C287" s="17" t="s">
-        <v>220</v>
+        <v>228</v>
       </c>
       <c r="D287" s="18"/>
       <c r="E287" s="24" t="s">
@@ -9088,7 +9162,7 @@
       <c r="C288" s="17"/>
       <c r="D288" s="18"/>
       <c r="E288" s="24" t="s">
-        <v>221</v>
+        <v>229</v>
       </c>
       <c r="F288" s="25">
         <v>1.0</v>
@@ -9261,7 +9335,7 @@
     <row r="295">
       <c r="A295" s="8"/>
       <c r="B295" s="16" t="s">
-        <v>222</v>
+        <v>230</v>
       </c>
       <c r="C295" s="17" t="s">
         <v>13</v>
@@ -9295,7 +9369,7 @@
       <c r="F296" s="13"/>
       <c r="H296" s="8"/>
       <c r="I296" s="19" t="s">
-        <v>223</v>
+        <v>231</v>
       </c>
       <c r="J296" s="27" t="s">
         <v>106</v>
@@ -9392,7 +9466,7 @@
       <c r="A300" s="8"/>
       <c r="B300" s="9"/>
       <c r="C300" s="17" t="s">
-        <v>220</v>
+        <v>228</v>
       </c>
       <c r="D300" s="18"/>
       <c r="E300" s="24" t="s">
@@ -9422,7 +9496,7 @@
       <c r="C301" s="17"/>
       <c r="D301" s="18"/>
       <c r="E301" s="24" t="s">
-        <v>221</v>
+        <v>229</v>
       </c>
       <c r="F301" s="25">
         <v>1.0</v>
@@ -9569,7 +9643,7 @@
     <row r="307">
       <c r="A307" s="8"/>
       <c r="B307" s="16" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="C307" s="17" t="s">
         <v>46</v>
@@ -9637,7 +9711,7 @@
       <c r="F309" s="13"/>
       <c r="H309" s="8"/>
       <c r="I309" s="19" t="s">
-        <v>225</v>
+        <v>233</v>
       </c>
       <c r="J309" s="27" t="s">
         <v>26</v>
@@ -9730,7 +9804,7 @@
       <c r="A313" s="8"/>
       <c r="B313" s="9"/>
       <c r="C313" s="17" t="s">
-        <v>220</v>
+        <v>228</v>
       </c>
       <c r="D313" s="11"/>
       <c r="E313" s="24" t="s">
@@ -9760,7 +9834,7 @@
       <c r="C314" s="10"/>
       <c r="D314" s="11"/>
       <c r="E314" s="24" t="s">
-        <v>221</v>
+        <v>229</v>
       </c>
       <c r="F314" s="25">
         <v>1.0</v>
@@ -9907,7 +9981,7 @@
     <row r="320">
       <c r="A320" s="8"/>
       <c r="B320" s="16" t="s">
-        <v>226</v>
+        <v>234</v>
       </c>
       <c r="C320" s="17" t="s">
         <v>46</v>
@@ -9999,10 +10073,10 @@
       <c r="F323" s="13"/>
       <c r="H323" s="8"/>
       <c r="I323" s="19" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="J323" s="27" t="s">
-        <v>228</v>
+        <v>236</v>
       </c>
       <c r="K323" s="26">
         <v>4.0</v>
@@ -10028,7 +10102,7 @@
       <c r="H324" s="8"/>
       <c r="I324" s="19"/>
       <c r="J324" s="27" t="s">
-        <v>229</v>
+        <v>237</v>
       </c>
       <c r="K324" s="28"/>
       <c r="L324" s="22"/>
@@ -10052,7 +10126,7 @@
       <c r="H325" s="8"/>
       <c r="I325" s="19"/>
       <c r="J325" s="27" t="s">
-        <v>230</v>
+        <v>238</v>
       </c>
       <c r="K325" s="26"/>
       <c r="L325" s="22"/>
@@ -10094,7 +10168,7 @@
       <c r="A327" s="8"/>
       <c r="B327" s="9"/>
       <c r="C327" s="17" t="s">
-        <v>220</v>
+        <v>228</v>
       </c>
       <c r="D327" s="11"/>
       <c r="E327" s="24" t="s">
@@ -10106,7 +10180,7 @@
       <c r="H327" s="8"/>
       <c r="I327" s="19"/>
       <c r="J327" s="27" t="s">
-        <v>231</v>
+        <v>239</v>
       </c>
       <c r="K327" s="26"/>
       <c r="L327" s="22"/>
@@ -10124,7 +10198,7 @@
       <c r="C328" s="10"/>
       <c r="D328" s="11"/>
       <c r="E328" s="24" t="s">
-        <v>221</v>
+        <v>229</v>
       </c>
       <c r="F328" s="25">
         <v>1.0</v>
@@ -10271,7 +10345,7 @@
     <row r="334">
       <c r="A334" s="8"/>
       <c r="B334" s="16" t="s">
-        <v>232</v>
+        <v>240</v>
       </c>
       <c r="C334" s="17" t="s">
         <v>62</v>
@@ -10357,10 +10431,10 @@
       <c r="F337" s="13"/>
       <c r="H337" s="8"/>
       <c r="I337" s="19" t="s">
-        <v>233</v>
+        <v>241</v>
       </c>
       <c r="J337" s="27" t="s">
-        <v>228</v>
+        <v>236</v>
       </c>
       <c r="K337" s="26">
         <v>4.0</v>
@@ -10386,7 +10460,7 @@
       <c r="H338" s="8"/>
       <c r="I338" s="19"/>
       <c r="J338" s="27" t="s">
-        <v>229</v>
+        <v>237</v>
       </c>
       <c r="K338" s="26"/>
       <c r="L338" s="22"/>
@@ -10402,7 +10476,7 @@
       <c r="A339" s="8"/>
       <c r="B339" s="9"/>
       <c r="C339" s="17" t="s">
-        <v>220</v>
+        <v>228</v>
       </c>
       <c r="D339" s="11"/>
       <c r="E339" s="24" t="s">
@@ -10414,7 +10488,7 @@
       <c r="H339" s="8"/>
       <c r="I339" s="19"/>
       <c r="J339" s="27" t="s">
-        <v>230</v>
+        <v>238</v>
       </c>
       <c r="K339" s="28"/>
       <c r="L339" s="22"/>
@@ -10432,7 +10506,7 @@
       <c r="C340" s="10"/>
       <c r="D340" s="11"/>
       <c r="E340" s="24" t="s">
-        <v>221</v>
+        <v>229</v>
       </c>
       <c r="F340" s="25">
         <v>1.0</v>
@@ -10466,7 +10540,7 @@
       <c r="H341" s="8"/>
       <c r="I341" s="19"/>
       <c r="J341" s="27" t="s">
-        <v>231</v>
+        <v>239</v>
       </c>
       <c r="K341" s="26"/>
       <c r="L341" s="22"/>
@@ -10579,7 +10653,7 @@
     <row r="346">
       <c r="A346" s="8"/>
       <c r="B346" s="16" t="s">
-        <v>234</v>
+        <v>242</v>
       </c>
       <c r="C346" s="17" t="s">
         <v>62</v>
@@ -10715,7 +10789,7 @@
       <c r="F351" s="13"/>
       <c r="H351" s="8"/>
       <c r="I351" s="19" t="s">
-        <v>235</v>
+        <v>243</v>
       </c>
       <c r="J351" s="27" t="s">
         <v>24</v>
@@ -10736,7 +10810,7 @@
       <c r="A352" s="8"/>
       <c r="B352" s="9"/>
       <c r="C352" s="17" t="s">
-        <v>220</v>
+        <v>228</v>
       </c>
       <c r="D352" s="11"/>
       <c r="E352" s="24" t="s">
@@ -10766,7 +10840,7 @@
       <c r="C353" s="10"/>
       <c r="D353" s="11"/>
       <c r="E353" s="24" t="s">
-        <v>221</v>
+        <v>229</v>
       </c>
       <c r="F353" s="25">
         <v>1.0</v>
@@ -10913,7 +10987,7 @@
     <row r="359">
       <c r="A359" s="8"/>
       <c r="B359" s="16" t="s">
-        <v>236</v>
+        <v>244</v>
       </c>
       <c r="C359" s="17" t="s">
         <v>39</v>
@@ -11042,7 +11116,7 @@
       <c r="A364" s="8"/>
       <c r="B364" s="9"/>
       <c r="C364" s="17" t="s">
-        <v>220</v>
+        <v>228</v>
       </c>
       <c r="D364" s="11"/>
       <c r="E364" s="24" t="s">
@@ -11053,7 +11127,7 @@
       </c>
       <c r="H364" s="8"/>
       <c r="I364" s="19" t="s">
-        <v>237</v>
+        <v>245</v>
       </c>
       <c r="J364" s="27" t="s">
         <v>24</v>
@@ -11076,7 +11150,7 @@
       <c r="C365" s="10"/>
       <c r="D365" s="11"/>
       <c r="E365" s="24" t="s">
-        <v>221</v>
+        <v>229</v>
       </c>
       <c r="F365" s="25">
         <v>1.0</v>
@@ -11247,7 +11321,7 @@
     <row r="372">
       <c r="A372" s="8"/>
       <c r="B372" s="16" t="s">
-        <v>238</v>
+        <v>246</v>
       </c>
       <c r="C372" s="17" t="s">
         <v>39</v>
@@ -11383,7 +11457,7 @@
       <c r="F377" s="13"/>
       <c r="H377" s="8"/>
       <c r="I377" s="19" t="s">
-        <v>239</v>
+        <v>247</v>
       </c>
       <c r="J377" s="27" t="s">
         <v>24</v>
@@ -11404,7 +11478,7 @@
       <c r="A378" s="8"/>
       <c r="B378" s="9"/>
       <c r="C378" s="17" t="s">
-        <v>220</v>
+        <v>228</v>
       </c>
       <c r="D378" s="11"/>
       <c r="E378" s="24" t="s">
@@ -11434,7 +11508,7 @@
       <c r="C379" s="10"/>
       <c r="D379" s="11"/>
       <c r="E379" s="24" t="s">
-        <v>221</v>
+        <v>229</v>
       </c>
       <c r="F379" s="25">
         <v>1.0</v>
@@ -11605,10 +11679,10 @@
     <row r="386">
       <c r="A386" s="8"/>
       <c r="B386" s="16" t="s">
-        <v>240</v>
+        <v>248</v>
       </c>
       <c r="C386" s="17" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="D386" s="18">
         <v>4.0</v>
@@ -11666,13 +11740,13 @@
       <c r="A388" s="8"/>
       <c r="B388" s="9"/>
       <c r="C388" s="17" t="s">
-        <v>242</v>
+        <v>250</v>
       </c>
       <c r="D388" s="18">
         <v>3.0</v>
       </c>
       <c r="E388" s="24" t="s">
-        <v>243</v>
+        <v>251</v>
       </c>
       <c r="F388" s="25">
         <v>1.5</v>
@@ -11729,7 +11803,7 @@
       <c r="F390" s="13"/>
       <c r="H390" s="8"/>
       <c r="I390" s="19" t="s">
-        <v>244</v>
+        <v>252</v>
       </c>
       <c r="J390" s="27" t="s">
         <v>24</v>
@@ -11798,7 +11872,7 @@
       <c r="A393" s="8"/>
       <c r="B393" s="9"/>
       <c r="C393" s="17" t="s">
-        <v>220</v>
+        <v>228</v>
       </c>
       <c r="D393" s="11"/>
       <c r="E393" s="24" t="s">
@@ -11830,7 +11904,7 @@
       <c r="C394" s="10"/>
       <c r="D394" s="11"/>
       <c r="E394" s="24" t="s">
-        <v>221</v>
+        <v>229</v>
       </c>
       <c r="F394" s="25">
         <v>1.0</v>
@@ -12025,10 +12099,10 @@
     <row r="402">
       <c r="A402" s="8"/>
       <c r="B402" s="16" t="s">
-        <v>245</v>
+        <v>253</v>
       </c>
       <c r="C402" s="17" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="D402" s="18">
         <v>4.0</v>
@@ -12084,20 +12158,20 @@
       <c r="A404" s="8"/>
       <c r="B404" s="9"/>
       <c r="C404" s="17" t="s">
-        <v>242</v>
+        <v>250</v>
       </c>
       <c r="D404" s="18">
         <v>3.0</v>
       </c>
       <c r="E404" s="24" t="s">
-        <v>243</v>
+        <v>251</v>
       </c>
       <c r="F404" s="25">
         <v>1.5</v>
       </c>
       <c r="H404" s="8"/>
       <c r="I404" s="19" t="s">
-        <v>246</v>
+        <v>254</v>
       </c>
       <c r="J404" s="27" t="s">
         <v>62</v>
@@ -12242,7 +12316,7 @@
       <c r="A410" s="8"/>
       <c r="B410" s="9"/>
       <c r="C410" s="17" t="s">
-        <v>220</v>
+        <v>228</v>
       </c>
       <c r="D410" s="11"/>
       <c r="E410" s="24" t="s">
@@ -12272,7 +12346,7 @@
       <c r="C411" s="10"/>
       <c r="D411" s="11"/>
       <c r="E411" s="24" t="s">
-        <v>221</v>
+        <v>229</v>
       </c>
       <c r="F411" s="25">
         <v>1.0</v>
@@ -12332,7 +12406,7 @@
       <c r="H413" s="8"/>
       <c r="I413" s="33"/>
       <c r="J413" s="27" t="s">
-        <v>247</v>
+        <v>255</v>
       </c>
       <c r="K413" s="26"/>
       <c r="L413" s="22"/>
@@ -12429,7 +12503,7 @@
       <c r="F417" s="13"/>
       <c r="H417" s="8"/>
       <c r="I417" s="19" t="s">
-        <v>248</v>
+        <v>256</v>
       </c>
       <c r="J417" s="27" t="s">
         <v>62</v>
@@ -12471,7 +12545,7 @@
     <row r="419">
       <c r="A419" s="8"/>
       <c r="B419" s="16" t="s">
-        <v>249</v>
+        <v>257</v>
       </c>
       <c r="C419" s="17" t="s">
         <v>95</v>
@@ -12600,7 +12674,7 @@
       <c r="A424" s="8"/>
       <c r="B424" s="9"/>
       <c r="C424" s="17" t="s">
-        <v>220</v>
+        <v>228</v>
       </c>
       <c r="D424" s="11"/>
       <c r="E424" s="24" t="s">
@@ -12632,7 +12706,7 @@
       <c r="C425" s="10"/>
       <c r="D425" s="11"/>
       <c r="E425" s="24" t="s">
-        <v>221</v>
+        <v>229</v>
       </c>
       <c r="F425" s="25">
         <v>1.0</v>
@@ -12666,7 +12740,7 @@
       <c r="H426" s="8"/>
       <c r="I426" s="33"/>
       <c r="J426" s="27" t="s">
-        <v>247</v>
+        <v>255</v>
       </c>
       <c r="K426" s="26"/>
       <c r="L426" s="22"/>
@@ -12761,7 +12835,7 @@
       <c r="F430" s="13"/>
       <c r="H430" s="8"/>
       <c r="I430" s="19" t="s">
-        <v>250</v>
+        <v>258</v>
       </c>
       <c r="J430" s="27" t="s">
         <v>62</v>
@@ -12829,7 +12903,7 @@
     <row r="433">
       <c r="A433" s="8"/>
       <c r="B433" s="16" t="s">
-        <v>251</v>
+        <v>259</v>
       </c>
       <c r="C433" s="17" t="s">
         <v>95</v>
@@ -12984,7 +13058,7 @@
       <c r="A439" s="8"/>
       <c r="B439" s="9"/>
       <c r="C439" s="17" t="s">
-        <v>220</v>
+        <v>228</v>
       </c>
       <c r="D439" s="11"/>
       <c r="E439" s="24" t="s">
@@ -13014,7 +13088,7 @@
       <c r="C440" s="10"/>
       <c r="D440" s="11"/>
       <c r="E440" s="24" t="s">
-        <v>221</v>
+        <v>229</v>
       </c>
       <c r="F440" s="25">
         <v>1.0</v>
@@ -13095,7 +13169,7 @@
       <c r="F443" s="13"/>
       <c r="H443" s="8"/>
       <c r="I443" s="19" t="s">
-        <v>252</v>
+        <v>260</v>
       </c>
       <c r="J443" s="27" t="s">
         <v>201</v>
@@ -13213,7 +13287,7 @@
     <row r="448">
       <c r="A448" s="8"/>
       <c r="B448" s="16" t="s">
-        <v>253</v>
+        <v>261</v>
       </c>
       <c r="C448" s="17" t="s">
         <v>39</v>
@@ -13300,7 +13374,7 @@
       <c r="H451" s="8"/>
       <c r="I451" s="19"/>
       <c r="J451" s="27" t="s">
-        <v>254</v>
+        <v>262</v>
       </c>
       <c r="K451" s="21">
         <v>2.0</v>
@@ -13318,7 +13392,7 @@
       <c r="A452" s="8"/>
       <c r="B452" s="9"/>
       <c r="C452" s="17" t="s">
-        <v>220</v>
+        <v>228</v>
       </c>
       <c r="D452" s="11"/>
       <c r="E452" s="24" t="s">
@@ -13348,7 +13422,7 @@
       <c r="C453" s="10"/>
       <c r="D453" s="11"/>
       <c r="E453" s="24" t="s">
-        <v>221</v>
+        <v>229</v>
       </c>
       <c r="F453" s="25">
         <v>1.0</v>
@@ -13356,7 +13430,7 @@
       <c r="H453" s="8"/>
       <c r="I453" s="19"/>
       <c r="J453" s="20" t="s">
-        <v>247</v>
+        <v>255</v>
       </c>
       <c r="K453" s="26"/>
       <c r="L453" s="22"/>
@@ -13453,7 +13527,7 @@
       <c r="F457" s="13"/>
       <c r="H457" s="8"/>
       <c r="I457" s="19" t="s">
-        <v>255</v>
+        <v>263</v>
       </c>
       <c r="J457" s="27" t="s">
         <v>201</v>
@@ -13595,7 +13669,7 @@
     <row r="463">
       <c r="A463" s="8"/>
       <c r="B463" s="32" t="s">
-        <v>256</v>
+        <v>264</v>
       </c>
       <c r="C463" s="20" t="s">
         <v>39</v>
@@ -13658,7 +13732,7 @@
       <c r="H465" s="8"/>
       <c r="I465" s="19"/>
       <c r="J465" s="27" t="s">
-        <v>254</v>
+        <v>262</v>
       </c>
       <c r="K465" s="21">
         <v>2.0</v>
@@ -13708,7 +13782,7 @@
       <c r="H467" s="8"/>
       <c r="I467" s="19"/>
       <c r="J467" s="27" t="s">
-        <v>247</v>
+        <v>255</v>
       </c>
       <c r="K467" s="28"/>
       <c r="L467" s="22"/>
@@ -13724,7 +13798,7 @@
       <c r="A468" s="8"/>
       <c r="B468" s="19"/>
       <c r="C468" s="20" t="s">
-        <v>220</v>
+        <v>228</v>
       </c>
       <c r="D468" s="26"/>
       <c r="E468" s="22" t="s">
@@ -13754,7 +13828,7 @@
       <c r="C469" s="20"/>
       <c r="D469" s="26"/>
       <c r="E469" s="22" t="s">
-        <v>221</v>
+        <v>229</v>
       </c>
       <c r="F469" s="30">
         <v>1.0</v>
@@ -13811,7 +13885,7 @@
       <c r="F471" s="23"/>
       <c r="H471" s="8"/>
       <c r="I471" s="19" t="s">
-        <v>257</v>
+        <v>265</v>
       </c>
       <c r="J471" s="27" t="s">
         <v>201</v>
@@ -14000,9 +14074,15 @@
     </row>
     <row r="479">
       <c r="A479" s="8"/>
-      <c r="B479" s="9"/>
-      <c r="C479" s="17"/>
-      <c r="D479" s="11"/>
+      <c r="B479" s="16" t="s">
+        <v>266</v>
+      </c>
+      <c r="C479" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D479" s="18">
+        <v>4.0</v>
+      </c>
       <c r="E479" s="24"/>
       <c r="F479" s="25"/>
       <c r="H479" s="8"/>
@@ -14025,8 +14105,12 @@
     <row r="480">
       <c r="A480" s="8"/>
       <c r="B480" s="9"/>
-      <c r="C480" s="10"/>
-      <c r="D480" s="11"/>
+      <c r="C480" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="D480" s="21">
+        <v>3.0</v>
+      </c>
       <c r="E480" s="24"/>
       <c r="F480" s="25"/>
       <c r="H480" s="8"/>
@@ -14047,8 +14131,10 @@
     <row r="481">
       <c r="A481" s="8"/>
       <c r="B481" s="9"/>
-      <c r="C481" s="17"/>
-      <c r="D481" s="11"/>
+      <c r="C481" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="D481" s="26"/>
       <c r="E481" s="24"/>
       <c r="F481" s="25"/>
       <c r="H481" s="8"/>
@@ -14069,8 +14155,10 @@
     <row r="482">
       <c r="A482" s="8"/>
       <c r="B482" s="9"/>
-      <c r="C482" s="10"/>
-      <c r="D482" s="11"/>
+      <c r="C482" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="D482" s="26"/>
       <c r="E482" s="24"/>
       <c r="F482" s="25"/>
       <c r="H482" s="8"/>
@@ -14091,7 +14179,9 @@
     <row r="483">
       <c r="A483" s="8"/>
       <c r="B483" s="9"/>
-      <c r="C483" s="10"/>
+      <c r="C483" s="17" t="s">
+        <v>54</v>
+      </c>
       <c r="D483" s="11"/>
       <c r="E483" s="24"/>
       <c r="F483" s="25"/>
@@ -14115,7 +14205,9 @@
     <row r="484">
       <c r="A484" s="8"/>
       <c r="B484" s="9"/>
-      <c r="C484" s="10"/>
+      <c r="C484" s="17" t="s">
+        <v>267</v>
+      </c>
       <c r="D484" s="11"/>
       <c r="E484" s="24"/>
       <c r="F484" s="25"/>
@@ -14135,16 +14227,20 @@
     <row r="485">
       <c r="A485" s="8"/>
       <c r="B485" s="9"/>
-      <c r="C485" s="17"/>
-      <c r="D485" s="18"/>
+      <c r="C485" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="D485" s="18">
+        <v>2.0</v>
+      </c>
       <c r="E485" s="12"/>
       <c r="F485" s="13"/>
       <c r="H485" s="8"/>
       <c r="I485" s="33"/>
-      <c r="J485" s="34"/>
-      <c r="K485" s="26"/>
-      <c r="L485" s="12"/>
-      <c r="M485" s="13"/>
+      <c r="J485" s="27"/>
+      <c r="K485" s="21"/>
+      <c r="L485" s="22"/>
+      <c r="M485" s="30"/>
       <c r="O485" s="8"/>
       <c r="P485" s="9"/>
       <c r="Q485" s="10"/>
@@ -14155,7 +14251,9 @@
     <row r="486">
       <c r="A486" s="8"/>
       <c r="B486" s="9"/>
-      <c r="C486" s="10"/>
+      <c r="C486" s="17" t="s">
+        <v>62</v>
+      </c>
       <c r="D486" s="11"/>
       <c r="E486" s="12"/>
       <c r="F486" s="13"/>
@@ -14163,8 +14261,8 @@
       <c r="I486" s="19"/>
       <c r="J486" s="20"/>
       <c r="K486" s="26"/>
-      <c r="L486" s="12"/>
-      <c r="M486" s="13"/>
+      <c r="L486" s="22"/>
+      <c r="M486" s="30"/>
       <c r="O486" s="8"/>
       <c r="P486" s="9"/>
       <c r="Q486" s="10"/>
@@ -14175,16 +14273,18 @@
     <row r="487">
       <c r="A487" s="8"/>
       <c r="B487" s="16"/>
-      <c r="C487" s="17"/>
+      <c r="C487" s="17" t="s">
+        <v>55</v>
+      </c>
       <c r="D487" s="18"/>
       <c r="E487" s="12"/>
       <c r="F487" s="13"/>
       <c r="H487" s="8"/>
       <c r="I487" s="19"/>
       <c r="J487" s="20"/>
-      <c r="K487" s="21"/>
-      <c r="L487" s="12"/>
-      <c r="M487" s="13"/>
+      <c r="K487" s="26"/>
+      <c r="L487" s="22"/>
+      <c r="M487" s="23"/>
       <c r="O487" s="8"/>
       <c r="P487" s="9"/>
       <c r="Q487" s="10"/>
@@ -14195,16 +14295,18 @@
     <row r="488">
       <c r="A488" s="8"/>
       <c r="B488" s="9"/>
-      <c r="C488" s="17"/>
+      <c r="C488" s="17" t="s">
+        <v>268</v>
+      </c>
       <c r="D488" s="11"/>
       <c r="E488" s="12"/>
       <c r="F488" s="13"/>
       <c r="H488" s="8"/>
       <c r="I488" s="19"/>
-      <c r="J488" s="36"/>
+      <c r="J488" s="20"/>
       <c r="K488" s="26"/>
-      <c r="L488" s="12"/>
-      <c r="M488" s="13"/>
+      <c r="L488" s="22"/>
+      <c r="M488" s="23"/>
       <c r="O488" s="8"/>
       <c r="P488" s="9"/>
       <c r="Q488" s="10"/>
@@ -14215,7 +14317,9 @@
     <row r="489">
       <c r="A489" s="8"/>
       <c r="B489" s="9"/>
-      <c r="C489" s="17"/>
+      <c r="C489" s="17" t="s">
+        <v>269</v>
+      </c>
       <c r="D489" s="11"/>
       <c r="E489" s="12"/>
       <c r="F489" s="13"/>
@@ -14223,8 +14327,8 @@
       <c r="I489" s="19"/>
       <c r="J489" s="20"/>
       <c r="K489" s="26"/>
-      <c r="L489" s="12"/>
-      <c r="M489" s="13"/>
+      <c r="L489" s="22"/>
+      <c r="M489" s="23"/>
       <c r="O489" s="8"/>
       <c r="P489" s="9"/>
       <c r="Q489" s="10"/>
@@ -14235,16 +14339,18 @@
     <row r="490">
       <c r="A490" s="8"/>
       <c r="B490" s="9"/>
-      <c r="C490" s="17"/>
+      <c r="C490" s="17" t="s">
+        <v>270</v>
+      </c>
       <c r="D490" s="11"/>
       <c r="E490" s="12"/>
       <c r="F490" s="13"/>
       <c r="H490" s="8"/>
       <c r="I490" s="19"/>
       <c r="J490" s="20"/>
-      <c r="K490" s="26"/>
-      <c r="L490" s="12"/>
-      <c r="M490" s="13"/>
+      <c r="K490" s="21"/>
+      <c r="L490" s="22"/>
+      <c r="M490" s="23"/>
       <c r="O490" s="8"/>
       <c r="P490" s="9"/>
       <c r="Q490" s="10"/>
@@ -14255,16 +14361,18 @@
     <row r="491">
       <c r="A491" s="8"/>
       <c r="B491" s="9"/>
-      <c r="C491" s="17"/>
+      <c r="C491" s="17" t="s">
+        <v>36</v>
+      </c>
       <c r="D491" s="11"/>
       <c r="E491" s="12"/>
       <c r="F491" s="13"/>
       <c r="H491" s="8"/>
       <c r="I491" s="19"/>
       <c r="J491" s="20"/>
-      <c r="K491" s="21"/>
-      <c r="L491" s="12"/>
-      <c r="M491" s="13"/>
+      <c r="K491" s="26"/>
+      <c r="L491" s="22"/>
+      <c r="M491" s="23"/>
       <c r="O491" s="8"/>
       <c r="P491" s="9"/>
       <c r="Q491" s="10"/>
@@ -14275,16 +14383,20 @@
     <row r="492">
       <c r="A492" s="8"/>
       <c r="B492" s="9"/>
-      <c r="C492" s="17"/>
-      <c r="D492" s="11"/>
+      <c r="C492" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="D492" s="18">
+        <v>1.0</v>
+      </c>
       <c r="E492" s="24"/>
       <c r="F492" s="25"/>
       <c r="H492" s="8"/>
-      <c r="I492" s="9"/>
-      <c r="J492" s="10"/>
-      <c r="K492" s="11"/>
-      <c r="L492" s="12"/>
-      <c r="M492" s="13"/>
+      <c r="I492" s="19"/>
+      <c r="J492" s="20"/>
+      <c r="K492" s="26"/>
+      <c r="L492" s="22"/>
+      <c r="M492" s="23"/>
       <c r="O492" s="8"/>
       <c r="P492" s="9"/>
       <c r="Q492" s="10"/>
@@ -14300,11 +14412,11 @@
       <c r="E493" s="24"/>
       <c r="F493" s="25"/>
       <c r="H493" s="8"/>
-      <c r="I493" s="9"/>
-      <c r="J493" s="10"/>
-      <c r="K493" s="11"/>
-      <c r="L493" s="12"/>
-      <c r="M493" s="13"/>
+      <c r="I493" s="19"/>
+      <c r="J493" s="20"/>
+      <c r="K493" s="26"/>
+      <c r="L493" s="22"/>
+      <c r="M493" s="23"/>
       <c r="O493" s="8"/>
       <c r="P493" s="9"/>
       <c r="Q493" s="10"/>
@@ -14314,17 +14426,23 @@
     </row>
     <row r="494">
       <c r="A494" s="8"/>
-      <c r="B494" s="9"/>
-      <c r="C494" s="17"/>
-      <c r="D494" s="11"/>
+      <c r="B494" s="16" t="s">
+        <v>271</v>
+      </c>
+      <c r="C494" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D494" s="18">
+        <v>4.0</v>
+      </c>
       <c r="E494" s="24"/>
       <c r="F494" s="25"/>
       <c r="H494" s="8"/>
-      <c r="I494" s="9"/>
-      <c r="J494" s="10"/>
-      <c r="K494" s="11"/>
-      <c r="L494" s="12"/>
-      <c r="M494" s="13"/>
+      <c r="I494" s="19"/>
+      <c r="J494" s="20"/>
+      <c r="K494" s="21"/>
+      <c r="L494" s="22"/>
+      <c r="M494" s="23"/>
       <c r="O494" s="8"/>
       <c r="P494" s="9"/>
       <c r="Q494" s="10"/>
@@ -14335,8 +14453,12 @@
     <row r="495">
       <c r="A495" s="8"/>
       <c r="B495" s="9"/>
-      <c r="C495" s="10"/>
-      <c r="D495" s="11"/>
+      <c r="C495" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="D495" s="21">
+        <v>3.0</v>
+      </c>
       <c r="E495" s="24"/>
       <c r="F495" s="25"/>
       <c r="H495" s="8"/>
@@ -14355,8 +14477,10 @@
     <row r="496">
       <c r="A496" s="8"/>
       <c r="B496" s="9"/>
-      <c r="C496" s="10"/>
-      <c r="D496" s="11"/>
+      <c r="C496" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="D496" s="26"/>
       <c r="E496" s="24"/>
       <c r="F496" s="25"/>
       <c r="H496" s="8"/>
@@ -14375,8 +14499,10 @@
     <row r="497">
       <c r="A497" s="8"/>
       <c r="B497" s="9"/>
-      <c r="C497" s="10"/>
-      <c r="D497" s="11"/>
+      <c r="C497" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="D497" s="26"/>
       <c r="E497" s="24"/>
       <c r="F497" s="25"/>
       <c r="H497" s="8"/>
@@ -14395,8 +14521,10 @@
     <row r="498">
       <c r="A498" s="8"/>
       <c r="B498" s="9"/>
-      <c r="C498" s="17"/>
-      <c r="D498" s="18"/>
+      <c r="C498" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="D498" s="11"/>
       <c r="E498" s="12"/>
       <c r="F498" s="13"/>
       <c r="H498" s="8"/>
@@ -14415,7 +14543,9 @@
     <row r="499">
       <c r="A499" s="8"/>
       <c r="B499" s="9"/>
-      <c r="C499" s="10"/>
+      <c r="C499" s="17" t="s">
+        <v>267</v>
+      </c>
       <c r="D499" s="11"/>
       <c r="E499" s="12"/>
       <c r="F499" s="13"/>
@@ -14435,8 +14565,10 @@
     <row r="500">
       <c r="A500" s="8"/>
       <c r="B500" s="9"/>
-      <c r="C500" s="10"/>
-      <c r="D500" s="11"/>
+      <c r="C500" s="35" t="s">
+        <v>269</v>
+      </c>
+      <c r="D500" s="28"/>
       <c r="E500" s="12"/>
       <c r="F500" s="13"/>
       <c r="H500" s="8"/>
@@ -14455,7 +14587,9 @@
     <row r="501">
       <c r="A501" s="8"/>
       <c r="B501" s="9"/>
-      <c r="C501" s="10"/>
+      <c r="C501" s="17" t="s">
+        <v>221</v>
+      </c>
       <c r="D501" s="11"/>
       <c r="E501" s="12"/>
       <c r="F501" s="13"/>
@@ -14474,9 +14608,11 @@
     </row>
     <row r="502">
       <c r="A502" s="8"/>
-      <c r="B502" s="9"/>
-      <c r="C502" s="10"/>
-      <c r="D502" s="11"/>
+      <c r="B502" s="16"/>
+      <c r="C502" s="17" t="s">
+        <v>222</v>
+      </c>
+      <c r="D502" s="18"/>
       <c r="E502" s="12"/>
       <c r="F502" s="13"/>
       <c r="H502" s="8"/>
@@ -14495,8 +14631,12 @@
     <row r="503">
       <c r="A503" s="8"/>
       <c r="B503" s="9"/>
-      <c r="C503" s="10"/>
-      <c r="D503" s="11"/>
+      <c r="C503" s="35" t="s">
+        <v>229</v>
+      </c>
+      <c r="D503" s="37">
+        <v>2.0</v>
+      </c>
       <c r="E503" s="12"/>
       <c r="F503" s="13"/>
       <c r="H503" s="8"/>
@@ -14515,8 +14655,10 @@
     <row r="504">
       <c r="A504" s="8"/>
       <c r="B504" s="9"/>
-      <c r="C504" s="10"/>
-      <c r="D504" s="11"/>
+      <c r="C504" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="D504" s="26"/>
       <c r="E504" s="12"/>
       <c r="F504" s="13"/>
       <c r="H504" s="8"/>
@@ -14535,8 +14677,10 @@
     <row r="505">
       <c r="A505" s="8"/>
       <c r="B505" s="9"/>
-      <c r="C505" s="10"/>
-      <c r="D505" s="11"/>
+      <c r="C505" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="D505" s="26"/>
       <c r="E505" s="12"/>
       <c r="F505" s="13"/>
       <c r="H505" s="8"/>
@@ -14555,8 +14699,12 @@
     <row r="506">
       <c r="A506" s="8"/>
       <c r="B506" s="9"/>
-      <c r="C506" s="10"/>
-      <c r="D506" s="11"/>
+      <c r="C506" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="D506" s="21">
+        <v>1.0</v>
+      </c>
       <c r="E506" s="12"/>
       <c r="F506" s="13"/>
       <c r="H506" s="8"/>
@@ -14575,8 +14723,8 @@
     <row r="507">
       <c r="A507" s="8"/>
       <c r="B507" s="9"/>
-      <c r="C507" s="10"/>
-      <c r="D507" s="11"/>
+      <c r="C507" s="34"/>
+      <c r="D507" s="28"/>
       <c r="E507" s="12"/>
       <c r="F507" s="13"/>
       <c r="H507" s="8"/>
@@ -14594,11 +14742,11 @@
     </row>
     <row r="508">
       <c r="A508" s="8"/>
-      <c r="B508" s="9"/>
-      <c r="C508" s="10"/>
-      <c r="D508" s="11"/>
-      <c r="E508" s="12"/>
-      <c r="F508" s="13"/>
+      <c r="B508" s="16"/>
+      <c r="C508" s="35"/>
+      <c r="D508" s="37"/>
+      <c r="E508" s="24"/>
+      <c r="F508" s="25"/>
       <c r="H508" s="8"/>
       <c r="I508" s="9"/>
       <c r="J508" s="10"/>
@@ -14615,10 +14763,10 @@
     <row r="509">
       <c r="A509" s="8"/>
       <c r="B509" s="9"/>
-      <c r="C509" s="10"/>
-      <c r="D509" s="11"/>
-      <c r="E509" s="12"/>
-      <c r="F509" s="13"/>
+      <c r="C509" s="20"/>
+      <c r="D509" s="26"/>
+      <c r="E509" s="24"/>
+      <c r="F509" s="25"/>
       <c r="H509" s="8"/>
       <c r="I509" s="9"/>
       <c r="J509" s="10"/>
@@ -14635,8 +14783,8 @@
     <row r="510">
       <c r="A510" s="8"/>
       <c r="B510" s="9"/>
-      <c r="C510" s="10"/>
-      <c r="D510" s="11"/>
+      <c r="C510" s="35"/>
+      <c r="D510" s="21"/>
       <c r="E510" s="12"/>
       <c r="F510" s="13"/>
       <c r="H510" s="8"/>
@@ -14655,7 +14803,7 @@
     <row r="511">
       <c r="A511" s="8"/>
       <c r="B511" s="9"/>
-      <c r="C511" s="10"/>
+      <c r="C511" s="17"/>
       <c r="D511" s="11"/>
       <c r="E511" s="12"/>
       <c r="F511" s="13"/>
@@ -14675,7 +14823,7 @@
     <row r="512">
       <c r="A512" s="8"/>
       <c r="B512" s="9"/>
-      <c r="C512" s="10"/>
+      <c r="C512" s="17"/>
       <c r="D512" s="11"/>
       <c r="E512" s="12"/>
       <c r="F512" s="13"/>
@@ -14695,8 +14843,8 @@
     <row r="513">
       <c r="A513" s="8"/>
       <c r="B513" s="9"/>
-      <c r="C513" s="10"/>
-      <c r="D513" s="11"/>
+      <c r="C513" s="17"/>
+      <c r="D513" s="18"/>
       <c r="E513" s="12"/>
       <c r="F513" s="13"/>
       <c r="H513" s="8"/>
@@ -14715,7 +14863,7 @@
     <row r="514">
       <c r="A514" s="8"/>
       <c r="B514" s="9"/>
-      <c r="C514" s="10"/>
+      <c r="C514" s="17"/>
       <c r="D514" s="11"/>
       <c r="E514" s="12"/>
       <c r="F514" s="13"/>
@@ -14735,7 +14883,7 @@
     <row r="515">
       <c r="A515" s="8"/>
       <c r="B515" s="9"/>
-      <c r="C515" s="10"/>
+      <c r="C515" s="17"/>
       <c r="D515" s="11"/>
       <c r="E515" s="12"/>
       <c r="F515" s="13"/>
@@ -14755,7 +14903,7 @@
     <row r="516">
       <c r="A516" s="8"/>
       <c r="B516" s="9"/>
-      <c r="C516" s="10"/>
+      <c r="C516" s="17"/>
       <c r="D516" s="11"/>
       <c r="E516" s="12"/>
       <c r="F516" s="13"/>
@@ -14775,8 +14923,8 @@
     <row r="517">
       <c r="A517" s="8"/>
       <c r="B517" s="9"/>
-      <c r="C517" s="10"/>
-      <c r="D517" s="11"/>
+      <c r="C517" s="17"/>
+      <c r="D517" s="18"/>
       <c r="E517" s="12"/>
       <c r="F517" s="13"/>
       <c r="H517" s="8"/>

</xml_diff>

<commit_message>
Added 2GA3D and 1GA3D
</commit_message>
<xml_diff>
--- a/assets/All Classes.xlsx
+++ b/assets/All Classes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\felix\Documents\GitHub\Datz-master\Datz-master\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6CB8E5F-8BB3-40ED-B688-B285B73B89B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98F8AD73-3A55-4E2B-A22F-486FCE8FA5BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1459" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1489" uniqueCount="297">
   <si>
     <t>ClassNames</t>
   </si>
@@ -890,6 +890,27 @@
   </si>
   <si>
     <t>1CLA-MAT</t>
+  </si>
+  <si>
+    <t>2GA3D</t>
+  </si>
+  <si>
+    <t>Francais</t>
+  </si>
+  <si>
+    <t>Développment durable</t>
+  </si>
+  <si>
+    <t>Questions philosophiques</t>
+  </si>
+  <si>
+    <t>ConMo</t>
+  </si>
+  <si>
+    <t>Construction</t>
+  </si>
+  <si>
+    <t>1GA3D</t>
   </si>
 </sst>
 </file>
@@ -1026,7 +1047,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1057,6 +1078,7 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1377,8 +1399,8 @@
   <dimension ref="A1:X1020"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A114" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S142" sqref="S142"/>
+      <pane ySplit="1" topLeftCell="A302" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R322" sqref="R322"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -10427,9 +10449,15 @@
       <c r="L318" s="18"/>
       <c r="M318" s="19"/>
       <c r="O318" s="8"/>
-      <c r="P318" s="9"/>
-      <c r="Q318" s="10"/>
-      <c r="R318" s="11"/>
+      <c r="P318" s="26" t="s">
+        <v>296</v>
+      </c>
+      <c r="Q318" s="24" t="s">
+        <v>245</v>
+      </c>
+      <c r="R318" s="20">
+        <v>4</v>
+      </c>
       <c r="S318" s="12"/>
       <c r="T318" s="13"/>
     </row>
@@ -10453,9 +10481,11 @@
       <c r="L319" s="18"/>
       <c r="M319" s="19"/>
       <c r="O319" s="8"/>
-      <c r="P319" s="9"/>
-      <c r="Q319" s="10"/>
-      <c r="R319" s="11"/>
+      <c r="P319" s="15"/>
+      <c r="Q319" s="24" t="s">
+        <v>295</v>
+      </c>
+      <c r="R319" s="20"/>
       <c r="S319" s="12"/>
       <c r="T319" s="13"/>
     </row>
@@ -10479,9 +10509,11 @@
       <c r="L320" s="18"/>
       <c r="M320" s="19"/>
       <c r="O320" s="8"/>
-      <c r="P320" s="9"/>
-      <c r="Q320" s="10"/>
-      <c r="R320" s="11"/>
+      <c r="P320" s="15"/>
+      <c r="Q320" s="24" t="s">
+        <v>247</v>
+      </c>
+      <c r="R320" s="20"/>
       <c r="S320" s="12"/>
       <c r="T320" s="13"/>
     </row>
@@ -10503,9 +10535,13 @@
       <c r="L321" s="18"/>
       <c r="M321" s="19"/>
       <c r="O321" s="8"/>
-      <c r="P321" s="9"/>
-      <c r="Q321" s="10"/>
-      <c r="R321" s="11"/>
+      <c r="P321" s="15"/>
+      <c r="Q321" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="R321" s="20">
+        <v>3</v>
+      </c>
       <c r="S321" s="12"/>
       <c r="T321" s="13"/>
     </row>
@@ -10535,9 +10571,11 @@
       <c r="L322" s="18"/>
       <c r="M322" s="19"/>
       <c r="O322" s="8"/>
-      <c r="P322" s="9"/>
-      <c r="Q322" s="10"/>
-      <c r="R322" s="11"/>
+      <c r="P322" s="15"/>
+      <c r="Q322" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="R322" s="20"/>
       <c r="S322" s="12"/>
       <c r="T322" s="13"/>
     </row>
@@ -10561,9 +10599,11 @@
       <c r="L323" s="18"/>
       <c r="M323" s="19"/>
       <c r="O323" s="8"/>
-      <c r="P323" s="9"/>
-      <c r="Q323" s="10"/>
-      <c r="R323" s="11"/>
+      <c r="P323" s="15"/>
+      <c r="Q323" s="24" t="s">
+        <v>291</v>
+      </c>
+      <c r="R323" s="20"/>
       <c r="S323" s="12"/>
       <c r="T323" s="13"/>
     </row>
@@ -10589,9 +10629,11 @@
       <c r="L324" s="18"/>
       <c r="M324" s="19"/>
       <c r="O324" s="8"/>
-      <c r="P324" s="9"/>
-      <c r="Q324" s="10"/>
-      <c r="R324" s="11"/>
+      <c r="P324" s="15"/>
+      <c r="Q324" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="R324" s="20"/>
       <c r="S324" s="12"/>
       <c r="T324" s="13"/>
     </row>
@@ -10613,9 +10655,11 @@
       <c r="L325" s="18"/>
       <c r="M325" s="19"/>
       <c r="O325" s="8"/>
-      <c r="P325" s="9"/>
-      <c r="Q325" s="10"/>
-      <c r="R325" s="11"/>
+      <c r="P325" s="15"/>
+      <c r="Q325" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="R325" s="20"/>
       <c r="S325" s="12"/>
       <c r="T325" s="13"/>
     </row>
@@ -10635,9 +10679,11 @@
       <c r="L326" s="18"/>
       <c r="M326" s="19"/>
       <c r="O326" s="8"/>
-      <c r="P326" s="9"/>
-      <c r="Q326" s="10"/>
-      <c r="R326" s="11"/>
+      <c r="P326" s="15"/>
+      <c r="Q326" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="R326" s="20"/>
       <c r="S326" s="12"/>
       <c r="T326" s="13"/>
     </row>
@@ -10663,9 +10709,13 @@
       <c r="L327" s="18"/>
       <c r="M327" s="19"/>
       <c r="O327" s="8"/>
-      <c r="P327" s="9"/>
-      <c r="Q327" s="10"/>
-      <c r="R327" s="11"/>
+      <c r="P327" s="15"/>
+      <c r="Q327" s="24" t="s">
+        <v>292</v>
+      </c>
+      <c r="R327" s="20">
+        <v>2</v>
+      </c>
       <c r="S327" s="12"/>
       <c r="T327" s="13"/>
     </row>
@@ -10687,9 +10737,11 @@
       <c r="L328" s="18"/>
       <c r="M328" s="19"/>
       <c r="O328" s="8"/>
-      <c r="P328" s="9"/>
-      <c r="Q328" s="10"/>
-      <c r="R328" s="11"/>
+      <c r="P328" s="15"/>
+      <c r="Q328" s="24" t="s">
+        <v>293</v>
+      </c>
+      <c r="R328" s="20"/>
       <c r="S328" s="12"/>
       <c r="T328" s="13"/>
     </row>
@@ -10715,9 +10767,11 @@
       <c r="L329" s="18"/>
       <c r="M329" s="19"/>
       <c r="O329" s="8"/>
-      <c r="P329" s="9"/>
-      <c r="Q329" s="10"/>
-      <c r="R329" s="11"/>
+      <c r="P329" s="15"/>
+      <c r="Q329" s="24" t="s">
+        <v>294</v>
+      </c>
+      <c r="R329" s="20"/>
       <c r="S329" s="12"/>
       <c r="T329" s="13"/>
     </row>
@@ -10743,9 +10797,11 @@
       <c r="L330" s="18"/>
       <c r="M330" s="19"/>
       <c r="O330" s="8"/>
-      <c r="P330" s="9"/>
-      <c r="Q330" s="10"/>
-      <c r="R330" s="11"/>
+      <c r="P330" s="15"/>
+      <c r="Q330" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="R330" s="20"/>
       <c r="S330" s="12"/>
       <c r="T330" s="13"/>
     </row>
@@ -10767,9 +10823,13 @@
       <c r="L331" s="18"/>
       <c r="M331" s="19"/>
       <c r="O331" s="8"/>
-      <c r="P331" s="9"/>
-      <c r="Q331" s="10"/>
-      <c r="R331" s="11"/>
+      <c r="P331" s="15"/>
+      <c r="Q331" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="R331" s="20">
+        <v>1</v>
+      </c>
       <c r="S331" s="12"/>
       <c r="T331" s="13"/>
     </row>
@@ -15567,9 +15627,15 @@
       <c r="E517" s="12"/>
       <c r="F517" s="13"/>
       <c r="H517" s="8"/>
-      <c r="I517" s="15"/>
-      <c r="J517" s="16"/>
-      <c r="K517" s="20"/>
+      <c r="I517" s="26" t="s">
+        <v>290</v>
+      </c>
+      <c r="J517" s="24" t="s">
+        <v>245</v>
+      </c>
+      <c r="K517" s="20">
+        <v>4</v>
+      </c>
       <c r="L517" s="18"/>
       <c r="M517" s="19"/>
       <c r="O517" s="8"/>
@@ -15590,7 +15656,9 @@
       <c r="F518" s="13"/>
       <c r="H518" s="8"/>
       <c r="I518" s="15"/>
-      <c r="J518" s="16"/>
+      <c r="J518" s="24" t="s">
+        <v>295</v>
+      </c>
       <c r="K518" s="20"/>
       <c r="L518" s="18"/>
       <c r="M518" s="19"/>
@@ -15612,7 +15680,9 @@
       <c r="F519" s="13"/>
       <c r="H519" s="8"/>
       <c r="I519" s="15"/>
-      <c r="J519" s="16"/>
+      <c r="J519" s="24" t="s">
+        <v>247</v>
+      </c>
       <c r="K519" s="20"/>
       <c r="L519" s="18"/>
       <c r="M519" s="19"/>
@@ -15634,8 +15704,12 @@
       <c r="F520" s="13"/>
       <c r="H520" s="8"/>
       <c r="I520" s="15"/>
-      <c r="J520" s="16"/>
-      <c r="K520" s="20"/>
+      <c r="J520" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="K520" s="20">
+        <v>3</v>
+      </c>
       <c r="L520" s="18"/>
       <c r="M520" s="19"/>
       <c r="O520" s="8"/>
@@ -15656,7 +15730,9 @@
       <c r="F521" s="13"/>
       <c r="H521" s="8"/>
       <c r="I521" s="15"/>
-      <c r="J521" s="16"/>
+      <c r="J521" s="24" t="s">
+        <v>22</v>
+      </c>
       <c r="K521" s="20"/>
       <c r="L521" s="18"/>
       <c r="M521" s="19"/>
@@ -15680,7 +15756,9 @@
       <c r="F522" s="13"/>
       <c r="H522" s="8"/>
       <c r="I522" s="15"/>
-      <c r="J522" s="16"/>
+      <c r="J522" s="24" t="s">
+        <v>291</v>
+      </c>
       <c r="K522" s="20"/>
       <c r="L522" s="18"/>
       <c r="M522" s="19"/>
@@ -15700,7 +15778,9 @@
       <c r="F523" s="13"/>
       <c r="H523" s="8"/>
       <c r="I523" s="15"/>
-      <c r="J523" s="16"/>
+      <c r="J523" s="24" t="s">
+        <v>24</v>
+      </c>
       <c r="K523" s="20"/>
       <c r="L523" s="18"/>
       <c r="M523" s="19"/>
@@ -15726,7 +15806,9 @@
       <c r="F524" s="13"/>
       <c r="H524" s="8"/>
       <c r="I524" s="15"/>
-      <c r="J524" s="16"/>
+      <c r="J524" s="24" t="s">
+        <v>55</v>
+      </c>
       <c r="K524" s="20"/>
       <c r="L524" s="18"/>
       <c r="M524" s="19"/>
@@ -15748,7 +15830,9 @@
       <c r="F525" s="13"/>
       <c r="H525" s="8"/>
       <c r="I525" s="15"/>
-      <c r="J525" s="16"/>
+      <c r="J525" s="24" t="s">
+        <v>54</v>
+      </c>
       <c r="K525" s="20"/>
       <c r="L525" s="18"/>
       <c r="M525" s="19"/>
@@ -15770,8 +15854,12 @@
       <c r="F526" s="13"/>
       <c r="H526" s="8"/>
       <c r="I526" s="15"/>
-      <c r="J526" s="16"/>
-      <c r="K526" s="20"/>
+      <c r="J526" s="24" t="s">
+        <v>292</v>
+      </c>
+      <c r="K526" s="20">
+        <v>2</v>
+      </c>
       <c r="L526" s="18"/>
       <c r="M526" s="19"/>
       <c r="O526" s="8"/>
@@ -15794,7 +15882,9 @@
       <c r="F527" s="13"/>
       <c r="H527" s="8"/>
       <c r="I527" s="15"/>
-      <c r="J527" s="16"/>
+      <c r="J527" s="24" t="s">
+        <v>293</v>
+      </c>
       <c r="K527" s="20"/>
       <c r="L527" s="18"/>
       <c r="M527" s="19"/>
@@ -15816,7 +15906,9 @@
       <c r="F528" s="13"/>
       <c r="H528" s="8"/>
       <c r="I528" s="15"/>
-      <c r="J528" s="16"/>
+      <c r="J528" s="24" t="s">
+        <v>294</v>
+      </c>
       <c r="K528" s="20"/>
       <c r="L528" s="18"/>
       <c r="M528" s="19"/>
@@ -15842,7 +15934,9 @@
       </c>
       <c r="H529" s="8"/>
       <c r="I529" s="15"/>
-      <c r="J529" s="16"/>
+      <c r="J529" s="24" t="s">
+        <v>41</v>
+      </c>
       <c r="K529" s="20"/>
       <c r="L529" s="18"/>
       <c r="M529" s="19"/>
@@ -15866,8 +15960,12 @@
       </c>
       <c r="H530" s="8"/>
       <c r="I530" s="15"/>
-      <c r="J530" s="16"/>
-      <c r="K530" s="20"/>
+      <c r="J530" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="K530" s="20">
+        <v>1</v>
+      </c>
       <c r="L530" s="18"/>
       <c r="M530" s="19"/>
       <c r="O530" s="8"/>

</xml_diff>